<commit_message>
modified mapping of functors (to be completed)
</commit_message>
<xml_diff>
--- a/tecto2umr/PDT-mozne-chyby.xlsx
+++ b/tecto2umr/PDT-mozne-chyby.xlsx
@@ -1,21 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lopatkova\SVN\GitHub-UMR\tecto2umr\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28640" windowHeight="12870"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28635" windowHeight="12870"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="95">
   <si>
     <t>#Gen</t>
   </si>
@@ -683,6 +678,41 @@
       </rPr>
       <t>NEUMÍM nějak rozumně zkontrolovat :-((</t>
     </r>
+  </si>
+  <si>
+    <t>t_lemma pro funktor CONTRA</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>pomlčka, 3x</t>
+  </si>
+  <si>
+    <t>asi by měla být nahrazena #Dash ??</t>
+  </si>
+  <si>
+    <t>tenhle</t>
+  </si>
+  <si>
+    <t>v</t>
+  </si>
+  <si>
+    <t>hs_004.02-SCzechT-hs_004-d1e906-x2-root 
+hs_004.06-SCzechT-hs_004-1176-root
+T-wsj2202-001-p1s28</t>
+  </si>
+  <si>
+    <t>lk_010.08-SCzechT-lk_010-d1e3290-x2-root</t>
+  </si>
+  <si>
+    <t>???</t>
+  </si>
+  <si>
+    <t>T-wsj1671-001-p1s51</t>
+  </si>
+  <si>
+    <t>?? nemá být vs?</t>
   </si>
 </sst>
 </file>
@@ -827,8 +857,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Check Cell" xfId="1" builtinId="23"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Kontrolní buňka" xfId="1" builtinId="23"/>
+    <cellStyle name="Normální" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1098,7 +1128,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1106,23 +1136,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.90625" style="5" customWidth="1"/>
-    <col min="2" max="2" width="15.6328125" style="5" customWidth="1"/>
-    <col min="3" max="3" width="54.90625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="30.08984375" style="5" customWidth="1"/>
+    <col min="1" max="1" width="16.85546875" style="5" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="54.85546875" style="4" customWidth="1"/>
+    <col min="4" max="4" width="30.140625" style="5" customWidth="1"/>
     <col min="5" max="5" width="86" style="4" customWidth="1"/>
-    <col min="6" max="16384" width="8.7265625" style="5"/>
+    <col min="6" max="16384" width="8.7109375" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:5" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
         <v>15</v>
       </c>
@@ -1139,7 +1169,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="87.5" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" ht="120.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -1156,7 +1186,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="116" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" ht="135" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
@@ -1173,7 +1203,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>2</v>
       </c>
@@ -1188,7 +1218,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>13</v>
       </c>
@@ -1200,7 +1230,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>3</v>
       </c>
@@ -1215,7 +1245,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>4</v>
       </c>
@@ -1232,7 +1262,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>5</v>
       </c>
@@ -1247,7 +1277,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>6</v>
       </c>
@@ -1262,7 +1292,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>7</v>
       </c>
@@ -1279,7 +1309,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>8</v>
       </c>
@@ -1294,7 +1324,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>9</v>
       </c>
@@ -1309,7 +1339,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>10</v>
       </c>
@@ -1324,7 +1354,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>11</v>
       </c>
@@ -1341,7 +1371,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>12</v>
       </c>
@@ -1356,8 +1386,8 @@
         <v>59</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="20" spans="1:5" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="20" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="9" t="s">
         <v>70</v>
       </c>
@@ -1374,7 +1404,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="49" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" ht="48.95" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>62</v>
       </c>
@@ -1386,7 +1416,7 @@
       </c>
       <c r="E21"/>
     </row>
-    <row r="22" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>65</v>
       </c>
@@ -1403,7 +1433,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>65</v>
       </c>
@@ -1420,7 +1450,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="s">
         <v>67</v>
       </c>
@@ -1431,7 +1461,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="87" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>77</v>
       </c>
@@ -1442,7 +1472,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" s="11" t="s">
         <v>69</v>
       </c>
@@ -1453,20 +1483,59 @@
         <v>80</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A28" s="4"/>
-      <c r="B28" s="4"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A29" s="4"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A30" s="4"/>
-      <c r="B30" s="4"/>
+    <row r="28" spans="1:5" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="B28" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D28" s="10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="75.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>85</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>88</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D31" t="s">
+        <v>93</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1480,7 +1549,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
how to map COMPL (part)
</commit_message>
<xml_diff>
--- a/tecto2umr/PDT-mozne-chyby.xlsx
+++ b/tecto2umr/PDT-mozne-chyby.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lopatkova\SVN\GitHub-UMR\tecto2umr\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28635" windowHeight="12870"/>
   </bookViews>
@@ -20,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="129">
   <si>
     <t>#Gen</t>
   </si>
@@ -686,9 +691,6 @@
     <t>-</t>
   </si>
   <si>
-    <t>pomlčka, 3x</t>
-  </si>
-  <si>
     <t>asi by měla být nahrazena #Dash ??</t>
   </si>
   <si>
@@ -706,20 +708,488 @@
     <t>lk_010.08-SCzechT-lk_010-d1e3290-x2-root</t>
   </si>
   <si>
-    <t>???</t>
-  </si>
-  <si>
     <t>T-wsj1671-001-p1s51</t>
   </si>
   <si>
     <t>?? nemá být vs?</t>
+  </si>
+  <si>
+    <t>COMPL visí a n.pron.* (a nikde okolo sloveso??)</t>
+  </si>
+  <si>
+    <t>chybný sempos</t>
+  </si>
+  <si>
+    <t>podezřelé konstrukce s COMPL</t>
+  </si>
+  <si>
+    <t>??? vůbec nerozumím notaci</t>
+  </si>
+  <si>
+    <t>chybné lemma</t>
+  </si>
+  <si>
+    <t>chybné lemma … pomlčka, 3x</t>
+  </si>
+  <si>
+    <t>"stát" anotováno jako "v", jde as "n" (asi denom?)</t>
+  </si>
+  <si>
+    <t>COMPL s 2 subst. rodiči</t>
+  </si>
+  <si>
+    <t>?? doplnit</t>
+  </si>
+  <si>
+    <t>… fotografiemi sama sebe, jak se plaví … ?? sama jako rodič sebe?? PAK divně doplněk (visí na sebe, sám???)
+???OPRAVA: sebe.RSTR k fotografii, sám.COMPL k fotografii, šipka k "sebe" ??</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">…  fotografiemi </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>sama sebe</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, jak se </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">plaví nebo létá </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>...</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Samozřejmě, že státní liberálové ještě nejsou </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>stát</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> sám pro sebe.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Přesto </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">stát </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>jako takový prodává semena a stroje.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">… kde </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>máme</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> kromě informací o studiu pro posluchače prvních ročníků také </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>kurz rychlého čtení jako úvod do studia .</t>
+    </r>
+  </si>
+  <si>
+    <t>COMPL visí na "kurz", šipka k "mít" … má viset na "mít" a šipka ke "kurz"??</t>
+  </si>
+  <si>
+    <t>obrácená anotace COMPL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">compl.rf šipka k špatnému uzlu?? </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">... jeho </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>jídlo</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> se potom </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>nejí</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> tak </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>horké</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ...</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Asi je vždycky </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ráda</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>vidíte</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> .</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Každý se </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>mi divil</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> , že </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>jsem blázen</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> , že jdu do JZD .</t>
+    </r>
+  </si>
+  <si>
+    <t>horké.COMPL má mít šipku k jídlu.PAT (ne k potom.TWHEN)</t>
+  </si>
+  <si>
+    <t>ráda.COMPL má mít šipku k ACT (ne k vždycky.TWHEN)</t>
+  </si>
+  <si>
+    <t>jsem blázen.COMPL má mít šipku k PAT (ne ke každý.ACT)</t>
+  </si>
+  <si>
+    <t>Ostatní jsou všechno naši kamarádi .</t>
+  </si>
+  <si>
+    <t>funktory ??</t>
+  </si>
+  <si>
+    <t>"ostaní" bych povzžovala za ACT, "kamarádi" za PAT (ani kontext mě nepšesvědčil, že by to mělo být opačně)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Stela Špicová , </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>provdaná</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> později Adlerová , učila taky v Kyjově .</t>
+    </r>
+  </si>
+  <si>
+    <t>??? COMPL</t>
+  </si>
+  <si>
+    <t>nerozumím, k jakému slovesu to má být COMPL??
+koref. šipka k nadřízenému subst. "Špicová"</t>
+  </si>
+  <si>
+    <t>koref. šipka k sourozenci "Korýtková" … tedy jinak než předchozí</t>
+  </si>
+  <si>
+    <t>Pak byl zaměstnaný na okresním výboru v Chebu jako okresní zootechnik .</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">… maminka Anna Ceplechová , </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>rozená</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Korýtková .</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">manuál předpokládá 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>- 1 rodiče sloveso, 
+- 2. rodiče sémantické subst. … ale může to být např. obsahová klauze (pak uzel se sempos "v"), neurč. tvar slovesa</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+??? ale i případy, kdy oba rodiče substantiva … </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 
+"…  fotografiemi sama sebe, jak se plaví nebo létá ..."</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">…, a které byly odpočitatelné jakožto platby pojistného </t>
+  </si>
+  <si>
+    <t>?? jako zootechnik.COMPL má mít šipku spíš k ACT (ne k zaměstnaný.PAT, které tvoří predikát spolu s být), to je substantivní rodič ??</t>
+  </si>
+  <si>
+    <t>??? jakožto platby.COMPL pojistného má mít šipku spíš k ACT (platby) (ne k odpočitatelný.PAT, které tvoří predikát spolu s být), to je substantivní rodič ??</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -778,6 +1248,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -820,7 +1298,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -855,10 +1333,13 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Kontrolní buňka" xfId="1" builtinId="23"/>
-    <cellStyle name="Normální" xfId="0" builtinId="0"/>
+    <cellStyle name="Check Cell" xfId="1" builtinId="23"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1128,7 +1609,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1136,18 +1617,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:E46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+    <sheetView tabSelected="1" topLeftCell="B34" workbookViewId="0">
+      <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.85546875" style="5" customWidth="1"/>
-    <col min="2" max="2" width="15.5703125" style="5" customWidth="1"/>
+    <col min="1" max="1" width="23.42578125" style="5" customWidth="1"/>
+    <col min="2" max="2" width="30.85546875" style="5" customWidth="1"/>
     <col min="3" max="3" width="54.85546875" style="4" customWidth="1"/>
-    <col min="4" max="4" width="30.140625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="49.7109375" style="5" customWidth="1"/>
     <col min="5" max="5" width="86" style="4" customWidth="1"/>
     <col min="6" max="16384" width="8.7109375" style="5"/>
   </cols>
@@ -1500,41 +1981,207 @@
       <c r="D28" s="10" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" ht="75.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="E28" s="10" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="45.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>85</v>
       </c>
-      <c r="B29" s="5" t="s">
+      <c r="B29" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C29" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="C29" s="4" t="s">
-        <v>87</v>
-      </c>
       <c r="D29" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>88</v>
-      </c>
+        <v>87</v>
+      </c>
+      <c r="B30" s="1"/>
       <c r="C30" s="4" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>97</v>
       </c>
       <c r="C31" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="D31" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="33" spans="1:5" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="B33" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D33" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="E33" s="10" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="120.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>100</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C34" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="D34" s="4"/>
+    </row>
+    <row r="35" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A35" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B36" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="D31" t="s">
-        <v>93</v>
+      <c r="C36" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="E36" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C37" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="E37" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B38" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B39" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="E39" s="4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B40" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="E40" s="4" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B41" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="E41" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B42" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="E42" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B43" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="E43" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B44" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="E44" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="B45" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="E45" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="B46" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="E46" s="4" t="s">
+        <v>126</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
possible errors in PDT (as sent to MM)
</commit_message>
<xml_diff>
--- a/tecto2umr/PDT-mozne-chyby.xlsx
+++ b/tecto2umr/PDT-mozne-chyby.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lopatkova\SVN\GitHub-UMR\tecto2umr\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28635" windowHeight="12870"/>
   </bookViews>
@@ -534,9 +529,6 @@
     <t>ID v PDT-VAllexu</t>
   </si>
   <si>
-    <t>Mně byly asi čtyři roky ... má být asi rámec v-w243f177_ZU (být-006)</t>
-  </si>
-  <si>
     <t>hg-28105_01.00-SCzechT-hg-28105_01-1955-root</t>
   </si>
   <si>
@@ -611,47 +603,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">???
-To.ACT [=argument, že všude se vyplácejí prémie za zápasy, tak proč by to u nás mělo být jinak] je (jako kdyby si stěžoval...).PAT … </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>nesedí forma ani sémantika PAT.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>?? sjednotit:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-ACT … plnovýznamové nebo ukazovací (to, tohle,   ; ALE 8x co) 
-PAT .. tázací slovo (177x co, copak; ALE 8x ten, tenhle, tenhleten)</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
@@ -1183,13 +1134,115 @@
   </si>
   <si>
     <t>??? jakožto platby.COMPL pojistného má mít šipku spíš k ACT (platby) (ne k odpočitatelný.PAT, které tvoří predikát spolu s být), to je substantivní rodič ??</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>?? sjednotit:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+ACT … plnovýznamové nebo ukazovací (to, tohle,   ; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ALE 8x co</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">) 
+PAT .. tázací slovo (177x co, copak; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ALE 8x ten, tenhle, tenhleten</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>Mně byly asi čtyři roky ... má být asi rámec v-w243f177_ZU (být-006), potvrdila Zdenka</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>???</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+To.ACT [=argument, že všude se vyplácejí prémie za zápasy, tak proč by to u nás mělo být jinak] je (jako kdyby si stěžoval...).PAT … </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>nesedí forma ani sémantika PAT.</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1256,6 +1309,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color theme="0" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -1298,7 +1359,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1336,10 +1397,13 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Check Cell" xfId="1" builtinId="23"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Kontrolní buňka" xfId="1" builtinId="23"/>
+    <cellStyle name="Normální" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1609,7 +1673,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1619,8 +1683,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B34" workbookViewId="0">
-      <selection activeCell="D43" sqref="D43"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1633,7 +1697,7 @@
     <col min="6" max="16384" width="8.7109375" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
         <v>15</v>
       </c>
@@ -1650,7 +1714,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="120.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="60.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -1726,7 +1790,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>4</v>
       </c>
@@ -1773,7 +1837,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>7</v>
       </c>
@@ -1835,7 +1899,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>11</v>
       </c>
@@ -1885,7 +1949,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="48.95" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" ht="59.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>62</v>
       </c>
@@ -1893,7 +1957,7 @@
         <v>63</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>82</v>
+        <v>126</v>
       </c>
       <c r="E21"/>
     </row>
@@ -1905,13 +1969,13 @@
         <v>64</v>
       </c>
       <c r="C22" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="D22" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="E22" s="2" t="s">
         <v>73</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -1922,46 +1986,46 @@
         <v>64</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>81</v>
+        <v>128</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="B24" s="11" t="s">
+      <c r="B24" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="C24" s="11" t="s">
-        <v>79</v>
+      <c r="C24" s="13" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B25" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="B25" s="4" t="s">
-        <v>78</v>
-      </c>
       <c r="C25" s="4" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="B26" s="11" t="s">
+      <c r="B26" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="C26" s="11" t="s">
-        <v>80</v>
+      <c r="C26" s="13" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1970,7 +2034,7 @@
     </row>
     <row r="28" spans="1:5" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="9" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B28" s="10" t="s">
         <v>17</v>
@@ -1987,48 +2051,48 @@
     </row>
     <row r="29" spans="1:5" ht="45.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C29" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D29" s="4" t="s">
         <v>86</v>
-      </c>
-      <c r="D29" s="4" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B30" s="1"/>
       <c r="C30" s="4" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="D31" t="s">
         <v>88</v>
       </c>
-      <c r="B31" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="C31" s="4" t="s">
+    </row>
+    <row r="32" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="33" spans="1:5" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="9" t="s">
         <v>92</v>
-      </c>
-      <c r="D31" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="33" spans="1:5" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="9" t="s">
-        <v>95</v>
       </c>
       <c r="B33" s="10" t="s">
         <v>17</v>
@@ -2045,148 +2109,148 @@
     </row>
     <row r="34" spans="1:5" ht="120.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C34" s="12" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="D34" s="4"/>
     </row>
     <row r="35" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B36" s="5" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="E36" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C37" s="4" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="E37" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B38" s="5" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B39" s="5" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B40" s="5" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B41" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="E41" t="s">
         <v>109</v>
-      </c>
-      <c r="C41" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="E41" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B42" s="5" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="E42" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B43" s="5" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="E43" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B44" s="5" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E44" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B45" s="5" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="E45" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B46" s="5" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="E46" s="4" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
improved FPHR mapping and another suspicious sentence in PDT-C
</commit_message>
<xml_diff>
--- a/tecto2umr/PDT-mozne-chyby.xlsx
+++ b/tecto2umr/PDT-mozne-chyby.xlsx
@@ -10,7 +10,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="145621" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="136">
   <si>
     <t>#Gen</t>
   </si>
@@ -1236,6 +1236,28 @@
       </rPr>
       <t>nesedí forma ani sémantika PAT.</t>
     </r>
+  </si>
+  <si>
+    <t>Počítačová společnost Hewlett-Packard se sídlem ve městě Palo Alto v Kalifornii uvedla, že akcie získala proto, aby "rozvíjela a udržovala strategické partnerství, ve kterém obě společnosti zůstanou nezávislé, zatímco na obchodování a prodeji svého zboží budou pracovat společně".</t>
+  </si>
+  <si>
+    <t>několik podezřelých rozhodnutí</t>
+  </si>
+  <si>
+    <t>??? ACMP</t>
+  </si>
+  <si>
+    <t>jev</t>
+  </si>
+  <si>
+    <t>společnost se sídlem.ACMP … ??? opravdu ACMP (a ne např. RSTR ???)</t>
+  </si>
+  <si>
+    <t>??? CAUS</t>
+  </si>
+  <si>
+    <t>spíš AIM??  … je to cíl/účel (do budoucna), nikoli příčina (v minulosti)
+získala akcie proto, aby rozvíjela.AIM a udržovala.AIN strategické partnerství</t>
   </si>
 </sst>
 </file>
@@ -1359,7 +1381,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1399,6 +1421,9 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1673,7 +1698,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1681,10 +1706,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E46"/>
+  <dimension ref="A1:E52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+    <sheetView tabSelected="1" topLeftCell="B40" workbookViewId="0">
+      <selection activeCell="C54" sqref="C54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2247,6 +2272,47 @@
       <c r="E46" s="4" t="s">
         <v>123</v>
       </c>
+    </row>
+    <row r="47" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="48" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="B48" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C48" s="9"/>
+      <c r="D48" s="10"/>
+      <c r="E48" s="10"/>
+    </row>
+    <row r="49" spans="1:5" ht="60.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="E49" s="14" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="B50" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="E50"/>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E51"/>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E52"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
mapping of functors (some more comments)
</commit_message>
<xml_diff>
--- a/tecto2umr/PDT-mozne-chyby.xlsx
+++ b/tecto2umr/PDT-mozne-chyby.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lopatkova\SVN\GitHub-UMR\tecto2umr\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28635" windowHeight="12870"/>
   </bookViews>
@@ -20,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="143">
   <si>
     <t>#Gen</t>
   </si>
@@ -1258,6 +1263,27 @@
   <si>
     <t>spíš AIM??  … je to cíl/účel (do budoucna), nikoli příčina (v minulosti)
 získala akcie proto, aby rozvíjela.AIM a udržovala.AIN strategické partnerství</t>
+  </si>
+  <si>
+    <t>FPHR</t>
+  </si>
+  <si>
+    <t>Mezi tyto řetězce patřily Bloomingdale's, vlastněný Campeau Corp. z Toro</t>
+  </si>
+  <si>
+    <t>slovo "vlastněný" by asi nemělo mít FPHR, ale třeba RSTR??</t>
+  </si>
+  <si>
+    <t>Health Care Property Investors Inc., nabízející 2250000 kmenových akcií</t>
+  </si>
+  <si>
+    <t>slovo "nabízející" by asi nemělo mít FPHR, ale třeba RSTR??</t>
+  </si>
+  <si>
+    <t>… její předpovědi týkající se společnosti PS of New Hampshire - například růst poptávky po elektřině či zvýšená provozní efektivita - by se nevyplnily.</t>
+  </si>
+  <si>
+    <t>PAR "například růst poptávky po elektřině či zvýšená provozní efektivita" … má spíš viset na "předpovědi", možná jako RSTR</t>
   </si>
 </sst>
 </file>
@@ -1427,8 +1453,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Kontrolní buňka" xfId="1" builtinId="23"/>
-    <cellStyle name="Normální" xfId="0" builtinId="0"/>
+    <cellStyle name="Check Cell" xfId="1" builtinId="23"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1698,7 +1724,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1706,10 +1732,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E52"/>
+  <dimension ref="A1:E54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B40" workbookViewId="0">
-      <selection activeCell="C54" sqref="C54"/>
+    <sheetView tabSelected="1" topLeftCell="B46" workbookViewId="0">
+      <selection activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2312,7 +2338,37 @@
       <c r="E51"/>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E52"/>
+      <c r="B52" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="E52" s="4" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B53" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="E53" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="B54" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="C54" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="E54" s="14" t="s">
+        <v>141</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
PDT to UMR functors
</commit_message>
<xml_diff>
--- a/tecto2umr/PDT-mozne-chyby.xlsx
+++ b/tecto2umr/PDT-mozne-chyby.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lopatkova\SVN\GitHub-UMR\tecto2umr\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28635" windowHeight="12870"/>
   </bookViews>
@@ -25,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="170">
   <si>
     <t>#Gen</t>
   </si>
@@ -1539,6 +1534,38 @@
   </si>
   <si>
     <t>T-wsj0329-001-p1s0</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Alcoa uzavřela na newyorkské burze na 72 dolarech za </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>akcii, tedy o 4.75</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> dolaru méně, a to v ostře nižším objemu obchodů.</t>
+    </r>
+  </si>
+  <si>
+    <t>CM</t>
+  </si>
+  <si>
+    <t>akcie.REG visí pod CM, asi má viset na dolaru??</t>
   </si>
 </sst>
 </file>
@@ -1730,8 +1757,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Check Cell" xfId="1" builtinId="23"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Kontrolní buňka" xfId="1" builtinId="23"/>
+    <cellStyle name="Normální" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2001,7 +2028,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2009,11 +2036,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E61"/>
+  <dimension ref="A1:E62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D60" sqref="D60"/>
+      <pane ySplit="1" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E62" sqref="E62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2785,6 +2812,17 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E61" s="3"/>
+    </row>
+    <row r="62" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B62" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="E62" s="6" t="s">
+        <v>167</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
functors - conversion (intensifiers, attitude etc., part)
</commit_message>
<xml_diff>
--- a/tecto2umr/PDT-mozne-chyby.xlsx
+++ b/tecto2umr/PDT-mozne-chyby.xlsx
@@ -1,16 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lopatkova\SVN\GitHub-UMR\tecto2umr\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28635" windowHeight="12870"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28640" windowHeight="12870"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="145621" iterateDelta="1E-4"/>
+  <calcPr calcId="152511" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="186">
   <si>
     <t>#Gen</t>
   </si>
@@ -1566,6 +1571,267 @@
   </si>
   <si>
     <t>akcie.REG visí pod CM, asi má viset na dolaru??</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Ve druhém tahu 18. týdne Sportky v I. pořadí je 1 výhra 1998352 Kč, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ve II. není žádná výhra</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, ve III. je 73 výher po 9759 Kč, ve IV. je 4630 výher po 307 Kč, v V. je 80873 výher po 37 Kč.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Nebudeme mít žáky</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> výlučně z velmi bohatých rodin, upozorňuje ředitel Ward.</t>
+    </r>
+  </si>
+  <si>
+    <t>proč negace #Neg nevisí pod slovesem "být", ale pod "žák"?</t>
+  </si>
+  <si>
+    <t>proč negace #Neg nevisí pod slovesem "být", ale pod "výhra"?
+ #Neg jen 3x pod uzlem se sempos n.denot (1x jde o deverb. "nezakázání, kde je to asi OK")</t>
+  </si>
+  <si>
+    <t>RHEM</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Společnost TRW Inc. ohlásila 12% snížení příjmů za třetí čtvrtletí, ale uvedla, že provozní zisk vzrostl o 16 %, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>nepočítaje</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> v to mimořádné zisky v obou čtvrtletích.</t>
+    </r>
+  </si>
+  <si>
+    <t>"nepočítaje" má negaci v t_lemmatu a ještě k tomu dítě #Neg.RHEM … je to OK?</t>
+  </si>
+  <si>
+    <t>INTF</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">divná t_lemmata (číslo znamená frekvenci) … nevím, jaká jsou pravidla pro anotování:
+#PersPron 24 
+on 11 (nemá se převést na #PersPron ?)
+onen 5
+tak 5
+co 3
+tenhle 2
+toť 2
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. 1
+fakt 1
+Georgias 1
+houba 1
+To 1  (nemá se převést na "ten"?)</t>
+    </r>
+  </si>
+  <si>
+    <t>PREC a jeho edítě.RSTR</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">různá lemmatizace - sjednotit ???
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"dva"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (52x, typ "na druhé straně") VS.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"druhý"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (8x, též "na druhé straně")
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"jeden"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (9x typ "v první řadě", "na jednu stranu", "na jedné straně")  VS.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"první"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 4 ("v první řadě")</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">"Ještě nejsme v žádném případě z této situace venku," řekl George R. Mateyo, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>prezident a výkonný ředitel společnosti Carnegie Capital Management Co. z Clevelandu.</t>
+    </r>
+  </si>
+  <si>
+    <t>PREC a jeho edítě.DIR1</t>
+  </si>
+  <si>
+    <t>"společnost" nemá být PREC !!!</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Ortega ukončil příměří s opozičními silami, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>známými</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> jako Contras, a prohlásil, že volby byly ohroženy.</t>
+    </r>
+  </si>
+  <si>
+    <t>chybí sempos u slova "známý"</t>
   </si>
 </sst>
 </file>
@@ -1695,7 +1961,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1755,10 +2021,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Kontrolní buňka" xfId="1" builtinId="23"/>
-    <cellStyle name="Normální" xfId="0" builtinId="0"/>
+    <cellStyle name="Check Cell" xfId="1" builtinId="23"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2028,7 +2295,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2036,24 +2303,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E62"/>
+  <dimension ref="A1:E69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E62" sqref="E62"/>
+      <pane ySplit="1" topLeftCell="A67" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D75" sqref="D75"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.42578125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="30.85546875" style="3" customWidth="1"/>
-    <col min="3" max="3" width="54.85546875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="49.7109375" style="3" customWidth="1"/>
+    <col min="1" max="1" width="23.453125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="30.81640625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="54.81640625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="49.7265625" style="3" customWidth="1"/>
     <col min="5" max="5" width="86" style="2" customWidth="1"/>
-    <col min="6" max="16384" width="8.7109375" style="3"/>
+    <col min="6" max="16384" width="8.7265625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
         <v>15</v>
       </c>
@@ -2070,7 +2337,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="9" customFormat="1" ht="60.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" s="9" customFormat="1" ht="58.5" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
@@ -2087,7 +2354,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="9" customFormat="1" ht="135" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" s="9" customFormat="1" ht="116" x14ac:dyDescent="0.35">
       <c r="A3" s="7" t="s">
         <v>1</v>
       </c>
@@ -2104,7 +2371,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" s="9" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="7" t="s">
         <v>2</v>
       </c>
@@ -2119,7 +2386,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="7" t="s">
         <v>13</v>
       </c>
@@ -2132,7 +2399,7 @@
       </c>
       <c r="E5" s="7"/>
     </row>
-    <row r="6" spans="1:5" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="7" t="s">
         <v>3</v>
       </c>
@@ -2147,7 +2414,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" s="9" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" s="7" t="s">
         <v>4</v>
       </c>
@@ -2164,7 +2431,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:5" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" s="9" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" s="7" t="s">
         <v>5</v>
       </c>
@@ -2179,7 +2446,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:5" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" s="9" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A9" s="7" t="s">
         <v>6</v>
       </c>
@@ -2194,7 +2461,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:5" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" s="9" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A10" s="7" t="s">
         <v>7</v>
       </c>
@@ -2211,7 +2478,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:5" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" s="9" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A11" s="7" t="s">
         <v>8</v>
       </c>
@@ -2226,7 +2493,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A12" s="7" t="s">
         <v>9</v>
       </c>
@@ -2241,7 +2508,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="13" spans="1:5" s="9" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" s="9" customFormat="1" ht="58" x14ac:dyDescent="0.35">
       <c r="A13" s="7" t="s">
         <v>10</v>
       </c>
@@ -2256,7 +2523,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="14" spans="1:5" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" s="9" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A14" s="7" t="s">
         <v>11</v>
       </c>
@@ -2273,7 +2540,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="15" spans="1:5" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" s="9" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A15" s="7" t="s">
         <v>12</v>
       </c>
@@ -2288,23 +2555,23 @@
         <v>59</v>
       </c>
     </row>
-    <row r="16" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="C16" s="7"/>
       <c r="E16" s="7"/>
     </row>
-    <row r="17" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="C17" s="7"/>
       <c r="E17" s="7"/>
     </row>
-    <row r="18" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="C18" s="7"/>
       <c r="E18" s="7"/>
     </row>
-    <row r="19" spans="1:5" s="9" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" s="9" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C19" s="7"/>
       <c r="E19" s="7"/>
     </row>
-    <row r="20" spans="1:5" s="9" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" s="9" customFormat="1" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="14" t="s">
         <v>70</v>
       </c>
@@ -2321,7 +2588,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="21" spans="1:5" s="9" customFormat="1" ht="59.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" s="9" customFormat="1" ht="59.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A21" s="7" t="s">
         <v>62</v>
       </c>
@@ -2333,7 +2600,7 @@
       </c>
       <c r="E21" s="11"/>
     </row>
-    <row r="22" spans="1:5" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" s="9" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A22" s="7" t="s">
         <v>65</v>
       </c>
@@ -2350,7 +2617,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="23" spans="1:5" s="9" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" s="9" customFormat="1" ht="58" x14ac:dyDescent="0.35">
       <c r="A23" s="7" t="s">
         <v>65</v>
       </c>
@@ -2367,7 +2634,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="24" spans="1:5" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" s="9" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A24" s="17" t="s">
         <v>67</v>
       </c>
@@ -2379,7 +2646,7 @@
       </c>
       <c r="E24" s="7"/>
     </row>
-    <row r="25" spans="1:5" s="9" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" s="9" customFormat="1" ht="87" x14ac:dyDescent="0.35">
       <c r="A25" s="7" t="s">
         <v>76</v>
       </c>
@@ -2391,7 +2658,7 @@
       </c>
       <c r="E25" s="7"/>
     </row>
-    <row r="26" spans="1:5" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" s="9" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A26" s="17" t="s">
         <v>69</v>
       </c>
@@ -2403,13 +2670,13 @@
       </c>
       <c r="E26" s="7"/>
     </row>
-    <row r="27" spans="1:5" s="9" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" s="9" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27" s="7"/>
       <c r="B27" s="7"/>
       <c r="C27" s="7"/>
       <c r="E27" s="7"/>
     </row>
-    <row r="28" spans="1:5" s="9" customFormat="1" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" s="9" customFormat="1" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A28" s="14" t="s">
         <v>81</v>
       </c>
@@ -2426,7 +2693,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="29" spans="1:5" s="9" customFormat="1" ht="45.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" s="9" customFormat="1" ht="44" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A29" s="11" t="s">
         <v>82</v>
       </c>
@@ -2441,7 +2708,7 @@
       </c>
       <c r="E29" s="7"/>
     </row>
-    <row r="30" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A30" s="11" t="s">
         <v>84</v>
       </c>
@@ -2454,7 +2721,7 @@
       </c>
       <c r="E30" s="7"/>
     </row>
-    <row r="31" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A31" s="9" t="s">
         <v>85</v>
       </c>
@@ -2469,11 +2736,11 @@
       </c>
       <c r="E31" s="7"/>
     </row>
-    <row r="32" spans="1:5" s="9" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" s="9" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C32" s="7"/>
       <c r="E32" s="7"/>
     </row>
-    <row r="33" spans="1:5" s="9" customFormat="1" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" s="9" customFormat="1" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A33" s="14" t="s">
         <v>92</v>
       </c>
@@ -2490,7 +2757,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="34" spans="1:5" s="9" customFormat="1" ht="120.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" s="9" customFormat="1" ht="102" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A34" s="11" t="s">
         <v>97</v>
       </c>
@@ -2503,7 +2770,7 @@
       <c r="D34" s="7"/>
       <c r="E34" s="7"/>
     </row>
-    <row r="35" spans="1:5" s="9" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" s="9" customFormat="1" ht="58" x14ac:dyDescent="0.35">
       <c r="A35" s="7" t="s">
         <v>90</v>
       </c>
@@ -2514,7 +2781,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="36" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B36" s="9" t="s">
         <v>91</v>
       </c>
@@ -2525,7 +2792,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="37" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="C37" s="7" t="s">
         <v>96</v>
       </c>
@@ -2533,7 +2800,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="38" spans="1:5" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" s="9" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="B38" s="9" t="s">
         <v>105</v>
       </c>
@@ -2544,7 +2811,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="39" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B39" s="9" t="s">
         <v>106</v>
       </c>
@@ -2555,7 +2822,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="40" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B40" s="9" t="s">
         <v>106</v>
       </c>
@@ -2566,7 +2833,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="41" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B41" s="9" t="s">
         <v>106</v>
       </c>
@@ -2577,7 +2844,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="42" spans="1:5" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" s="9" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="B42" s="9" t="s">
         <v>114</v>
       </c>
@@ -2588,7 +2855,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="43" spans="1:5" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" s="9" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="B43" s="9" t="s">
         <v>117</v>
       </c>
@@ -2599,7 +2866,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="44" spans="1:5" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" s="9" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="B44" s="9" t="s">
         <v>117</v>
       </c>
@@ -2610,7 +2877,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="45" spans="1:5" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" s="9" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B45" s="9" t="s">
         <v>106</v>
       </c>
@@ -2621,7 +2888,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="46" spans="1:5" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" s="9" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B46" s="9" t="s">
         <v>106</v>
       </c>
@@ -2632,14 +2899,14 @@
         <v>123</v>
       </c>
     </row>
-    <row r="47" spans="1:5" s="9" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" s="9" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A47" s="9" t="s">
         <v>141</v>
       </c>
       <c r="C47" s="7"/>
       <c r="E47" s="7"/>
     </row>
-    <row r="48" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A48" s="4" t="s">
         <v>131</v>
       </c>
@@ -2650,7 +2917,7 @@
       <c r="D48" s="5"/>
       <c r="E48" s="5"/>
     </row>
-    <row r="49" spans="1:5" ht="60.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" ht="44" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
         <v>129</v>
       </c>
@@ -2667,7 +2934,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="B50" s="3" t="s">
         <v>133</v>
       </c>
@@ -2681,10 +2948,10 @@
         <v>142</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
       <c r="E51"/>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B52" s="3" t="s">
         <v>135</v>
       </c>
@@ -2698,7 +2965,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B53" s="3" t="s">
         <v>135</v>
       </c>
@@ -2712,7 +2979,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="54" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="B54" s="3" t="s">
         <v>135</v>
       </c>
@@ -2726,7 +2993,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="55" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="B55" s="3" t="s">
         <v>135</v>
       </c>
@@ -2740,7 +3007,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="56" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B56" s="3" t="s">
         <v>135</v>
       </c>
@@ -2754,7 +3021,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="57" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="B57" s="3" t="s">
         <v>135</v>
       </c>
@@ -2768,7 +3035,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="58" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" ht="87" x14ac:dyDescent="0.35">
       <c r="B58" s="3" t="s">
         <v>135</v>
       </c>
@@ -2782,7 +3049,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="59" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="B59" s="3" t="s">
         <v>135</v>
       </c>
@@ -2796,7 +3063,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="60" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="B60" s="3" t="s">
         <v>135</v>
       </c>
@@ -2810,10 +3077,10 @@
         <v>155</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
       <c r="E61" s="3"/>
     </row>
-    <row r="62" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="B62" s="3" t="s">
         <v>168</v>
       </c>
@@ -2822,6 +3089,75 @@
       </c>
       <c r="E62" s="6" t="s">
         <v>167</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B63" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="D63" s="2"/>
+      <c r="E63" s="21" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B64" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="E64" s="21" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="65" spans="2:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="B65" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="E65" s="2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="66" spans="2:5" ht="203" x14ac:dyDescent="0.35">
+      <c r="B66" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="67" spans="2:5" ht="87" x14ac:dyDescent="0.35">
+      <c r="B67" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="68" spans="2:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="B68" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="E68" s="6" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="69" spans="2:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="C69" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="E69" s="2" t="s">
+        <v>184</v>
       </c>
     </row>
   </sheetData>
@@ -2836,7 +3172,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
functors - conversion, esp. more notes on MOD
</commit_message>
<xml_diff>
--- a/tecto2umr/PDT-mozne-chyby.xlsx
+++ b/tecto2umr/PDT-mozne-chyby.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511" iterateDelta="1E-4"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="188">
   <si>
     <t>#Gen</t>
   </si>
@@ -1832,6 +1832,36 @@
   </si>
   <si>
     <t>chybí sempos u slova "známý"</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">V boji o Bílý dům je volič </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>nepatrně více</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> motivován k tomu, aby se přiklonil k republikánům.</t>
+    </r>
+  </si>
+  <si>
+    <t>"nepatrně" spíš vidí na "hodně"? 
+a není to spíš EXT (podobně 5 dalších vět s nepatrně.MOD)</t>
   </si>
 </sst>
 </file>
@@ -2303,11 +2333,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E69"/>
+  <dimension ref="A1:E70"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A67" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D75" sqref="D75"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A64" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D67" sqref="D67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3158,6 +3188,14 @@
       </c>
       <c r="E69" s="2" t="s">
         <v>184</v>
+      </c>
+    </row>
+    <row r="70" spans="2:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="C70" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="E70" s="6" t="s">
+        <v>186</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
functors - MOD finished
</commit_message>
<xml_diff>
--- a/tecto2umr/PDT-mozne-chyby.xlsx
+++ b/tecto2umr/PDT-mozne-chyby.xlsx
@@ -1,21 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lopatkova\SVN\GitHub-UMR\tecto2umr\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28640" windowHeight="12870"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28635" windowHeight="12870"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="190">
   <si>
     <t>#Gen</t>
   </si>
@@ -1862,6 +1857,57 @@
   <si>
     <t>"nepatrně" spíš vidí na "hodně"? 
 a není to spíš EXT (podobně 5 dalších vět s nepatrně.MOD)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">V obecné škole jsem v </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>každém</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> případě byla jediná Židovka .
+V </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>každém</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> případě zareagovaly makléřské firmy ve výrobě nových reklam zřetelně rychleji než při pádu v roce 1987.</t>
+    </r>
+  </si>
+  <si>
+    <t>?? každý --&gt; který (jako v 5 jiných větách)</t>
   </si>
 </sst>
 </file>
@@ -2054,8 +2100,8 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Check Cell" xfId="1" builtinId="23"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Kontrolní buňka" xfId="1" builtinId="23"/>
+    <cellStyle name="Normální" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2325,7 +2371,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2333,24 +2379,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E70"/>
+  <dimension ref="A1:E71"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A64" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D67" sqref="D67"/>
+      <selection pane="bottomLeft" activeCell="E66" sqref="E66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.453125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="30.81640625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="54.81640625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="49.7265625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="23.42578125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="30.85546875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="54.85546875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="49.7109375" style="3" customWidth="1"/>
     <col min="5" max="5" width="86" style="2" customWidth="1"/>
-    <col min="6" max="16384" width="8.7265625" style="3"/>
+    <col min="6" max="16384" width="8.7109375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:5" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>15</v>
       </c>
@@ -2367,7 +2413,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="9" customFormat="1" ht="58.5" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" s="9" customFormat="1" ht="60.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
@@ -2384,7 +2430,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="9" customFormat="1" ht="116" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" s="9" customFormat="1" ht="135" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>1</v>
       </c>
@@ -2401,7 +2447,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="9" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>2</v>
       </c>
@@ -2416,7 +2462,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>13</v>
       </c>
@@ -2429,7 +2475,7 @@
       </c>
       <c r="E5" s="7"/>
     </row>
-    <row r="6" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>3</v>
       </c>
@@ -2444,7 +2490,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="9" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>4</v>
       </c>
@@ -2461,7 +2507,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:5" s="9" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>5</v>
       </c>
@@ -2476,7 +2522,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:5" s="9" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>6</v>
       </c>
@@ -2491,7 +2537,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:5" s="9" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>7</v>
       </c>
@@ -2508,7 +2554,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:5" s="9" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>8</v>
       </c>
@@ -2523,7 +2569,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>9</v>
       </c>
@@ -2538,7 +2584,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="13" spans="1:5" s="9" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" s="9" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>10</v>
       </c>
@@ -2553,7 +2599,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="14" spans="1:5" s="9" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>11</v>
       </c>
@@ -2570,7 +2616,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="15" spans="1:5" s="9" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>12</v>
       </c>
@@ -2585,23 +2631,23 @@
         <v>59</v>
       </c>
     </row>
-    <row r="16" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" s="9" customFormat="1" ht="14.45" x14ac:dyDescent="0.35">
       <c r="C16" s="7"/>
       <c r="E16" s="7"/>
     </row>
-    <row r="17" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" s="9" customFormat="1" ht="14.45" x14ac:dyDescent="0.35">
       <c r="C17" s="7"/>
       <c r="E17" s="7"/>
     </row>
-    <row r="18" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" s="9" customFormat="1" ht="14.45" x14ac:dyDescent="0.35">
       <c r="C18" s="7"/>
       <c r="E18" s="7"/>
     </row>
-    <row r="19" spans="1:5" s="9" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:5" s="9" customFormat="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C19" s="7"/>
       <c r="E19" s="7"/>
     </row>
-    <row r="20" spans="1:5" s="9" customFormat="1" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:5" s="9" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="14" t="s">
         <v>70</v>
       </c>
@@ -2618,7 +2664,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="21" spans="1:5" s="9" customFormat="1" ht="59.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" s="9" customFormat="1" ht="59.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>62</v>
       </c>
@@ -2630,7 +2676,7 @@
       </c>
       <c r="E21" s="11"/>
     </row>
-    <row r="22" spans="1:5" s="9" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>65</v>
       </c>
@@ -2647,7 +2693,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="23" spans="1:5" s="9" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" s="9" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>65</v>
       </c>
@@ -2664,7 +2710,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="24" spans="1:5" s="9" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="17" t="s">
         <v>67</v>
       </c>
@@ -2676,7 +2722,7 @@
       </c>
       <c r="E24" s="7"/>
     </row>
-    <row r="25" spans="1:5" s="9" customFormat="1" ht="87" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" s="9" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>76</v>
       </c>
@@ -2688,7 +2734,7 @@
       </c>
       <c r="E25" s="7"/>
     </row>
-    <row r="26" spans="1:5" s="9" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" s="17" t="s">
         <v>69</v>
       </c>
@@ -2700,13 +2746,13 @@
       </c>
       <c r="E26" s="7"/>
     </row>
-    <row r="27" spans="1:5" s="9" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:5" s="9" customFormat="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27" s="7"/>
       <c r="B27" s="7"/>
       <c r="C27" s="7"/>
       <c r="E27" s="7"/>
     </row>
-    <row r="28" spans="1:5" s="9" customFormat="1" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:5" s="9" customFormat="1" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="14" t="s">
         <v>81</v>
       </c>
@@ -2723,7 +2769,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="29" spans="1:5" s="9" customFormat="1" ht="44" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" s="9" customFormat="1" ht="45.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A29" s="11" t="s">
         <v>82</v>
       </c>
@@ -2738,7 +2784,7 @@
       </c>
       <c r="E29" s="7"/>
     </row>
-    <row r="30" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="11" t="s">
         <v>84</v>
       </c>
@@ -2751,7 +2797,7 @@
       </c>
       <c r="E30" s="7"/>
     </row>
-    <row r="31" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="9" t="s">
         <v>85</v>
       </c>
@@ -2766,11 +2812,11 @@
       </c>
       <c r="E31" s="7"/>
     </row>
-    <row r="32" spans="1:5" s="9" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:5" s="9" customFormat="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C32" s="7"/>
       <c r="E32" s="7"/>
     </row>
-    <row r="33" spans="1:5" s="9" customFormat="1" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:5" s="9" customFormat="1" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="14" t="s">
         <v>92</v>
       </c>
@@ -2787,7 +2833,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="34" spans="1:5" s="9" customFormat="1" ht="102" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:5" s="9" customFormat="1" ht="120.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A34" s="11" t="s">
         <v>97</v>
       </c>
@@ -2800,7 +2846,7 @@
       <c r="D34" s="7"/>
       <c r="E34" s="7"/>
     </row>
-    <row r="35" spans="1:5" s="9" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:5" s="9" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
         <v>90</v>
       </c>
@@ -2811,7 +2857,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="36" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B36" s="9" t="s">
         <v>91</v>
       </c>
@@ -2822,7 +2868,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="37" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C37" s="7" t="s">
         <v>96</v>
       </c>
@@ -2830,7 +2876,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="38" spans="1:5" s="9" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:5" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B38" s="9" t="s">
         <v>105</v>
       </c>
@@ -2841,7 +2887,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="39" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B39" s="9" t="s">
         <v>106</v>
       </c>
@@ -2852,7 +2898,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="40" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B40" s="9" t="s">
         <v>106</v>
       </c>
@@ -2863,7 +2909,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="41" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B41" s="9" t="s">
         <v>106</v>
       </c>
@@ -2874,7 +2920,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="42" spans="1:5" s="9" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:5" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B42" s="9" t="s">
         <v>114</v>
       </c>
@@ -2885,7 +2931,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="43" spans="1:5" s="9" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:5" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B43" s="9" t="s">
         <v>117</v>
       </c>
@@ -2896,7 +2942,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="44" spans="1:5" s="9" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:5" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B44" s="9" t="s">
         <v>117</v>
       </c>
@@ -2907,7 +2953,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="45" spans="1:5" s="9" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:5" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="B45" s="9" t="s">
         <v>106</v>
       </c>
@@ -2918,7 +2964,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="46" spans="1:5" s="9" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:5" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="B46" s="9" t="s">
         <v>106</v>
       </c>
@@ -2929,14 +2975,14 @@
         <v>123</v>
       </c>
     </row>
-    <row r="47" spans="1:5" s="9" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:5" s="9" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="9" t="s">
         <v>141</v>
       </c>
       <c r="C47" s="7"/>
       <c r="E47" s="7"/>
     </row>
-    <row r="48" spans="1:5" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A48" s="4" t="s">
         <v>131</v>
       </c>
@@ -2947,7 +2993,7 @@
       <c r="D48" s="5"/>
       <c r="E48" s="5"/>
     </row>
-    <row r="49" spans="1:5" ht="44" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:5" ht="60.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>129</v>
       </c>
@@ -2964,7 +3010,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B50" s="3" t="s">
         <v>133</v>
       </c>
@@ -2978,10 +3024,10 @@
         <v>142</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
       <c r="E51"/>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B52" s="3" t="s">
         <v>135</v>
       </c>
@@ -2995,7 +3041,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B53" s="3" t="s">
         <v>135</v>
       </c>
@@ -3009,7 +3055,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="54" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B54" s="3" t="s">
         <v>135</v>
       </c>
@@ -3023,7 +3069,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="55" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B55" s="3" t="s">
         <v>135</v>
       </c>
@@ -3037,7 +3083,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="56" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B56" s="3" t="s">
         <v>135</v>
       </c>
@@ -3051,7 +3097,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="57" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B57" s="3" t="s">
         <v>135</v>
       </c>
@@ -3065,7 +3111,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="58" spans="1:5" ht="87" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="B58" s="3" t="s">
         <v>135</v>
       </c>
@@ -3079,7 +3125,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="59" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B59" s="3" t="s">
         <v>135</v>
       </c>
@@ -3093,7 +3139,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="60" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B60" s="3" t="s">
         <v>135</v>
       </c>
@@ -3107,10 +3153,10 @@
         <v>155</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
       <c r="E61" s="3"/>
     </row>
-    <row r="62" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B62" s="3" t="s">
         <v>168</v>
       </c>
@@ -3121,7 +3167,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="63" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B63" s="3" t="s">
         <v>174</v>
       </c>
@@ -3133,7 +3179,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B64" s="3" t="s">
         <v>174</v>
       </c>
@@ -3144,7 +3190,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="65" spans="2:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="65" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B65" s="3" t="s">
         <v>174</v>
       </c>
@@ -3155,7 +3201,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="66" spans="2:5" ht="203" x14ac:dyDescent="0.35">
+    <row r="66" spans="2:5" ht="210" x14ac:dyDescent="0.25">
       <c r="B66" s="3" t="s">
         <v>177</v>
       </c>
@@ -3163,7 +3209,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="67" spans="2:5" ht="87" x14ac:dyDescent="0.35">
+    <row r="67" spans="2:5" ht="90" x14ac:dyDescent="0.25">
       <c r="B67" s="3" t="s">
         <v>179</v>
       </c>
@@ -3171,7 +3217,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="68" spans="2:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="68" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B68" s="3" t="s">
         <v>182</v>
       </c>
@@ -3182,7 +3228,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="69" spans="2:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="69" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="C69" s="2" t="s">
         <v>185</v>
       </c>
@@ -3190,12 +3236,20 @@
         <v>184</v>
       </c>
     </row>
-    <row r="70" spans="2:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="70" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="C70" s="2" t="s">
         <v>187</v>
       </c>
       <c r="E70" s="6" t="s">
         <v>186</v>
+      </c>
+    </row>
+    <row r="71" spans="2:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="C71" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="E71" s="2" t="s">
+        <v>188</v>
       </c>
     </row>
   </sheetData>
@@ -3210,7 +3264,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
more on functors (clausal markers)
</commit_message>
<xml_diff>
--- a/tecto2umr/PDT-mozne-chyby.xlsx
+++ b/tecto2umr/PDT-mozne-chyby.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lopatkova\SVN\GitHub-UMR\tecto2umr\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28635" windowHeight="12870"/>
   </bookViews>
@@ -20,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="193">
   <si>
     <t>#Gen</t>
   </si>
@@ -1909,12 +1914,21 @@
   <si>
     <t>?? každý --&gt; který (jako v 5 jiných větách)</t>
   </si>
+  <si>
+    <t xml:space="preserve">Tento.RSTR nátlak.ACT byl.PRED nepochybně.(t_lemma = "pochybně").MOD slabý.PAT </t>
+  </si>
+  <si>
+    <t>t_lemma … pochybně --&gt; nepochybně")</t>
+  </si>
+  <si>
+    <t>wsj0936s26</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2037,7 +2051,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -2098,10 +2112,13 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Kontrolní buňka" xfId="1" builtinId="23"/>
-    <cellStyle name="Normální" xfId="0" builtinId="0"/>
+    <cellStyle name="Check Cell" xfId="1" builtinId="23"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2371,7 +2388,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2379,14 +2396,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E71"/>
+  <dimension ref="A1:E72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A64" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E66" sqref="E66"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D72" sqref="D72"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="23.42578125" style="3" customWidth="1"/>
     <col min="2" max="2" width="30.85546875" style="3" customWidth="1"/>
@@ -2396,7 +2413,7 @@
     <col min="6" max="16384" width="8.7109375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="31.5" thickTop="1" thickBot="1">
       <c r="A1" s="4" t="s">
         <v>15</v>
       </c>
@@ -2413,7 +2430,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="9" customFormat="1" ht="60.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" s="9" customFormat="1" ht="60.75" thickTop="1">
       <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
@@ -2430,7 +2447,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="9" customFormat="1" ht="135" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" s="9" customFormat="1" ht="135">
       <c r="A3" s="7" t="s">
         <v>1</v>
       </c>
@@ -2447,7 +2464,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" s="9" customFormat="1" ht="30">
       <c r="A4" s="7" t="s">
         <v>2</v>
       </c>
@@ -2462,7 +2479,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" s="9" customFormat="1">
       <c r="A5" s="7" t="s">
         <v>13</v>
       </c>
@@ -2475,7 +2492,7 @@
       </c>
       <c r="E5" s="7"/>
     </row>
-    <row r="6" spans="1:5" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" s="9" customFormat="1" ht="30">
       <c r="A6" s="7" t="s">
         <v>3</v>
       </c>
@@ -2490,7 +2507,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" s="9" customFormat="1" ht="30">
       <c r="A7" s="7" t="s">
         <v>4</v>
       </c>
@@ -2507,7 +2524,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:5" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" s="9" customFormat="1" ht="30">
       <c r="A8" s="7" t="s">
         <v>5</v>
       </c>
@@ -2522,7 +2539,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:5" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" s="9" customFormat="1" ht="45">
       <c r="A9" s="7" t="s">
         <v>6</v>
       </c>
@@ -2537,7 +2554,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:5" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" s="9" customFormat="1" ht="30">
       <c r="A10" s="7" t="s">
         <v>7</v>
       </c>
@@ -2554,7 +2571,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:5" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" s="9" customFormat="1" ht="30">
       <c r="A11" s="7" t="s">
         <v>8</v>
       </c>
@@ -2569,7 +2586,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" s="9" customFormat="1">
       <c r="A12" s="7" t="s">
         <v>9</v>
       </c>
@@ -2584,7 +2601,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="13" spans="1:5" s="9" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" s="9" customFormat="1" ht="60">
       <c r="A13" s="7" t="s">
         <v>10</v>
       </c>
@@ -2599,7 +2616,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="14" spans="1:5" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" s="9" customFormat="1" ht="30">
       <c r="A14" s="7" t="s">
         <v>11</v>
       </c>
@@ -2616,7 +2633,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="15" spans="1:5" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" s="9" customFormat="1" ht="30">
       <c r="A15" s="7" t="s">
         <v>12</v>
       </c>
@@ -2631,23 +2648,23 @@
         <v>59</v>
       </c>
     </row>
-    <row r="16" spans="1:5" s="9" customFormat="1" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" s="9" customFormat="1" ht="14.45">
       <c r="C16" s="7"/>
       <c r="E16" s="7"/>
     </row>
-    <row r="17" spans="1:5" s="9" customFormat="1" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" s="9" customFormat="1" ht="14.45">
       <c r="C17" s="7"/>
       <c r="E17" s="7"/>
     </row>
-    <row r="18" spans="1:5" s="9" customFormat="1" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" s="9" customFormat="1" ht="14.45">
       <c r="C18" s="7"/>
       <c r="E18" s="7"/>
     </row>
-    <row r="19" spans="1:5" s="9" customFormat="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:5" s="9" customFormat="1" thickBot="1">
       <c r="C19" s="7"/>
       <c r="E19" s="7"/>
     </row>
-    <row r="20" spans="1:5" s="9" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" s="9" customFormat="1" ht="16.5" thickTop="1" thickBot="1">
       <c r="A20" s="14" t="s">
         <v>70</v>
       </c>
@@ -2664,7 +2681,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="21" spans="1:5" s="9" customFormat="1" ht="59.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" s="9" customFormat="1" ht="59.25" customHeight="1" thickTop="1">
       <c r="A21" s="7" t="s">
         <v>62</v>
       </c>
@@ -2676,7 +2693,7 @@
       </c>
       <c r="E21" s="11"/>
     </row>
-    <row r="22" spans="1:5" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" s="9" customFormat="1" ht="30">
       <c r="A22" s="7" t="s">
         <v>65</v>
       </c>
@@ -2693,7 +2710,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="23" spans="1:5" s="9" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" s="9" customFormat="1" ht="60">
       <c r="A23" s="7" t="s">
         <v>65</v>
       </c>
@@ -2710,7 +2727,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="24" spans="1:5" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" s="9" customFormat="1" ht="30">
       <c r="A24" s="17" t="s">
         <v>67</v>
       </c>
@@ -2722,7 +2739,7 @@
       </c>
       <c r="E24" s="7"/>
     </row>
-    <row r="25" spans="1:5" s="9" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" s="9" customFormat="1" ht="90">
       <c r="A25" s="7" t="s">
         <v>76</v>
       </c>
@@ -2734,7 +2751,7 @@
       </c>
       <c r="E25" s="7"/>
     </row>
-    <row r="26" spans="1:5" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" s="9" customFormat="1" ht="45">
       <c r="A26" s="17" t="s">
         <v>69</v>
       </c>
@@ -2746,13 +2763,13 @@
       </c>
       <c r="E26" s="7"/>
     </row>
-    <row r="27" spans="1:5" s="9" customFormat="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:5" s="9" customFormat="1" thickBot="1">
       <c r="A27" s="7"/>
       <c r="B27" s="7"/>
       <c r="C27" s="7"/>
       <c r="E27" s="7"/>
     </row>
-    <row r="28" spans="1:5" s="9" customFormat="1" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" s="9" customFormat="1" ht="31.5" thickTop="1" thickBot="1">
       <c r="A28" s="14" t="s">
         <v>81</v>
       </c>
@@ -2769,7 +2786,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="29" spans="1:5" s="9" customFormat="1" ht="45.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" s="9" customFormat="1" ht="45.75" thickTop="1">
       <c r="A29" s="11" t="s">
         <v>82</v>
       </c>
@@ -2784,7 +2801,7 @@
       </c>
       <c r="E29" s="7"/>
     </row>
-    <row r="30" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" s="9" customFormat="1">
       <c r="A30" s="11" t="s">
         <v>84</v>
       </c>
@@ -2797,7 +2814,7 @@
       </c>
       <c r="E30" s="7"/>
     </row>
-    <row r="31" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" s="9" customFormat="1">
       <c r="A31" s="9" t="s">
         <v>85</v>
       </c>
@@ -2812,11 +2829,11 @@
       </c>
       <c r="E31" s="7"/>
     </row>
-    <row r="32" spans="1:5" s="9" customFormat="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:5" s="9" customFormat="1" thickBot="1">
       <c r="C32" s="7"/>
       <c r="E32" s="7"/>
     </row>
-    <row r="33" spans="1:5" s="9" customFormat="1" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" s="9" customFormat="1" ht="31.5" thickTop="1" thickBot="1">
       <c r="A33" s="14" t="s">
         <v>92</v>
       </c>
@@ -2833,7 +2850,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="34" spans="1:5" s="9" customFormat="1" ht="120.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" s="9" customFormat="1" ht="120.75" thickTop="1">
       <c r="A34" s="11" t="s">
         <v>97</v>
       </c>
@@ -2846,7 +2863,7 @@
       <c r="D34" s="7"/>
       <c r="E34" s="7"/>
     </row>
-    <row r="35" spans="1:5" s="9" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" s="9" customFormat="1" ht="60">
       <c r="A35" s="7" t="s">
         <v>90</v>
       </c>
@@ -2857,7 +2874,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="36" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" s="9" customFormat="1">
       <c r="B36" s="9" t="s">
         <v>91</v>
       </c>
@@ -2868,7 +2885,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="37" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" s="9" customFormat="1">
       <c r="C37" s="7" t="s">
         <v>96</v>
       </c>
@@ -2876,7 +2893,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="38" spans="1:5" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" s="9" customFormat="1" ht="30">
       <c r="B38" s="9" t="s">
         <v>105</v>
       </c>
@@ -2887,7 +2904,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="39" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" s="9" customFormat="1">
       <c r="B39" s="9" t="s">
         <v>106</v>
       </c>
@@ -2898,7 +2915,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="40" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" s="9" customFormat="1">
       <c r="B40" s="9" t="s">
         <v>106</v>
       </c>
@@ -2909,7 +2926,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="41" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" s="9" customFormat="1">
       <c r="B41" s="9" t="s">
         <v>106</v>
       </c>
@@ -2920,7 +2937,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="42" spans="1:5" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" s="9" customFormat="1" ht="30">
       <c r="B42" s="9" t="s">
         <v>114</v>
       </c>
@@ -2931,7 +2948,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="43" spans="1:5" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" s="9" customFormat="1" ht="30">
       <c r="B43" s="9" t="s">
         <v>117</v>
       </c>
@@ -2942,7 +2959,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="44" spans="1:5" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" s="9" customFormat="1" ht="30">
       <c r="B44" s="9" t="s">
         <v>117</v>
       </c>
@@ -2953,7 +2970,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="45" spans="1:5" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" s="9" customFormat="1" ht="45">
       <c r="B45" s="9" t="s">
         <v>106</v>
       </c>
@@ -2964,7 +2981,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="46" spans="1:5" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" s="9" customFormat="1" ht="45">
       <c r="B46" s="9" t="s">
         <v>106</v>
       </c>
@@ -2975,14 +2992,14 @@
         <v>123</v>
       </c>
     </row>
-    <row r="47" spans="1:5" s="9" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" s="9" customFormat="1" ht="15.75" thickBot="1">
       <c r="A47" s="9" t="s">
         <v>141</v>
       </c>
       <c r="C47" s="7"/>
       <c r="E47" s="7"/>
     </row>
-    <row r="48" spans="1:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:5" ht="15.6" thickTop="1" thickBot="1">
       <c r="A48" s="4" t="s">
         <v>131</v>
       </c>
@@ -2993,7 +3010,7 @@
       <c r="D48" s="5"/>
       <c r="E48" s="5"/>
     </row>
-    <row r="49" spans="1:5" ht="60.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" ht="60.75" thickTop="1">
       <c r="A49" s="1" t="s">
         <v>129</v>
       </c>
@@ -3010,7 +3027,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" ht="60">
       <c r="B50" s="3" t="s">
         <v>133</v>
       </c>
@@ -3024,10 +3041,10 @@
         <v>142</v>
       </c>
     </row>
-    <row r="51" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:5" ht="14.45">
       <c r="E51"/>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5">
       <c r="B52" s="3" t="s">
         <v>135</v>
       </c>
@@ -3041,7 +3058,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5">
       <c r="B53" s="3" t="s">
         <v>135</v>
       </c>
@@ -3055,7 +3072,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="54" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" ht="45">
       <c r="B54" s="3" t="s">
         <v>135</v>
       </c>
@@ -3069,7 +3086,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="55" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" ht="30">
       <c r="B55" s="3" t="s">
         <v>135</v>
       </c>
@@ -3083,7 +3100,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="56" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" ht="45">
       <c r="B56" s="3" t="s">
         <v>135</v>
       </c>
@@ -3097,7 +3114,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="57" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" ht="30">
       <c r="B57" s="3" t="s">
         <v>135</v>
       </c>
@@ -3111,7 +3128,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="58" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" ht="90">
       <c r="B58" s="3" t="s">
         <v>135</v>
       </c>
@@ -3125,7 +3142,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="59" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" ht="30">
       <c r="B59" s="3" t="s">
         <v>135</v>
       </c>
@@ -3139,7 +3156,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="60" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" ht="30">
       <c r="B60" s="3" t="s">
         <v>135</v>
       </c>
@@ -3153,10 +3170,10 @@
         <v>155</v>
       </c>
     </row>
-    <row r="61" spans="1:5" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:5" ht="14.45">
       <c r="E61" s="3"/>
     </row>
-    <row r="62" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" ht="30">
       <c r="B62" s="3" t="s">
         <v>168</v>
       </c>
@@ -3167,7 +3184,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="63" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" ht="60">
       <c r="B63" s="3" t="s">
         <v>174</v>
       </c>
@@ -3175,11 +3192,11 @@
         <v>173</v>
       </c>
       <c r="D63" s="2"/>
-      <c r="E63" s="21" t="s">
+      <c r="E63" s="22" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="64" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" ht="30">
       <c r="B64" s="3" t="s">
         <v>174</v>
       </c>
@@ -3190,7 +3207,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="65" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:5" ht="30">
       <c r="B65" s="3" t="s">
         <v>174</v>
       </c>
@@ -3201,7 +3218,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="66" spans="2:5" ht="210" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:5" ht="210">
       <c r="B66" s="3" t="s">
         <v>177</v>
       </c>
@@ -3209,7 +3226,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="67" spans="2:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:5" ht="90">
       <c r="B67" s="3" t="s">
         <v>179</v>
       </c>
@@ -3217,7 +3234,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="68" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:5" ht="30">
       <c r="B68" s="3" t="s">
         <v>182</v>
       </c>
@@ -3228,7 +3245,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="69" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:5" ht="30">
       <c r="C69" s="2" t="s">
         <v>185</v>
       </c>
@@ -3236,7 +3253,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="70" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:5" ht="30">
       <c r="C70" s="2" t="s">
         <v>187</v>
       </c>
@@ -3244,12 +3261,23 @@
         <v>186</v>
       </c>
     </row>
-    <row r="71" spans="2:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:5" ht="60">
       <c r="C71" s="2" t="s">
         <v>189</v>
       </c>
       <c r="E71" s="2" t="s">
         <v>188</v>
+      </c>
+    </row>
+    <row r="72" spans="2:5">
+      <c r="C72" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="D72" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="E72" s="2" t="s">
+        <v>190</v>
       </c>
     </row>
   </sheetData>
@@ -3264,7 +3292,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
small correction (CM functor)
</commit_message>
<xml_diff>
--- a/tecto2umr/PDT-mozne-chyby.xlsx
+++ b/tecto2umr/PDT-mozne-chyby.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lopatkova\SVN\GitHub-UMR\tecto2umr\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28635" windowHeight="12870"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28640" windowHeight="12870"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2436,7 +2441,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2451,6 +2456,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2483,7 +2500,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -2572,16 +2589,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Kontrolní buňka" xfId="1" builtinId="23"/>
-    <cellStyle name="Normální" xfId="0" builtinId="0"/>
+    <cellStyle name="Check Cell" xfId="1" builtinId="23"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -2842,7 +2868,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2853,21 +2879,21 @@
   <dimension ref="A1:E91"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A75" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D81" sqref="D81"/>
+      <pane ySplit="1" topLeftCell="A63" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D64" sqref="D64"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.42578125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="30.85546875" style="3" customWidth="1"/>
-    <col min="3" max="3" width="54.85546875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="49.7109375" style="3" customWidth="1"/>
+    <col min="1" max="1" width="23.453125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="30.81640625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="54.81640625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="49.7265625" style="3" customWidth="1"/>
     <col min="5" max="5" width="86" style="2" customWidth="1"/>
-    <col min="6" max="16384" width="8.7109375" style="3"/>
+    <col min="6" max="16384" width="8.7265625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
         <v>15</v>
       </c>
@@ -2884,7 +2910,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="8" customFormat="1" ht="60.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" s="8" customFormat="1" ht="58.5" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
@@ -2901,7 +2927,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="8" customFormat="1" ht="135" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" s="8" customFormat="1" ht="116" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
@@ -2918,7 +2944,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" s="8" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="6" t="s">
         <v>2</v>
       </c>
@@ -2933,7 +2959,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="6" t="s">
         <v>13</v>
       </c>
@@ -2946,7 +2972,7 @@
       </c>
       <c r="E5" s="6"/>
     </row>
-    <row r="6" spans="1:5" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="6" t="s">
         <v>3</v>
       </c>
@@ -2961,7 +2987,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" s="8" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" s="6" t="s">
         <v>4</v>
       </c>
@@ -2978,7 +3004,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:5" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" s="8" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" s="6" t="s">
         <v>5</v>
       </c>
@@ -2993,7 +3019,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:5" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" s="8" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A9" s="6" t="s">
         <v>6</v>
       </c>
@@ -3008,7 +3034,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:5" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" s="8" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A10" s="6" t="s">
         <v>7</v>
       </c>
@@ -3025,7 +3051,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:5" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" s="8" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A11" s="6" t="s">
         <v>8</v>
       </c>
@@ -3040,7 +3066,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A12" s="6" t="s">
         <v>9</v>
       </c>
@@ -3055,7 +3081,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="13" spans="1:5" s="8" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" s="8" customFormat="1" ht="58" x14ac:dyDescent="0.35">
       <c r="A13" s="6" t="s">
         <v>10</v>
       </c>
@@ -3070,7 +3096,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="14" spans="1:5" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" s="8" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A14" s="6" t="s">
         <v>11</v>
       </c>
@@ -3087,7 +3113,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="15" spans="1:5" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" s="8" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A15" s="6" t="s">
         <v>12</v>
       </c>
@@ -3102,23 +3128,23 @@
         <v>59</v>
       </c>
     </row>
-    <row r="16" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="C16" s="6"/>
       <c r="E16" s="6"/>
     </row>
-    <row r="17" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="C17" s="6"/>
       <c r="E17" s="6"/>
     </row>
-    <row r="18" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="C18" s="6"/>
       <c r="E18" s="6"/>
     </row>
-    <row r="19" spans="1:5" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" s="8" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C19" s="6"/>
       <c r="E19" s="6"/>
     </row>
-    <row r="20" spans="1:5" s="8" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" s="8" customFormat="1" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="13" t="s">
         <v>70</v>
       </c>
@@ -3135,7 +3161,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="21" spans="1:5" s="8" customFormat="1" ht="59.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" s="8" customFormat="1" ht="59.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A21" s="6" t="s">
         <v>62</v>
       </c>
@@ -3147,7 +3173,7 @@
       </c>
       <c r="E21" s="11"/>
     </row>
-    <row r="22" spans="1:5" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" s="8" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A22" s="6" t="s">
         <v>65</v>
       </c>
@@ -3164,7 +3190,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="23" spans="1:5" s="8" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" s="8" customFormat="1" ht="58" x14ac:dyDescent="0.35">
       <c r="A23" s="6" t="s">
         <v>65</v>
       </c>
@@ -3181,7 +3207,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="24" spans="1:5" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" s="8" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A24" s="16" t="s">
         <v>67</v>
       </c>
@@ -3193,7 +3219,7 @@
       </c>
       <c r="E24" s="6"/>
     </row>
-    <row r="25" spans="1:5" s="8" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" s="8" customFormat="1" ht="87" x14ac:dyDescent="0.35">
       <c r="A25" s="6" t="s">
         <v>76</v>
       </c>
@@ -3205,7 +3231,7 @@
       </c>
       <c r="E25" s="6"/>
     </row>
-    <row r="26" spans="1:5" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" s="8" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A26" s="16" t="s">
         <v>69</v>
       </c>
@@ -3217,13 +3243,13 @@
       </c>
       <c r="E26" s="6"/>
     </row>
-    <row r="27" spans="1:5" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" s="8" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27" s="6"/>
       <c r="B27" s="6"/>
       <c r="C27" s="6"/>
       <c r="E27" s="6"/>
     </row>
-    <row r="28" spans="1:5" s="8" customFormat="1" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" s="8" customFormat="1" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A28" s="13" t="s">
         <v>81</v>
       </c>
@@ -3240,7 +3266,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="29" spans="1:5" s="8" customFormat="1" ht="45.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" s="8" customFormat="1" ht="44" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A29" s="10" t="s">
         <v>82</v>
       </c>
@@ -3255,7 +3281,7 @@
       </c>
       <c r="E29" s="6"/>
     </row>
-    <row r="30" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A30" s="10" t="s">
         <v>84</v>
       </c>
@@ -3268,7 +3294,7 @@
       </c>
       <c r="E30" s="6"/>
     </row>
-    <row r="31" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A31" s="8" t="s">
         <v>85</v>
       </c>
@@ -3283,11 +3309,11 @@
       </c>
       <c r="E31" s="6"/>
     </row>
-    <row r="32" spans="1:5" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" s="8" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C32" s="6"/>
       <c r="E32" s="6"/>
     </row>
-    <row r="33" spans="1:5" s="8" customFormat="1" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" s="8" customFormat="1" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A33" s="13" t="s">
         <v>92</v>
       </c>
@@ -3304,7 +3330,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="34" spans="1:5" s="8" customFormat="1" ht="120.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" s="8" customFormat="1" ht="102" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A34" s="10" t="s">
         <v>97</v>
       </c>
@@ -3317,7 +3343,7 @@
       <c r="D34" s="6"/>
       <c r="E34" s="6"/>
     </row>
-    <row r="35" spans="1:5" s="8" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" s="8" customFormat="1" ht="58" x14ac:dyDescent="0.35">
       <c r="A35" s="6" t="s">
         <v>90</v>
       </c>
@@ -3328,7 +3354,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="36" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B36" s="8" t="s">
         <v>91</v>
       </c>
@@ -3339,7 +3365,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="37" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="C37" s="6" t="s">
         <v>96</v>
       </c>
@@ -3347,7 +3373,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="38" spans="1:5" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" s="8" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="B38" s="8" t="s">
         <v>105</v>
       </c>
@@ -3358,7 +3384,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="39" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B39" s="8" t="s">
         <v>106</v>
       </c>
@@ -3369,7 +3395,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="40" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B40" s="8" t="s">
         <v>106</v>
       </c>
@@ -3380,7 +3406,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="41" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B41" s="8" t="s">
         <v>106</v>
       </c>
@@ -3391,7 +3417,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="42" spans="1:5" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" s="8" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="B42" s="8" t="s">
         <v>114</v>
       </c>
@@ -3402,7 +3428,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="43" spans="1:5" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" s="8" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="B43" s="8" t="s">
         <v>117</v>
       </c>
@@ -3413,7 +3439,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="44" spans="1:5" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" s="8" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="B44" s="8" t="s">
         <v>117</v>
       </c>
@@ -3424,7 +3450,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="45" spans="1:5" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" s="8" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B45" s="8" t="s">
         <v>106</v>
       </c>
@@ -3435,7 +3461,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="46" spans="1:5" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" s="8" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B46" s="8" t="s">
         <v>106</v>
       </c>
@@ -3446,14 +3472,14 @@
         <v>123</v>
       </c>
     </row>
-    <row r="47" spans="1:5" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" s="8" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A47" s="8" t="s">
         <v>141</v>
       </c>
       <c r="C47" s="6"/>
       <c r="E47" s="6"/>
     </row>
-    <row r="48" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A48" s="4" t="s">
         <v>131</v>
       </c>
@@ -3464,7 +3490,7 @@
       <c r="D48" s="5"/>
       <c r="E48" s="5"/>
     </row>
-    <row r="49" spans="1:5" ht="60.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" ht="44" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
         <v>129</v>
       </c>
@@ -3481,7 +3507,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="B50" s="3" t="s">
         <v>133</v>
       </c>
@@ -3495,7 +3521,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B51" s="3" t="s">
         <v>135</v>
       </c>
@@ -3509,7 +3535,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B52" s="3" t="s">
         <v>135</v>
       </c>
@@ -3523,7 +3549,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="53" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="B53" s="3" t="s">
         <v>135</v>
       </c>
@@ -3537,7 +3563,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="54" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="B54" s="3" t="s">
         <v>135</v>
       </c>
@@ -3551,7 +3577,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="55" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B55" s="3" t="s">
         <v>135</v>
       </c>
@@ -3565,7 +3591,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="56" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="B56" s="3" t="s">
         <v>135</v>
       </c>
@@ -3579,7 +3605,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="57" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" ht="87" x14ac:dyDescent="0.35">
       <c r="B57" s="3" t="s">
         <v>135</v>
       </c>
@@ -3593,7 +3619,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="58" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="B58" s="3" t="s">
         <v>135</v>
       </c>
@@ -3607,7 +3633,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="59" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="B59" s="3" t="s">
         <v>135</v>
       </c>
@@ -3621,7 +3647,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="60" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="B60" s="3" t="s">
         <v>168</v>
       </c>
@@ -3635,7 +3661,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="61" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B61" s="3" t="s">
         <v>174</v>
       </c>
@@ -3649,7 +3675,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="62" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B62" s="3" t="s">
         <v>174</v>
       </c>
@@ -3663,7 +3689,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="63" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="B63" s="3" t="s">
         <v>174</v>
       </c>
@@ -3677,58 +3703,64 @@
         <v>175</v>
       </c>
     </row>
-    <row r="64" spans="1:5" ht="210" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" ht="203" x14ac:dyDescent="0.35">
       <c r="B64" s="3" t="s">
         <v>177</v>
       </c>
       <c r="C64" s="2" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="65" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="D64" s="32"/>
+    </row>
+    <row r="65" spans="1:5" ht="87" x14ac:dyDescent="0.35">
       <c r="B65" s="3" t="s">
         <v>178</v>
       </c>
       <c r="C65" s="2" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="66" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="D65" s="33"/>
+    </row>
+    <row r="66" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="B66" s="3" t="s">
         <v>181</v>
       </c>
       <c r="C66" s="2" t="s">
         <v>182</v>
       </c>
+      <c r="D66" s="33"/>
       <c r="E66" s="1" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="67" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="C67" s="2" t="s">
         <v>184</v>
       </c>
+      <c r="D67" s="33"/>
       <c r="E67" s="2" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="68" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="C68" s="2" t="s">
         <v>186</v>
       </c>
+      <c r="D68" s="33"/>
       <c r="E68" s="1" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="69" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="C69" s="2" t="s">
         <v>188</v>
       </c>
+      <c r="D69" s="33"/>
       <c r="E69" s="2" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
       <c r="C70" s="2" t="s">
         <v>190</v>
       </c>
@@ -3739,7 +3771,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="71" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A71" s="23"/>
       <c r="B71" s="23"/>
       <c r="C71" s="28" t="s">
@@ -3752,18 +3784,18 @@
         <v>199</v>
       </c>
     </row>
-    <row r="72" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A72" s="23"/>
       <c r="B72" s="23"/>
       <c r="C72" s="24" t="s">
         <v>200</v>
       </c>
-      <c r="D72" s="23"/>
+      <c r="D72" s="33"/>
       <c r="E72" s="24" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A73" s="23"/>
       <c r="B73" s="23"/>
       <c r="C73" s="24" t="s">
@@ -3776,60 +3808,60 @@
         <v>204</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A74" s="23"/>
       <c r="B74" s="23"/>
       <c r="C74" s="24" t="s">
         <v>205</v>
       </c>
-      <c r="D74" s="23"/>
+      <c r="D74" s="33"/>
       <c r="E74" s="24" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="75" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A75" s="23"/>
       <c r="B75" s="23"/>
       <c r="C75" s="24" t="s">
         <v>207</v>
       </c>
-      <c r="D75" s="23"/>
+      <c r="D75" s="33"/>
       <c r="E75" s="24" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="76" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A76" s="23"/>
       <c r="B76" s="23"/>
       <c r="C76" s="24" t="s">
         <v>209</v>
       </c>
-      <c r="D76" s="23"/>
+      <c r="D76" s="33"/>
       <c r="E76" s="24" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="77" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="B77" s="23"/>
       <c r="C77" s="24" t="s">
         <v>211</v>
       </c>
-      <c r="D77" s="23"/>
+      <c r="D77" s="33"/>
       <c r="E77" s="24" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="78" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B78" s="23"/>
       <c r="C78" s="24" t="s">
         <v>213</v>
       </c>
-      <c r="D78" s="23"/>
+      <c r="D78" s="33"/>
       <c r="E78" s="24" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="79" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="B79" s="25" t="s">
         <v>215</v>
       </c>
@@ -3843,7 +3875,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="80" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="B80" s="25" t="s">
         <v>215</v>
       </c>
@@ -3857,7 +3889,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="81" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:5" ht="29" x14ac:dyDescent="0.35">
       <c r="B81" s="25" t="s">
         <v>215</v>
       </c>
@@ -3871,7 +3903,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="82" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B82" s="25" t="s">
         <v>215</v>
       </c>
@@ -3885,7 +3917,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="83" spans="2:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B83" s="25" t="s">
         <v>215</v>
       </c>
@@ -3899,7 +3931,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="84" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:5" ht="29" x14ac:dyDescent="0.35">
       <c r="B84" s="25" t="s">
         <v>215</v>
       </c>
@@ -3913,7 +3945,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="85" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:5" ht="29" x14ac:dyDescent="0.35">
       <c r="B85" s="25" t="s">
         <v>215</v>
       </c>
@@ -3927,7 +3959,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="86" spans="2:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:5" ht="58" x14ac:dyDescent="0.35">
       <c r="B86" s="25" t="s">
         <v>236</v>
       </c>
@@ -3941,7 +3973,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="87" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:5" ht="29" x14ac:dyDescent="0.35">
       <c r="B87" s="25" t="s">
         <v>240</v>
       </c>
@@ -3955,7 +3987,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="88" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:5" ht="29" x14ac:dyDescent="0.35">
       <c r="B88" s="3" t="s">
         <v>244</v>
       </c>
@@ -3969,7 +4001,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="89" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:5" ht="29" x14ac:dyDescent="0.35">
       <c r="C89" s="2" t="s">
         <v>246</v>
       </c>
@@ -3980,7 +4012,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="90" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:5" ht="29" x14ac:dyDescent="0.35">
       <c r="C90" s="24" t="s">
         <v>246</v>
       </c>
@@ -3991,7 +4023,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="91" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:5" ht="29" x14ac:dyDescent="0.35">
       <c r="C91" s="2" t="s">
         <v>253</v>
       </c>
@@ -4014,7 +4046,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
updated list of suspicious PDT annotations (as sent to MM)
</commit_message>
<xml_diff>
--- a/tecto2umr/PDT-mozne-chyby.xlsx
+++ b/tecto2umr/PDT-mozne-chyby.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lopatkova\SVN\GitHub-UMR\tecto2umr\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28640" windowHeight="12870"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28635" windowHeight="12870"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="266">
   <si>
     <t>#Gen</t>
   </si>
@@ -1774,35 +1769,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Ortega ukončil příměří s opozičními silami, </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>známými</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> jako Contras, a prohlásil, že volby byly ohroženy.</t>
-    </r>
-  </si>
-  <si>
-    <t>chybí sempos u slova "známý"</t>
-  </si>
-  <si>
-    <r>
       <t xml:space="preserve">V boji o Bílý dům je volič </t>
     </r>
     <r>
@@ -1826,10 +1792,6 @@
       </rPr>
       <t xml:space="preserve"> motivován k tomu, aby se přiklonil k republikánům.</t>
     </r>
-  </si>
-  <si>
-    <t>"nepatrně" spíš vidí na "hodně"? 
-a není to spíš EXT (podobně 5 dalších vět s nepatrně.MOD)</t>
   </si>
   <si>
     <r>
@@ -1883,15 +1845,6 @@
     <t>?? každý --&gt; který (jako v 5 jiných větách)</t>
   </si>
   <si>
-    <t xml:space="preserve">Tento.RSTR nátlak.ACT byl.PRED nepochybně.(t_lemma = "pochybně").MOD slabý.PAT </t>
-  </si>
-  <si>
-    <t>t_lemma … pochybně --&gt; nepochybně")</t>
-  </si>
-  <si>
-    <t>wsj0936s26</t>
-  </si>
-  <si>
     <t>T-wsj2450-001-p1s12</t>
   </si>
   <si>
@@ -1904,16 +1857,391 @@
     <t>T-wsj2148-001-p1s0</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>divná t_lemmata (číslo znamená frekvenci</t>
+    <t>?? koord. substantiva, 
+obvykleji jako koordinace s elipsou slovesa (= nechtěl jsem výhody, ale chtěl jsem jednání)</t>
+  </si>
+  <si>
+    <t>jg-27638_04.04-SCzechT-jg-27638_04-3583-root</t>
+  </si>
+  <si>
+    <t>Nechtěl jsem žádné výhody , ale slušné jednání .</t>
+  </si>
+  <si>
+    <t xml:space="preserve">faust_2010_07_jh_05-SCzechT-p0436-s1A-root </t>
+  </si>
+  <si>
+    <t>?? jak se pozná, k čemu patří #Neg (k být, nikoli k trávit)</t>
+  </si>
+  <si>
+    <t>?? jak se pozná, k čemu patří #Neg (k prvnímu nezdálo)</t>
+  </si>
+  <si>
+    <t>GRAD</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">poznámka anotátora o chybné TR u "ale.GRAD" 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">??? asi není GRAD ??? </t>
+    </r>
+  </si>
+  <si>
+    <t>t-cmpr9413-008-p9s1</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> Firmy, které nejsou ochotny uvádět svou celou adresu, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ale</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> jen P.O.Box, raději jako obchodní partnery nebrat.</t>
+    </r>
+  </si>
+  <si>
+    <t>"jen" pod slovesem (jako RHEM), většinou (cca 60x) jako L bratr "#Neg.CM" s funktorem CM</t>
+  </si>
+  <si>
+    <t>t-cmpr9410-017-p12s1</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Manažerský svazový fond </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>se proto neorientuje jen na soustřeďování uchazečů</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> o zaměstnání a nabídku firem při jejich umístění, ale věnuje významnou pozornost práci s uchazeči a nalezení profesí, ve kterých zájemci mohou najít uplatnění podle svých dosavadních činností a podle poptávky.</t>
+    </r>
+  </si>
+  <si>
+    <t>t-ln94205-130-p4s12B</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Poprvé </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>nejste jenom lezec, ale i</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> organizátor a vedoucí výpravy.</t>
+    </r>
+  </si>
+  <si>
+    <t>ani - ani … opravdu je GRAD?? spíš CONJ?</t>
+  </si>
+  <si>
+    <t>es_149.07-SCzechT-es_149-d1e1482-x2-root</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Myslím si , že ne , že na to </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">nemají ani prostředky , ani síly </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>ne - ale … opravdu je GRAD?? spíš DISJ?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">t-cmpr9410-023-p4s4 </t>
+  </si>
+  <si>
+    <t>Neklade si za cíl detailně a vyčerpávajícím způsobem popsat jednotlivá témata, ale především upozornit na možné situace, v nichž se podnikatel může ocitnout, na možnosti a postupy, které při rozvoji své firmy může využít.</t>
+  </si>
+  <si>
+    <t>"jenom" zanořené (jako RHEM), většinou (cca 60x) jako L bratr "#Neg.CM" s funktorem CM</t>
+  </si>
+  <si>
+    <t>t-ln94200-30-p4s2</t>
+  </si>
+  <si>
+    <t>Nejde jenom o samotný příliv peněz, ale také o vytváření pracovních příležitostí, zvyšování kvalifikace pracovních sil, zavádění know-how.</t>
+  </si>
+  <si>
+    <t>není GRAD, viz pozn. anotátora (chce ADVS)</t>
+  </si>
+  <si>
+    <t>t-ln94200-127-p32s1</t>
+  </si>
+  <si>
+    <t>Když naposledy vstupovalo do EU Rakousko, nebylo konfrontováno s celým balíkem asi 120 tisíc jejích norem, ale jen asi s 1500, na něž Unie položila důraz.</t>
+  </si>
+  <si>
+    <t>aniž.CONJ</t>
+  </si>
+  <si>
+    <t>překombinované … asi nemá být druhé (generované) "poskytnout", ale pod "aniž" přímo sloveso "složit"
+(alespoň podle jiných vět s aniž.CONJ, pod nímž je #Neg.CM)</t>
+  </si>
+  <si>
+    <t>T-wsj1490-001-p1s18</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Investiční bankéři nicméně říkají, že banky pravděpodobně neposkytnou téměř 5 miliard dolarů, které jsou k převzetí společnosti nutné, ani za nižší cenu, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">aniž by někdo složil </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>pořádný balík peněz v hotovosti - pravděpodobně ještě větší než oněch 17 % v hotovosti, složených v červenci investory na zadlužené převzetí mateřské společnosti firmy Northwest Airlines, společnosti NWA Corp.</t>
+    </r>
+  </si>
+  <si>
+    <t>#Neg.RHEM</t>
+  </si>
+  <si>
+    <t>?? negace patří ke slovesu??</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Ve druhém tahu 18. týdne Sportky v I. pořadí je 1 výhra 1998352 Kč, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ve II. není žádná výhra</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, ve III. je 73 výher po 9759 Kč, ve IV. je 4630 výher po 307 Kč, v V. je 80873 výher po 37 Kč.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Christie ' s</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> brzy spustí aukci umění ve stylu dada a symbolismu, zatímco Sotheby láká sběratele aukcemi švýcarských, německých, španělských, australských a kanadských malířů.</t>
+    </r>
+  </si>
+  <si>
+    <t>#Forn</t>
+  </si>
+  <si>
+    <t>#Forn by mělo být ACT (ne ID)</t>
+  </si>
+  <si>
+    <t>stát je sempos n (nikoli v)!!</t>
+  </si>
+  <si>
+    <t>T-wsj2055-001-p1s33</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Americká Komise pro rovné pracovní příležitosti (EEOC) zažalovala </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>stát</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> New York za věkovou diskriminaci jmenovaných státních soudců.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Právě včera oznámil </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>stát</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> New Hampshire, že se se společností Drexel vyrovnal ve výši 75000 dolarů, což je v tomto státě rekordní pokuta ve věci práva cenných papírů.</t>
+    </r>
+  </si>
+  <si>
+    <t>T-wsj0469-001-p1s0  NEBO T-wsj1296-001-p1s3</t>
+  </si>
+  <si>
+    <t>t-ln94204-96-p2s2</t>
+  </si>
+  <si>
+    <r>
+      <t>Modlitba k Janince Jiřího Gruši s grafikou Jana Součka a</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Jedna loď</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (Laura Blair) Ivana Diviše s ilustrací Vladimíra Tesaře výrazně čerpají z již vydaných nebibliofilských verzí.</t>
+    </r>
+  </si>
+  <si>
+    <t>?? proč není "(sbírka) Jedna loď" ACT … divná anotace, nerozumím jí</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>divná t_lemmata u INTF (číslo znamená frekvenci</t>
     </r>
     <r>
       <rPr>
@@ -1950,415 +2278,433 @@
     </r>
   </si>
   <si>
-    <t>?? koord. substantiva, 
-obvykleji jako koordinace s elipsou slovesa (= nechtěl jsem výhody, ale chtěl jsem jednání)</t>
-  </si>
-  <si>
-    <t>jg-27638_04.04-SCzechT-jg-27638_04-3583-root</t>
-  </si>
-  <si>
-    <t>Nechtěl jsem žádné výhody , ale slušné jednání .</t>
-  </si>
-  <si>
-    <t>???</t>
-  </si>
-  <si>
-    <t>Nebyla účelem velká prohlídka , pouze zastavit se a podívat se na tehdejší trhy , které tam byly , a pokračovat dál .</t>
-  </si>
-  <si>
-    <t>?? prož negace až za "vidět" a za čárkou</t>
-  </si>
-  <si>
-    <t xml:space="preserve">faust_2010_07_jh_05-SCzechT-p0436-s1A-root </t>
-  </si>
-  <si>
-    <t>Normální kamarádi tuhle vnitřní bolest nevidí , jenom mí nejbližší ji poznají .</t>
-  </si>
-  <si>
-    <t>?? jak se pozná, k čemu patří #Neg (k být, nikoli k trávit)</t>
-  </si>
-  <si>
-    <t>Tam se dalo ve skupině , aniž byla příliš podezřelá , trávit řadu týdnů .</t>
-  </si>
-  <si>
-    <t>?? jak se pozná, k čemu patří #Neg (k prvnímu nezdálo)</t>
-  </si>
-  <si>
-    <t>Jako odborník jsem měl za úkol , abych všechno , co se mně nezdálo na jatka , ale k dalšímu chovu , dostával do svých stájí .</t>
-  </si>
-  <si>
-    <t xml:space="preserve">#Neg až za ADVS, patří k "odevzdávat" </t>
-  </si>
-  <si>
-    <t>Řekla : " Půjdeme tam dopoledne na cihly a dostaneme tam oběd , aniž bychom odevzdávaly přídělové lístky . "</t>
-  </si>
-  <si>
-    <t xml:space="preserve">#Neg až za ADVS, patří k "měnit" </t>
-  </si>
-  <si>
-    <t>Zvoníci poté začnou na znamení měnit pořadí, v němž zvony znějí, aniž by měnili pravidelný rytmus úderů.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">#Neg až za ADVS, patří k "změnit_se" </t>
-  </si>
-  <si>
-    <t>Když je odpověď na kritiku pouze lepším vysvětlením strategií, aniž by se změnily důvody té kritiky, jsem přesvědčen, že pan Kageyama stále nezaútočil na základní příčinu problému a léčí jen jeho příznaky.</t>
-  </si>
-  <si>
-    <t>GRAD</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">poznámka anotátora o chybné TR u "ale.GRAD" 
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">??? asi není GRAD ??? </t>
-    </r>
-  </si>
-  <si>
-    <t>t-cmpr9413-008-p9s1</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve"> Firmy, které nejsou ochotny uvádět svou celou adresu, </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>ale</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> jen P.O.Box, raději jako obchodní partnery nebrat.</t>
-    </r>
-  </si>
-  <si>
-    <t>"jen" pod slovesem (jako RHEM), většinou (cca 60x) jako L bratr "#Neg.CM" s funktorem CM</t>
-  </si>
-  <si>
-    <t>t-cmpr9410-017-p12s1</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Manažerský svazový fond </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>se proto neorientuje jen na soustřeďování uchazečů</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> o zaměstnání a nabídku firem při jejich umístění, ale věnuje významnou pozornost práci s uchazeči a nalezení profesí, ve kterých zájemci mohou najít uplatnění podle svých dosavadních činností a podle poptávky.</t>
-    </r>
-  </si>
-  <si>
-    <t>t-ln94205-130-p4s12B</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Poprvé </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>nejste jenom lezec, ale i</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> organizátor a vedoucí výpravy.</t>
-    </r>
-  </si>
-  <si>
-    <t>ani - ani … opravdu je GRAD?? spíš CONJ?</t>
-  </si>
-  <si>
-    <t>es_149.07-SCzechT-es_149-d1e1482-x2-root</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Myslím si , že ne , že na to </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">nemají ani prostředky , ani síly </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.</t>
-    </r>
-  </si>
-  <si>
-    <t>ne - ale … opravdu je GRAD?? spíš DISJ?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">t-cmpr9410-023-p4s4 </t>
-  </si>
-  <si>
-    <t>Neklade si za cíl detailně a vyčerpávajícím způsobem popsat jednotlivá témata, ale především upozornit na možné situace, v nichž se podnikatel může ocitnout, na možnosti a postupy, které při rozvoji své firmy může využít.</t>
-  </si>
-  <si>
-    <t>"jenom" zanořené (jako RHEM), většinou (cca 60x) jako L bratr "#Neg.CM" s funktorem CM</t>
-  </si>
-  <si>
-    <t>t-ln94200-30-p4s2</t>
-  </si>
-  <si>
-    <t>Nejde jenom o samotný příliv peněz, ale také o vytváření pracovních příležitostí, zvyšování kvalifikace pracovních sil, zavádění know-how.</t>
-  </si>
-  <si>
-    <t>není GRAD, viz pozn. anotátora (chce ADVS)</t>
-  </si>
-  <si>
-    <t>t-ln94200-127-p32s1</t>
-  </si>
-  <si>
-    <t>Když naposledy vstupovalo do EU Rakousko, nebylo konfrontováno s celým balíkem asi 120 tisíc jejích norem, ale jen asi s 1500, na něž Unie položila důraz.</t>
-  </si>
-  <si>
-    <t>aniž.CONJ</t>
-  </si>
-  <si>
-    <t>překombinované … asi nemá být druhé (generované) "poskytnout", ale pod "aniž" přímo sloveso "složit"
-(alespoň podle jiných vět s aniž.CONJ, pod nímž je #Neg.CM)</t>
-  </si>
-  <si>
-    <t>T-wsj1490-001-p1s18</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Investiční bankéři nicméně říkají, že banky pravděpodobně neposkytnou téměř 5 miliard dolarů, které jsou k převzetí společnosti nutné, ani za nižší cenu, </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">aniž by někdo složil </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>pořádný balík peněz v hotovosti - pravděpodobně ještě větší než oněch 17 % v hotovosti, složených v červenci investory na zadlužené převzetí mateřské společnosti firmy Northwest Airlines, společnosti NWA Corp.</t>
-    </r>
-  </si>
-  <si>
-    <t>#Neg.RHEM</t>
-  </si>
-  <si>
-    <t>?? negace patří ke slovesu??</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Ve druhém tahu 18. týdne Sportky v I. pořadí je 1 výhra 1998352 Kč, </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>ve II. není žádná výhra</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>, ve III. je 73 výher po 9759 Kč, ve IV. je 4630 výher po 307 Kč, v V. je 80873 výher po 37 Kč.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Christie ' s</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> brzy spustí aukci umění ve stylu dada a symbolismu, zatímco Sotheby láká sběratele aukcemi švýcarských, německých, španělských, australských a kanadských malířů.</t>
-    </r>
-  </si>
-  <si>
-    <t>#Forn</t>
-  </si>
-  <si>
-    <t>#Forn by mělo být ACT (ne ID)</t>
-  </si>
-  <si>
-    <t>stát je sempos n (nikoli v)!!</t>
-  </si>
-  <si>
-    <t>T-wsj2055-001-p1s33</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Americká Komise pro rovné pracovní příležitosti (EEOC) zažalovala </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>stát</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> New York za věkovou diskriminaci jmenovaných státních soudců.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Právě včera oznámil </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>stát</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> New Hampshire, že se se společností Drexel vyrovnal ve výši 75000 dolarů, což je v tomto státě rekordní pokuta ve věci práva cenných papírů.</t>
-    </r>
-  </si>
-  <si>
-    <t>T-wsj0469-001-p1s0  NEBO T-wsj1296-001-p1s3</t>
-  </si>
-  <si>
-    <t>t-ln94204-96-p2s2</t>
-  </si>
-  <si>
-    <r>
-      <t>Modlitba k Janince Jiřího Gruši s grafikou Jana Součka a</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Jedna loď</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> (Laura Blair) Ivana Diviše s ilustrací Vladimíra Tesaře výrazně čerpají z již vydaných nebibliofilských verzí.</t>
-    </r>
-  </si>
-  <si>
-    <t>?? proč není "(sbírka) Jedna loď" ACT … divná anotace, nerozumím jí</t>
+    <t>T-wsj1694-001-p1s22</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Ortega ukončil příměří s opozičními silami, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>známými</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> jako Contras, a prohlásil, že volby byly ohroženy.
+Rozsah propouštění není </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>znám,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> avšak bude zaměřeno na divizi výzkumu a výroby, která má na starost objevování zásob ropy, hloubení ropných vrtů a čerpání nafty a zemního plynu.
+Říkal jsem tomu mému </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>známému</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> : " Bude to paráda , budeme spát v hotelu Bělehrad . "</t>
+    </r>
+  </si>
+  <si>
+    <t>3x chybí sempos u slova "známý"</t>
+  </si>
+  <si>
+    <t>lk_035.07-SCzechT-lk_035-1514-root
+T-wsj0174-001-p1s0
+T-wsj1148-001-p1s1</t>
+  </si>
+  <si>
+    <t>"nepatrně" spíš visí na "hodně"? 
+a není to spíš EXT (podobně 5 dalších vět s nepatrně.MOD)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T-wsj1695-001-p1s15 </t>
+  </si>
+  <si>
+    <t>lk-26171_01.01-SCzechT-lk-26171_01-d1e393-x4-root
+T-wsj2201-001-p1s42</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">např. Tento.RSTR nátlak.ACT byl.PRED </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>nepochybně</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">.(t_lemma = "pochybně").MOD slabý.PAT </t>
+    </r>
+  </si>
+  <si>
+    <t>27x, např. wsj0936s26</t>
+  </si>
+  <si>
+    <t>t_lemma … pochybně --&gt; nepochybně ???
+nebo kde je zachycena info o negaci ??? (v Manuálu jsem nenašla)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">??? nerozumím moc anotaci - jak se pozná, k čemu patří #Neg.CM (prohlídka nebyla účelem) a k čemu pouze.CM (pouze bylo účelem) ...
+spíš bych doplnila na něco jako: "nebyla" účelem prohlídka, pouze [bylo účelem] zastavit se a ... </t>
+  </si>
+  <si>
+    <t>lk_123.06-SCzechT-lk_123-285-root</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Nebyla účelem</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> velká prohlídka , </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>pouze</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> zastavit se a podívat se na tehdejší trhy , které tam byly , a pokračovat dál .</t>
+    </r>
+  </si>
+  <si>
+    <t>#Neg.CM</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Normální kamarádi tuhle vnitřní bolest </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>nevidí</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> , jenom mí nejbližší ji poznají .</t>
+    </r>
+  </si>
+  <si>
+    <t>?? prož negace až za "vidět" a za čárkou
+?? špatná segmentace na věty</t>
+  </si>
+  <si>
+    <t>ADVS</t>
+  </si>
+  <si>
+    <t>dk_132.02-SCzechT-dk_132-111-root</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Tam se dalo ve skupině , aniž </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>byla</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> příliš podezřelá , </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>trávit</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> řadu týdnů .</t>
+    </r>
+  </si>
+  <si>
+    <t>lk-28105_04.01-SCzechT-lk-28105_04-d1e551-x5-root 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pk_015.06-SCzechT-pk_015-d1e1641-x2-root </t>
+  </si>
+  <si>
+    <t>T-wsj0089-001-p1s20</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Jako odborník jsem měl za úkol , abych všechno , co se mně </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>nezdálo</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> na jatka , ale k dalšímu chovu , dostával do svých stájí .</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">#Neg až za ADVS, patří k "odevzdávat", tj. asi by mělo být za "aniž"?  </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Řekla : " Půjdeme tam dopoledne na cihly a dostaneme tam oběd , </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>aniž</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> bychom </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>odevzdávaly</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> přídělové lístky . "</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Zvoníci poté začnou na znamení měnit pořadí, v němž zvony znějí, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>aniž</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> by </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>měnili</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> pravidelný rytmus úderů.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">#Neg až za ADVS, patří k "měnit",  tj. asi by mělo být za "aniž"?   </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Když je odpověď na kritiku pouze lepším vysvětlením strategií, aniž by </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>se změnily</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> důvody té kritiky, jsem přesvědčen, že pan Kageyama stále nezaútočil na základní příčinu problému a léčí jen jeho příznaky.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">#Neg až za ADVS, patří k "změnit_se",  tj. asi by mělo být za "aniž"?   </t>
+  </si>
+  <si>
+    <t>T-wsj1092-001-p1s27</t>
   </si>
 </sst>
 </file>
@@ -2441,7 +2787,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2462,12 +2808,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2592,13 +2932,13 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Check Cell" xfId="1" builtinId="23"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Kontrolní buňka" xfId="1" builtinId="23"/>
+    <cellStyle name="Normální" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2868,7 +3208,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2879,21 +3219,21 @@
   <dimension ref="A1:E91"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A63" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D64" sqref="D64"/>
+      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E78" sqref="E78"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.453125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="30.81640625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="54.81640625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="49.7265625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="23.42578125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="30.85546875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="54.85546875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="49.7109375" style="3" customWidth="1"/>
     <col min="5" max="5" width="86" style="2" customWidth="1"/>
-    <col min="6" max="16384" width="8.7265625" style="3"/>
+    <col min="6" max="16384" width="8.7109375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:5" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>15</v>
       </c>
@@ -2910,7 +3250,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="8" customFormat="1" ht="58.5" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" s="8" customFormat="1" ht="60.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
@@ -2927,7 +3267,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="8" customFormat="1" ht="116" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" s="8" customFormat="1" ht="135" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
@@ -2944,7 +3284,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="8" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>2</v>
       </c>
@@ -2959,7 +3299,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>13</v>
       </c>
@@ -2972,7 +3312,7 @@
       </c>
       <c r="E5" s="6"/>
     </row>
-    <row r="6" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>3</v>
       </c>
@@ -2987,7 +3327,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="8" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>4</v>
       </c>
@@ -3004,7 +3344,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:5" s="8" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>5</v>
       </c>
@@ -3019,7 +3359,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:5" s="8" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>6</v>
       </c>
@@ -3034,7 +3374,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:5" s="8" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>7</v>
       </c>
@@ -3051,7 +3391,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:5" s="8" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>8</v>
       </c>
@@ -3066,7 +3406,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>9</v>
       </c>
@@ -3081,7 +3421,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="13" spans="1:5" s="8" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" s="8" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>10</v>
       </c>
@@ -3096,7 +3436,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="14" spans="1:5" s="8" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>11</v>
       </c>
@@ -3113,7 +3453,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="15" spans="1:5" s="8" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>12</v>
       </c>
@@ -3128,23 +3468,23 @@
         <v>59</v>
       </c>
     </row>
-    <row r="16" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.35">
       <c r="C16" s="6"/>
       <c r="E16" s="6"/>
     </row>
-    <row r="17" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.35">
       <c r="C17" s="6"/>
       <c r="E17" s="6"/>
     </row>
-    <row r="18" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.35">
       <c r="C18" s="6"/>
       <c r="E18" s="6"/>
     </row>
-    <row r="19" spans="1:5" s="8" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:5" s="8" customFormat="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C19" s="6"/>
       <c r="E19" s="6"/>
     </row>
-    <row r="20" spans="1:5" s="8" customFormat="1" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:5" s="8" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="13" t="s">
         <v>70</v>
       </c>
@@ -3161,7 +3501,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="21" spans="1:5" s="8" customFormat="1" ht="59.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" s="8" customFormat="1" ht="59.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>62</v>
       </c>
@@ -3173,7 +3513,7 @@
       </c>
       <c r="E21" s="11"/>
     </row>
-    <row r="22" spans="1:5" s="8" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>65</v>
       </c>
@@ -3190,7 +3530,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="23" spans="1:5" s="8" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" s="8" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>65</v>
       </c>
@@ -3207,7 +3547,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="24" spans="1:5" s="8" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="16" t="s">
         <v>67</v>
       </c>
@@ -3219,7 +3559,7 @@
       </c>
       <c r="E24" s="6"/>
     </row>
-    <row r="25" spans="1:5" s="8" customFormat="1" ht="87" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" s="8" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
         <v>76</v>
       </c>
@@ -3231,7 +3571,7 @@
       </c>
       <c r="E25" s="6"/>
     </row>
-    <row r="26" spans="1:5" s="8" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" s="16" t="s">
         <v>69</v>
       </c>
@@ -3243,13 +3583,13 @@
       </c>
       <c r="E26" s="6"/>
     </row>
-    <row r="27" spans="1:5" s="8" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:5" s="8" customFormat="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27" s="6"/>
       <c r="B27" s="6"/>
       <c r="C27" s="6"/>
       <c r="E27" s="6"/>
     </row>
-    <row r="28" spans="1:5" s="8" customFormat="1" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:5" s="8" customFormat="1" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="13" t="s">
         <v>81</v>
       </c>
@@ -3266,7 +3606,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="29" spans="1:5" s="8" customFormat="1" ht="44" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" s="8" customFormat="1" ht="45.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A29" s="10" t="s">
         <v>82</v>
       </c>
@@ -3281,7 +3621,7 @@
       </c>
       <c r="E29" s="6"/>
     </row>
-    <row r="30" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="10" t="s">
         <v>84</v>
       </c>
@@ -3294,7 +3634,7 @@
       </c>
       <c r="E30" s="6"/>
     </row>
-    <row r="31" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
         <v>85</v>
       </c>
@@ -3309,11 +3649,11 @@
       </c>
       <c r="E31" s="6"/>
     </row>
-    <row r="32" spans="1:5" s="8" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:5" s="8" customFormat="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C32" s="6"/>
       <c r="E32" s="6"/>
     </row>
-    <row r="33" spans="1:5" s="8" customFormat="1" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:5" s="8" customFormat="1" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="13" t="s">
         <v>92</v>
       </c>
@@ -3330,7 +3670,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="34" spans="1:5" s="8" customFormat="1" ht="102" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:5" s="8" customFormat="1" ht="120.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A34" s="10" t="s">
         <v>97</v>
       </c>
@@ -3343,7 +3683,7 @@
       <c r="D34" s="6"/>
       <c r="E34" s="6"/>
     </row>
-    <row r="35" spans="1:5" s="8" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:5" s="8" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
         <v>90</v>
       </c>
@@ -3354,7 +3694,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="36" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B36" s="8" t="s">
         <v>91</v>
       </c>
@@ -3365,7 +3705,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="37" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C37" s="6" t="s">
         <v>96</v>
       </c>
@@ -3373,7 +3713,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="38" spans="1:5" s="8" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:5" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B38" s="8" t="s">
         <v>105</v>
       </c>
@@ -3384,7 +3724,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="39" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B39" s="8" t="s">
         <v>106</v>
       </c>
@@ -3395,7 +3735,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="40" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B40" s="8" t="s">
         <v>106</v>
       </c>
@@ -3406,7 +3746,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="41" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B41" s="8" t="s">
         <v>106</v>
       </c>
@@ -3417,7 +3757,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="42" spans="1:5" s="8" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:5" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B42" s="8" t="s">
         <v>114</v>
       </c>
@@ -3428,7 +3768,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="43" spans="1:5" s="8" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:5" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B43" s="8" t="s">
         <v>117</v>
       </c>
@@ -3439,7 +3779,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="44" spans="1:5" s="8" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:5" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B44" s="8" t="s">
         <v>117</v>
       </c>
@@ -3450,7 +3790,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="45" spans="1:5" s="8" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:5" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="B45" s="8" t="s">
         <v>106</v>
       </c>
@@ -3461,7 +3801,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="46" spans="1:5" s="8" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:5" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="B46" s="8" t="s">
         <v>106</v>
       </c>
@@ -3472,14 +3812,14 @@
         <v>123</v>
       </c>
     </row>
-    <row r="47" spans="1:5" s="8" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:5" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="8" t="s">
         <v>141</v>
       </c>
       <c r="C47" s="6"/>
       <c r="E47" s="6"/>
     </row>
-    <row r="48" spans="1:5" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A48" s="4" t="s">
         <v>131</v>
       </c>
@@ -3490,7 +3830,7 @@
       <c r="D48" s="5"/>
       <c r="E48" s="5"/>
     </row>
-    <row r="49" spans="1:5" ht="44" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:5" ht="60.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>129</v>
       </c>
@@ -3507,7 +3847,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B50" s="3" t="s">
         <v>133</v>
       </c>
@@ -3521,7 +3861,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B51" s="3" t="s">
         <v>135</v>
       </c>
@@ -3535,7 +3875,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B52" s="3" t="s">
         <v>135</v>
       </c>
@@ -3549,7 +3889,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="53" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B53" s="3" t="s">
         <v>135</v>
       </c>
@@ -3563,7 +3903,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="54" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B54" s="3" t="s">
         <v>135</v>
       </c>
@@ -3577,7 +3917,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="55" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B55" s="3" t="s">
         <v>135</v>
       </c>
@@ -3591,7 +3931,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="56" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B56" s="3" t="s">
         <v>135</v>
       </c>
@@ -3605,7 +3945,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="57" spans="1:5" ht="87" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="B57" s="3" t="s">
         <v>135</v>
       </c>
@@ -3619,7 +3959,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="58" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B58" s="3" t="s">
         <v>135</v>
       </c>
@@ -3633,7 +3973,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="59" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B59" s="3" t="s">
         <v>135</v>
       </c>
@@ -3647,7 +3987,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="60" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B60" s="3" t="s">
         <v>168</v>
       </c>
@@ -3655,13 +3995,13 @@
         <v>169</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="E60" s="1" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="61" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B61" s="3" t="s">
         <v>174</v>
       </c>
@@ -3669,13 +4009,13 @@
         <v>173</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="E61" s="21" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B62" s="3" t="s">
         <v>174</v>
       </c>
@@ -3683,13 +4023,13 @@
         <v>172</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="E62" s="22" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="63" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B63" s="3" t="s">
         <v>174</v>
       </c>
@@ -3697,341 +4037,375 @@
         <v>176</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="E63" s="2" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="64" spans="1:5" ht="203" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:5" ht="210" x14ac:dyDescent="0.25">
       <c r="B64" s="3" t="s">
         <v>177</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>196</v>
+        <v>235</v>
       </c>
       <c r="D64" s="32"/>
     </row>
-    <row r="65" spans="1:5" ht="87" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="B65" s="3" t="s">
         <v>178</v>
       </c>
       <c r="C65" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="D65" s="33"/>
-    </row>
-    <row r="66" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="D65" s="32"/>
+    </row>
+    <row r="66" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B66" s="3" t="s">
         <v>181</v>
       </c>
       <c r="C66" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="D66" s="33"/>
+      <c r="D66" s="31" t="s">
+        <v>236</v>
+      </c>
       <c r="E66" s="1" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="67" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="C67" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="D67" s="33" t="s">
+        <v>239</v>
+      </c>
+      <c r="E67" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="C68" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="D68" s="19" t="s">
+        <v>241</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="C69" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="D69" s="33" t="s">
+        <v>242</v>
+      </c>
+      <c r="E69" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="D67" s="33"/>
-      <c r="E67" s="2" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="C68" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="D68" s="33"/>
-      <c r="E68" s="1" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" ht="58" x14ac:dyDescent="0.35">
-      <c r="C69" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="D69" s="33"/>
-      <c r="E69" s="2" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="70" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="C70" s="2" t="s">
-        <v>190</v>
+        <v>245</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>191</v>
+        <v>244</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A71" s="23"/>
       <c r="B71" s="23"/>
       <c r="C71" s="28" t="s">
+        <v>190</v>
+      </c>
+      <c r="D71" s="29" t="s">
+        <v>191</v>
+      </c>
+      <c r="E71" s="28" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A72" s="23"/>
+      <c r="B72" s="23" t="s">
+        <v>249</v>
+      </c>
+      <c r="C72" s="24" t="s">
+        <v>246</v>
+      </c>
+      <c r="D72" s="19" t="s">
+        <v>247</v>
+      </c>
+      <c r="E72" s="24" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A73" s="23"/>
+      <c r="B73" s="23" t="s">
+        <v>252</v>
+      </c>
+      <c r="C73" s="24" t="s">
+        <v>251</v>
+      </c>
+      <c r="D73" s="25" t="s">
+        <v>193</v>
+      </c>
+      <c r="E73" s="24" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" s="23"/>
+      <c r="B74" s="23" t="s">
+        <v>252</v>
+      </c>
+      <c r="C74" s="24" t="s">
+        <v>194</v>
+      </c>
+      <c r="D74" s="19" t="s">
+        <v>253</v>
+      </c>
+      <c r="E74" s="24" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A75" s="23"/>
+      <c r="B75" s="23" t="s">
+        <v>252</v>
+      </c>
+      <c r="C75" s="24" t="s">
+        <v>195</v>
+      </c>
+      <c r="D75" s="19" t="s">
+        <v>255</v>
+      </c>
+      <c r="E75" s="24" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A76" s="23"/>
+      <c r="B76" s="23" t="s">
+        <v>252</v>
+      </c>
+      <c r="C76" s="24" t="s">
+        <v>259</v>
+      </c>
+      <c r="D76" s="19" t="s">
+        <v>256</v>
+      </c>
+      <c r="E76" s="24" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B77" s="23" t="s">
+        <v>252</v>
+      </c>
+      <c r="C77" s="24" t="s">
+        <v>262</v>
+      </c>
+      <c r="D77" s="19" t="s">
+        <v>257</v>
+      </c>
+      <c r="E77" s="24" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="B78" s="23" t="s">
+        <v>252</v>
+      </c>
+      <c r="C78" s="24" t="s">
+        <v>264</v>
+      </c>
+      <c r="D78" s="19" t="s">
+        <v>265</v>
+      </c>
+      <c r="E78" s="24" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B79" s="25" t="s">
+        <v>196</v>
+      </c>
+      <c r="C79" s="24" t="s">
         <v>197</v>
       </c>
-      <c r="D71" s="29" t="s">
+      <c r="D79" s="31" t="s">
         <v>198</v>
       </c>
-      <c r="E71" s="28" t="s">
+      <c r="E79" s="24" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="72" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A72" s="23"/>
-      <c r="B72" s="23"/>
-      <c r="C72" s="24" t="s">
+    <row r="80" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="B80" s="25" t="s">
+        <v>196</v>
+      </c>
+      <c r="C80" s="24" t="s">
         <v>200</v>
       </c>
-      <c r="D72" s="33"/>
-      <c r="E72" s="24" t="s">
+      <c r="D80" s="31" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A73" s="23"/>
-      <c r="B73" s="23"/>
-      <c r="C73" s="24" t="s">
+      <c r="E80" s="24" t="s">
         <v>202</v>
       </c>
-      <c r="D73" s="25" t="s">
+    </row>
+    <row r="81" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B81" s="25" t="s">
+        <v>196</v>
+      </c>
+      <c r="C81" s="24" t="s">
+        <v>200</v>
+      </c>
+      <c r="D81" s="31" t="s">
         <v>203</v>
       </c>
-      <c r="E73" s="24" t="s">
+      <c r="E81" s="26" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A74" s="23"/>
-      <c r="B74" s="23"/>
-      <c r="C74" s="24" t="s">
+    <row r="82" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B82" s="25" t="s">
+        <v>196</v>
+      </c>
+      <c r="C82" s="30" t="s">
         <v>205</v>
       </c>
-      <c r="D74" s="33"/>
-      <c r="E74" s="24" t="s">
+      <c r="D82" s="31" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="75" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A75" s="23"/>
-      <c r="B75" s="23"/>
-      <c r="C75" s="24" t="s">
+      <c r="E82" s="23" t="s">
         <v>207</v>
       </c>
-      <c r="D75" s="33"/>
-      <c r="E75" s="24" t="s">
+    </row>
+    <row r="83" spans="2:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="B83" s="25" t="s">
+        <v>196</v>
+      </c>
+      <c r="C83" s="30" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="76" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A76" s="23"/>
-      <c r="B76" s="23"/>
-      <c r="C76" s="24" t="s">
+      <c r="D83" s="25" t="s">
         <v>209</v>
       </c>
-      <c r="D76" s="33"/>
-      <c r="E76" s="24" t="s">
+      <c r="E83" s="24" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="77" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="B77" s="23"/>
-      <c r="C77" s="24" t="s">
+    <row r="84" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B84" s="25" t="s">
+        <v>196</v>
+      </c>
+      <c r="C84" s="24" t="s">
         <v>211</v>
       </c>
-      <c r="D77" s="33"/>
-      <c r="E77" s="24" t="s">
+      <c r="D84" s="25" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="78" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="B78" s="23"/>
-      <c r="C78" s="24" t="s">
+      <c r="E84" s="24" t="s">
         <v>213</v>
       </c>
-      <c r="D78" s="33"/>
-      <c r="E78" s="24" t="s">
+    </row>
+    <row r="85" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B85" s="25" t="s">
+        <v>196</v>
+      </c>
+      <c r="C85" s="30" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="79" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="B79" s="25" t="s">
+      <c r="D85" s="31" t="s">
         <v>215</v>
       </c>
-      <c r="C79" s="24" t="s">
+      <c r="E85" s="27" t="s">
         <v>216</v>
       </c>
-      <c r="D79" s="31" t="s">
+    </row>
+    <row r="86" spans="2:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="B86" s="25" t="s">
         <v>217</v>
       </c>
-      <c r="E79" s="24" t="s">
+      <c r="C86" s="24" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="80" spans="1:5" ht="58" x14ac:dyDescent="0.35">
-      <c r="B80" s="25" t="s">
-        <v>215</v>
-      </c>
-      <c r="C80" s="24" t="s">
+      <c r="D86" s="25" t="s">
         <v>219</v>
       </c>
-      <c r="D80" s="31" t="s">
+      <c r="E86" s="24" t="s">
         <v>220</v>
       </c>
-      <c r="E80" s="24" t="s">
+    </row>
+    <row r="87" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B87" s="25" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="81" spans="2:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="B81" s="25" t="s">
-        <v>215</v>
-      </c>
-      <c r="C81" s="24" t="s">
-        <v>219</v>
-      </c>
-      <c r="D81" s="31" t="s">
+      <c r="C87" s="24" t="s">
         <v>222</v>
       </c>
-      <c r="E81" s="26" t="s">
+      <c r="D87" s="31" t="s">
+        <v>187</v>
+      </c>
+      <c r="E87" s="24" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="82" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B82" s="25" t="s">
-        <v>215</v>
-      </c>
-      <c r="C82" s="30" t="s">
+    <row r="88" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B88" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="C88" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="D88" t="s">
+        <v>228</v>
+      </c>
+      <c r="E88" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="D82" s="31" t="s">
-        <v>225</v>
-      </c>
-      <c r="E82" s="23" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="83" spans="2:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="B83" s="25" t="s">
-        <v>215</v>
-      </c>
-      <c r="C83" s="30" t="s">
+    </row>
+    <row r="89" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="C89" s="2" t="s">
         <v>227</v>
       </c>
-      <c r="D83" s="25" t="s">
-        <v>228</v>
-      </c>
-      <c r="E83" s="24" t="s">
+      <c r="D89" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="E89" s="2" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="84" spans="2:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="B84" s="25" t="s">
-        <v>215</v>
-      </c>
-      <c r="C84" s="24" t="s">
+    <row r="90" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="C90" s="24" t="s">
+        <v>227</v>
+      </c>
+      <c r="D90" s="25" t="s">
+        <v>231</v>
+      </c>
+      <c r="E90" s="2" t="s">
         <v>230</v>
       </c>
-      <c r="D84" s="25" t="s">
-        <v>231</v>
-      </c>
-      <c r="E84" s="24" t="s">
+    </row>
+    <row r="91" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="C91" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="D91" s="3" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="85" spans="2:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="B85" s="25" t="s">
-        <v>215</v>
-      </c>
-      <c r="C85" s="30" t="s">
+      <c r="E91" s="2" t="s">
         <v>233</v>
-      </c>
-      <c r="D85" s="31" t="s">
-        <v>234</v>
-      </c>
-      <c r="E85" s="27" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="86" spans="2:5" ht="58" x14ac:dyDescent="0.35">
-      <c r="B86" s="25" t="s">
-        <v>236</v>
-      </c>
-      <c r="C86" s="24" t="s">
-        <v>237</v>
-      </c>
-      <c r="D86" s="25" t="s">
-        <v>238</v>
-      </c>
-      <c r="E86" s="24" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="87" spans="2:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="B87" s="25" t="s">
-        <v>240</v>
-      </c>
-      <c r="C87" s="24" t="s">
-        <v>241</v>
-      </c>
-      <c r="D87" s="31" t="s">
-        <v>193</v>
-      </c>
-      <c r="E87" s="24" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="88" spans="2:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="B88" s="3" t="s">
-        <v>244</v>
-      </c>
-      <c r="C88" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="D88" t="s">
-        <v>247</v>
-      </c>
-      <c r="E88" s="2" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="89" spans="2:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="C89" s="2" t="s">
-        <v>246</v>
-      </c>
-      <c r="D89" s="3" t="s">
-        <v>250</v>
-      </c>
-      <c r="E89" s="2" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="90" spans="2:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="C90" s="24" t="s">
-        <v>246</v>
-      </c>
-      <c r="D90" s="25" t="s">
-        <v>250</v>
-      </c>
-      <c r="E90" s="2" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="91" spans="2:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="C91" s="2" t="s">
-        <v>253</v>
-      </c>
-      <c r="D91" s="3" t="s">
-        <v>251</v>
-      </c>
-      <c r="E91" s="2" t="s">
-        <v>252</v>
       </c>
     </row>
   </sheetData>
@@ -4046,7 +4420,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
stative verbs; lemma substitutes
</commit_message>
<xml_diff>
--- a/tecto2umr/PDT-mozne-chyby.xlsx
+++ b/tecto2umr/PDT-mozne-chyby.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28635" windowHeight="12870"/>
@@ -10,12 +10,12 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="145621" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="268">
   <si>
     <t>#Gen</t>
   </si>
@@ -2706,12 +2706,18 @@
   <si>
     <t>T-wsj1092-001-p1s27</t>
   </si>
+  <si>
+    <t>ml_043.03-SCzechT-m-d1e1117-x4-457</t>
+  </si>
+  <si>
+    <t>t_lemma = ",#Comma" … nadbytečná</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2786,6 +2792,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -2807,8 +2828,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor rgb="FFA6A6A6"/>
       </patternFill>
     </fill>
   </fills>
@@ -2836,15 +2857,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -2894,60 +2915,34 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="5">
+    <cellStyle name="Excel Built-in Check Cell" xfId="4"/>
+    <cellStyle name="Excel Built-in Check Cell 1" xfId="3"/>
     <cellStyle name="Kontrolní buňka" xfId="1" builtinId="23"/>
     <cellStyle name="Normální" xfId="0" builtinId="0"/>
+    <cellStyle name="Normální 2" xfId="2"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -3208,7 +3203,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3216,1196 +3211,1204 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E91"/>
+  <dimension ref="A1:E92"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E78" sqref="E78"/>
+      <pane ySplit="1" topLeftCell="A86" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E104" sqref="E104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.42578125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="30.85546875" style="3" customWidth="1"/>
-    <col min="3" max="3" width="54.85546875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="49.7109375" style="3" customWidth="1"/>
-    <col min="5" max="5" width="86" style="2" customWidth="1"/>
-    <col min="6" max="16384" width="8.7109375" style="3"/>
+    <col min="1" max="1" width="23.42578125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="30.85546875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="54.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="49.7109375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="86" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.7109375" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="8" customFormat="1" ht="60.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+    <row r="2" spans="1:5" s="7" customFormat="1" ht="60.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="8" customFormat="1" ht="135" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+    <row r="3" spans="1:5" s="7" customFormat="1" ht="135" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+    <row r="4" spans="1:5" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="6"/>
-      <c r="C4" s="7" t="s">
+      <c r="B4" s="5"/>
+      <c r="C4" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="5" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
+    <row r="5" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="6"/>
-      <c r="C5" s="7" t="s">
+      <c r="B5" s="5"/>
+      <c r="C5" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="E5" s="6"/>
-    </row>
-    <row r="6" spans="1:5" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
+      <c r="E5" s="5"/>
+    </row>
+    <row r="6" spans="1:5" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="9" t="s">
+      <c r="B6" s="5"/>
+      <c r="C6" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E6" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
+    <row r="7" spans="1:5" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="5" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:5" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
+    <row r="8" spans="1:5" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="6"/>
-      <c r="C8" s="7" t="s">
+      <c r="B8" s="5"/>
+      <c r="C8" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D8" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="E8" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:5" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
+    <row r="9" spans="1:5" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="6"/>
-      <c r="C9" s="9" t="s">
+      <c r="B9" s="5"/>
+      <c r="C9" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D9" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="E9" s="5" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:5" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
+    <row r="10" spans="1:5" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D10" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="E10" s="6" t="s">
+      <c r="E10" s="5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:5" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
+    <row r="11" spans="1:5" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="6"/>
-      <c r="C11" s="7" t="s">
+      <c r="B11" s="5"/>
+      <c r="C11" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="D11" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="E11" s="7" t="s">
+      <c r="E11" s="6" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
+    <row r="12" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="6"/>
-      <c r="C12" s="7" t="s">
+      <c r="B12" s="5"/>
+      <c r="C12" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="D12" s="11" t="s">
+      <c r="D12" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="E12" s="6" t="s">
+      <c r="E12" s="5" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="13" spans="1:5" s="8" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
+    <row r="13" spans="1:5" s="7" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="6"/>
-      <c r="C13" s="9" t="s">
+      <c r="B13" s="5"/>
+      <c r="C13" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="D13" s="11" t="s">
+      <c r="D13" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="E13" s="12" t="s">
+      <c r="E13" s="11" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="14" spans="1:5" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
+    <row r="14" spans="1:5" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="C14" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="D14" s="11" t="s">
+      <c r="D14" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="E14" s="12" t="s">
+      <c r="E14" s="11" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="15" spans="1:5" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
+    <row r="15" spans="1:5" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="6"/>
-      <c r="C15" s="7" t="s">
+      <c r="B15" s="5"/>
+      <c r="C15" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="D15" s="11" t="s">
+      <c r="D15" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="E15" s="12" t="s">
+      <c r="E15" s="11" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="16" spans="1:5" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="C16" s="6"/>
-      <c r="E16" s="6"/>
-    </row>
-    <row r="17" spans="1:5" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="C17" s="6"/>
-      <c r="E17" s="6"/>
-    </row>
-    <row r="18" spans="1:5" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="C18" s="6"/>
-      <c r="E18" s="6"/>
-    </row>
-    <row r="19" spans="1:5" s="8" customFormat="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C19" s="6"/>
-      <c r="E19" s="6"/>
-    </row>
-    <row r="20" spans="1:5" s="8" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="13" t="s">
+    <row r="16" spans="1:5" s="7" customFormat="1" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="C16" s="5"/>
+      <c r="E16" s="5"/>
+    </row>
+    <row r="17" spans="1:5" s="7" customFormat="1" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="C17" s="5"/>
+      <c r="E17" s="5"/>
+    </row>
+    <row r="18" spans="1:5" s="7" customFormat="1" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="C18" s="5"/>
+      <c r="E18" s="5"/>
+    </row>
+    <row r="19" spans="1:5" s="7" customFormat="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C19" s="5"/>
+      <c r="E19" s="5"/>
+    </row>
+    <row r="20" spans="1:5" s="7" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="B20" s="14" t="s">
+      <c r="B20" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="C20" s="13" t="s">
+      <c r="C20" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="D20" s="14" t="s">
+      <c r="D20" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="E20" s="13" t="s">
+      <c r="E20" s="12" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="21" spans="1:5" s="8" customFormat="1" ht="59.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="6" t="s">
+    <row r="21" spans="1:5" s="7" customFormat="1" ht="59.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="B21" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C21" s="6" t="s">
+      <c r="C21" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="E21" s="11"/>
-    </row>
-    <row r="22" spans="1:5" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="6" t="s">
+      <c r="E21" s="10"/>
+    </row>
+    <row r="22" spans="1:5" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="B22" s="6" t="s">
+      <c r="B22" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="C22" s="6" t="s">
+      <c r="C22" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="D22" s="11" t="s">
+      <c r="D22" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="E22" s="11" t="s">
+      <c r="E22" s="10" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="23" spans="1:5" s="8" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A23" s="6" t="s">
+    <row r="23" spans="1:5" s="7" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="B23" s="6" t="s">
+      <c r="B23" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="C23" s="6" t="s">
+      <c r="C23" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="D23" s="8" t="s">
+      <c r="D23" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="E23" s="15" t="s">
+      <c r="E23" s="14" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="24" spans="1:5" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="16" t="s">
+    <row r="24" spans="1:5" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="B24" s="17" t="s">
+      <c r="B24" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="C24" s="17" t="s">
+      <c r="C24" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="E24" s="6"/>
-    </row>
-    <row r="25" spans="1:5" s="8" customFormat="1" ht="90" x14ac:dyDescent="0.25">
-      <c r="A25" s="6" t="s">
+      <c r="E24" s="5"/>
+    </row>
+    <row r="25" spans="1:5" s="7" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A25" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="B25" s="6" t="s">
+      <c r="B25" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="C25" s="6" t="s">
+      <c r="C25" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="E25" s="6"/>
-    </row>
-    <row r="26" spans="1:5" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A26" s="16" t="s">
+      <c r="E25" s="5"/>
+    </row>
+    <row r="26" spans="1:5" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A26" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="B26" s="17" t="s">
+      <c r="B26" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="C26" s="17" t="s">
+      <c r="C26" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="E26" s="6"/>
-    </row>
-    <row r="27" spans="1:5" s="8" customFormat="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A27" s="6"/>
-      <c r="B27" s="6"/>
-      <c r="C27" s="6"/>
-      <c r="E27" s="6"/>
-    </row>
-    <row r="28" spans="1:5" s="8" customFormat="1" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="13" t="s">
+      <c r="E26" s="5"/>
+    </row>
+    <row r="27" spans="1:5" s="7" customFormat="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A27" s="5"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="E27" s="5"/>
+    </row>
+    <row r="28" spans="1:5" s="7" customFormat="1" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="B28" s="14" t="s">
+      <c r="B28" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="C28" s="13" t="s">
+      <c r="C28" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="D28" s="14" t="s">
+      <c r="D28" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="E28" s="14" t="s">
+      <c r="E28" s="13" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="29" spans="1:5" s="8" customFormat="1" ht="45.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="10" t="s">
+    <row r="29" spans="1:5" s="7" customFormat="1" ht="45.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="B29" s="12" t="s">
+      <c r="B29" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="C29" s="6" t="s">
+      <c r="C29" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="D29" s="6" t="s">
+      <c r="D29" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="E29" s="6"/>
-    </row>
-    <row r="30" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="10" t="s">
+      <c r="E29" s="5"/>
+    </row>
+    <row r="30" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="B30" s="12"/>
-      <c r="C30" s="6" t="s">
+      <c r="B30" s="11"/>
+      <c r="C30" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="D30" s="8" t="s">
+      <c r="D30" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="E30" s="6"/>
-    </row>
-    <row r="31" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="8" t="s">
+      <c r="E30" s="5"/>
+    </row>
+    <row r="31" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="B31" s="12" t="s">
+      <c r="B31" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="C31" s="6" t="s">
+      <c r="C31" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="D31" s="11" t="s">
+      <c r="D31" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="E31" s="6"/>
-    </row>
-    <row r="32" spans="1:5" s="8" customFormat="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C32" s="6"/>
-      <c r="E32" s="6"/>
-    </row>
-    <row r="33" spans="1:5" s="8" customFormat="1" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="13" t="s">
+      <c r="E31" s="5"/>
+    </row>
+    <row r="32" spans="1:5" s="7" customFormat="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C32" s="5"/>
+      <c r="E32" s="5"/>
+    </row>
+    <row r="33" spans="1:5" s="7" customFormat="1" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="B33" s="14" t="s">
+      <c r="B33" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="C33" s="13" t="s">
+      <c r="C33" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="D33" s="14" t="s">
+      <c r="D33" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="E33" s="14" t="s">
+      <c r="E33" s="13" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="34" spans="1:5" s="8" customFormat="1" ht="120.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="10" t="s">
+    <row r="34" spans="1:5" s="7" customFormat="1" ht="120.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="B34" s="12" t="s">
+      <c r="B34" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="C34" s="18" t="s">
+      <c r="C34" s="17" t="s">
         <v>122</v>
       </c>
-      <c r="D34" s="6"/>
-      <c r="E34" s="6"/>
-    </row>
-    <row r="35" spans="1:5" s="8" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A35" s="6" t="s">
+      <c r="D34" s="5"/>
+      <c r="E34" s="5"/>
+    </row>
+    <row r="35" spans="1:5" s="7" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A35" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="C35" s="6" t="s">
+      <c r="C35" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="E35" s="6" t="s">
+      <c r="E35" s="5" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="36" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="8" t="s">
+    <row r="36" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="C36" s="6" t="s">
+      <c r="C36" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="E36" s="11" t="s">
+      <c r="E36" s="10" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="37" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C37" s="6" t="s">
+    <row r="37" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C37" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="E37" s="11" t="s">
+      <c r="E37" s="10" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="38" spans="1:5" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="B38" s="8" t="s">
+    <row r="38" spans="1:5" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="B38" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="C38" s="6" t="s">
+      <c r="C38" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="E38" s="6" t="s">
+      <c r="E38" s="5" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="39" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="8" t="s">
+    <row r="39" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B39" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="C39" s="6" t="s">
+      <c r="C39" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="E39" s="6" t="s">
+      <c r="E39" s="5" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="40" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="8" t="s">
+    <row r="40" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B40" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="C40" s="6" t="s">
+      <c r="C40" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="E40" s="6" t="s">
+      <c r="E40" s="5" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="41" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="8" t="s">
+    <row r="41" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B41" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="C41" s="6" t="s">
+      <c r="C41" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="E41" s="11" t="s">
+      <c r="E41" s="10" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="42" spans="1:5" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="B42" s="8" t="s">
+    <row r="42" spans="1:5" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="B42" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="C42" s="6" t="s">
+      <c r="C42" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="E42" s="11" t="s">
+      <c r="E42" s="10" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="43" spans="1:5" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="B43" s="8" t="s">
+    <row r="43" spans="1:5" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="B43" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="C43" s="6" t="s">
+      <c r="C43" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="E43" s="11" t="s">
+      <c r="E43" s="10" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="44" spans="1:5" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="B44" s="8" t="s">
+    <row r="44" spans="1:5" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="B44" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="C44" s="6" t="s">
+      <c r="C44" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="E44" s="11" t="s">
+      <c r="E44" s="10" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="45" spans="1:5" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="B45" s="8" t="s">
+    <row r="45" spans="1:5" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="B45" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="C45" s="6" t="s">
+      <c r="C45" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="E45" s="11" t="s">
+      <c r="E45" s="10" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="46" spans="1:5" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="B46" s="8" t="s">
+    <row r="46" spans="1:5" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="B46" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="C46" s="6" t="s">
+      <c r="C46" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="E46" s="6" t="s">
+      <c r="E46" s="5" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="47" spans="1:5" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="8" t="s">
+    <row r="47" spans="1:5" s="7" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="C47" s="6"/>
-      <c r="E47" s="6"/>
+      <c r="C47" s="5"/>
+      <c r="E47" s="5"/>
     </row>
     <row r="48" spans="1:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A48" s="4" t="s">
+      <c r="A48" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="B48" s="5" t="s">
+      <c r="B48" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C48" s="4"/>
-      <c r="D48" s="5"/>
-      <c r="E48" s="5"/>
-    </row>
-    <row r="49" spans="1:5" ht="60.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="1" t="s">
+      <c r="C48" s="3"/>
+      <c r="D48" s="4"/>
+      <c r="E48" s="4"/>
+    </row>
+    <row r="49" spans="1:5" s="7" customFormat="1" ht="60.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="B49" s="3" t="s">
+      <c r="B49" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="C49" s="2" t="s">
+      <c r="C49" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="D49" s="3" t="s">
+      <c r="D49" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="E49" s="1" t="s">
+      <c r="E49" s="11" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="B50" s="3" t="s">
+    <row r="50" spans="1:5" s="7" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="B50" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="C50" s="2" t="s">
+      <c r="C50" s="5" t="s">
         <v>134</v>
       </c>
-      <c r="D50" s="3" t="s">
+      <c r="D50" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="E50" s="1" t="s">
+      <c r="E50" s="11" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B51" s="3" t="s">
+    <row r="51" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B51" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="C51" s="2" t="s">
+      <c r="C51" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="D51" s="20" t="s">
+      <c r="D51" s="10" t="s">
         <v>164</v>
       </c>
-      <c r="E51" s="2" t="s">
+      <c r="E51" s="5" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B52" s="3" t="s">
+    <row r="52" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B52" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="C52" s="2" t="s">
+      <c r="C52" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="D52" s="19" t="s">
+      <c r="D52" s="7" t="s">
         <v>163</v>
       </c>
-      <c r="E52" s="20" t="s">
+      <c r="E52" s="10" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="53" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="B53" s="3" t="s">
+    <row r="53" spans="1:5" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="B53" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="C53" s="2" t="s">
+      <c r="C53" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="D53" s="3" t="s">
+      <c r="D53" s="7" t="s">
         <v>147</v>
       </c>
-      <c r="E53" s="1" t="s">
+      <c r="E53" s="11" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="54" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B54" s="3" t="s">
+    <row r="54" spans="1:5" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="B54" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="C54" s="2" t="s">
+      <c r="C54" s="5" t="s">
         <v>144</v>
       </c>
-      <c r="D54" s="3" t="s">
+      <c r="D54" s="7" t="s">
         <v>145</v>
       </c>
-      <c r="E54" s="1" t="s">
+      <c r="E54" s="11" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="55" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="B55" s="3" t="s">
+    <row r="55" spans="1:5" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="B55" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="C55" s="2" t="s">
+      <c r="C55" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="D55" s="20" t="s">
+      <c r="D55" s="10" t="s">
         <v>165</v>
       </c>
-      <c r="E55" s="2" t="s">
+      <c r="E55" s="5" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="56" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B56" s="3" t="s">
+    <row r="56" spans="1:5" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="B56" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="C56" s="2" t="s">
+      <c r="C56" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="D56" s="20" t="s">
+      <c r="D56" s="10" t="s">
         <v>166</v>
       </c>
-      <c r="E56" s="2" t="s">
+      <c r="E56" s="5" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="57" spans="1:5" ht="90" x14ac:dyDescent="0.25">
-      <c r="B57" s="3" t="s">
+    <row r="57" spans="1:5" s="7" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="B57" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="C57" s="2" t="s">
+      <c r="C57" s="5" t="s">
         <v>161</v>
       </c>
-      <c r="D57" s="3" t="s">
+      <c r="D57" s="7" t="s">
         <v>159</v>
       </c>
-      <c r="E57" s="2" t="s">
+      <c r="E57" s="5" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="58" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B58" s="3" t="s">
+    <row r="58" spans="1:5" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="B58" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="C58" s="2" t="s">
+      <c r="C58" s="5" t="s">
         <v>162</v>
       </c>
-      <c r="D58" s="3" t="s">
+      <c r="D58" s="7" t="s">
         <v>160</v>
       </c>
-      <c r="E58" s="20" t="s">
+      <c r="E58" s="10" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="59" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B59" s="3" t="s">
+    <row r="59" spans="1:5" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="B59" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="C59" s="2" t="s">
+      <c r="C59" s="5" t="s">
         <v>156</v>
       </c>
-      <c r="D59" s="20" t="s">
+      <c r="D59" s="10" t="s">
         <v>157</v>
       </c>
-      <c r="E59" s="2" t="s">
+      <c r="E59" s="5" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="60" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B60" s="3" t="s">
+    <row r="60" spans="1:5" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="B60" s="7" t="s">
         <v>168</v>
       </c>
-      <c r="C60" s="2" t="s">
+      <c r="C60" s="5" t="s">
         <v>169</v>
       </c>
-      <c r="D60" s="3" t="s">
+      <c r="D60" s="7" t="s">
         <v>186</v>
       </c>
-      <c r="E60" s="1" t="s">
+      <c r="E60" s="11" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="61" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="B61" s="3" t="s">
+    <row r="61" spans="1:5" s="7" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="B61" s="7" t="s">
         <v>174</v>
       </c>
-      <c r="C61" s="2" t="s">
+      <c r="C61" s="5" t="s">
         <v>173</v>
       </c>
-      <c r="D61" s="2" t="s">
+      <c r="D61" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="E61" s="21" t="s">
+      <c r="E61" s="18" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="62" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B62" s="3" t="s">
+    <row r="62" spans="1:5" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="B62" s="7" t="s">
         <v>174</v>
       </c>
-      <c r="C62" s="2" t="s">
+      <c r="C62" s="5" t="s">
         <v>172</v>
       </c>
-      <c r="D62" s="3" t="s">
+      <c r="D62" s="7" t="s">
         <v>188</v>
       </c>
-      <c r="E62" s="22" t="s">
+      <c r="E62" s="14" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="63" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B63" s="3" t="s">
+    <row r="63" spans="1:5" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="B63" s="7" t="s">
         <v>174</v>
       </c>
-      <c r="C63" s="2" t="s">
+      <c r="C63" s="5" t="s">
         <v>176</v>
       </c>
-      <c r="D63" s="3" t="s">
+      <c r="D63" s="7" t="s">
         <v>189</v>
       </c>
-      <c r="E63" s="2" t="s">
+      <c r="E63" s="5" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="64" spans="1:5" ht="210" x14ac:dyDescent="0.25">
-      <c r="B64" s="3" t="s">
+    <row r="64" spans="1:5" s="7" customFormat="1" ht="210" x14ac:dyDescent="0.25">
+      <c r="B64" s="7" t="s">
         <v>177</v>
       </c>
-      <c r="C64" s="2" t="s">
+      <c r="C64" s="5" t="s">
         <v>235</v>
       </c>
-      <c r="D64" s="32"/>
-    </row>
-    <row r="65" spans="1:5" ht="90" x14ac:dyDescent="0.25">
-      <c r="B65" s="3" t="s">
+      <c r="E64" s="5"/>
+    </row>
+    <row r="65" spans="1:5" s="7" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="B65" s="7" t="s">
         <v>178</v>
       </c>
-      <c r="C65" s="2" t="s">
+      <c r="C65" s="5" t="s">
         <v>179</v>
       </c>
-      <c r="D65" s="32"/>
-    </row>
-    <row r="66" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B66" s="3" t="s">
+      <c r="E65" s="5"/>
+    </row>
+    <row r="66" spans="1:5" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="B66" s="7" t="s">
         <v>181</v>
       </c>
-      <c r="C66" s="2" t="s">
+      <c r="C66" s="5" t="s">
         <v>182</v>
       </c>
-      <c r="D66" s="31" t="s">
+      <c r="D66" s="10" t="s">
         <v>236</v>
       </c>
-      <c r="E66" s="1" t="s">
+      <c r="E66" s="11" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="67" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="C67" s="2" t="s">
+    <row r="67" spans="1:5" s="7" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+      <c r="C67" s="5" t="s">
         <v>238</v>
       </c>
-      <c r="D67" s="33" t="s">
+      <c r="D67" s="5" t="s">
         <v>239</v>
       </c>
-      <c r="E67" s="2" t="s">
+      <c r="E67" s="5" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="68" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="C68" s="2" t="s">
+    <row r="68" spans="1:5" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="C68" s="5" t="s">
         <v>240</v>
       </c>
-      <c r="D68" s="19" t="s">
+      <c r="D68" s="7" t="s">
         <v>241</v>
       </c>
-      <c r="E68" s="1" t="s">
+      <c r="E68" s="11" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="69" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="C69" s="2" t="s">
+    <row r="69" spans="1:5" s="7" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="C69" s="5" t="s">
         <v>185</v>
       </c>
-      <c r="D69" s="33" t="s">
+      <c r="D69" s="5" t="s">
         <v>242</v>
       </c>
-      <c r="E69" s="2" t="s">
+      <c r="E69" s="5" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="70" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="C70" s="2" t="s">
+    <row r="70" spans="1:5" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="C70" s="5" t="s">
         <v>245</v>
       </c>
-      <c r="D70" s="3" t="s">
+      <c r="D70" s="7" t="s">
         <v>244</v>
       </c>
-      <c r="E70" s="2" t="s">
+      <c r="E70" s="5" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="71" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A71" s="23"/>
-      <c r="B71" s="23"/>
-      <c r="C71" s="28" t="s">
+    <row r="71" spans="1:5" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A71" s="9"/>
+      <c r="B71" s="9"/>
+      <c r="C71" s="19" t="s">
         <v>190</v>
       </c>
-      <c r="D71" s="29" t="s">
+      <c r="D71" s="20" t="s">
         <v>191</v>
       </c>
-      <c r="E71" s="28" t="s">
+      <c r="E71" s="19" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="72" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A72" s="23"/>
-      <c r="B72" s="23" t="s">
+    <row r="72" spans="1:5" s="7" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A72" s="9"/>
+      <c r="B72" s="9" t="s">
         <v>249</v>
       </c>
-      <c r="C72" s="24" t="s">
+      <c r="C72" s="5" t="s">
         <v>246</v>
       </c>
-      <c r="D72" s="19" t="s">
+      <c r="D72" s="7" t="s">
         <v>247</v>
       </c>
-      <c r="E72" s="24" t="s">
+      <c r="E72" s="5" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="73" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A73" s="23"/>
-      <c r="B73" s="23" t="s">
+    <row r="73" spans="1:5" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A73" s="9"/>
+      <c r="B73" s="9" t="s">
         <v>252</v>
       </c>
-      <c r="C73" s="24" t="s">
+      <c r="C73" s="5" t="s">
         <v>251</v>
       </c>
-      <c r="D73" s="25" t="s">
+      <c r="D73" s="7" t="s">
         <v>193</v>
       </c>
-      <c r="E73" s="24" t="s">
+      <c r="E73" s="5" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A74" s="23"/>
-      <c r="B74" s="23" t="s">
+    <row r="74" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="9"/>
+      <c r="B74" s="9" t="s">
         <v>252</v>
       </c>
-      <c r="C74" s="24" t="s">
+      <c r="C74" s="5" t="s">
         <v>194</v>
       </c>
-      <c r="D74" s="19" t="s">
+      <c r="D74" s="7" t="s">
         <v>253</v>
       </c>
-      <c r="E74" s="24" t="s">
+      <c r="E74" s="5" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="75" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A75" s="23"/>
-      <c r="B75" s="23" t="s">
+    <row r="75" spans="1:5" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A75" s="9"/>
+      <c r="B75" s="9" t="s">
         <v>252</v>
       </c>
-      <c r="C75" s="24" t="s">
+      <c r="C75" s="5" t="s">
         <v>195</v>
       </c>
-      <c r="D75" s="19" t="s">
+      <c r="D75" s="7" t="s">
         <v>255</v>
       </c>
-      <c r="E75" s="24" t="s">
+      <c r="E75" s="5" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="76" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A76" s="23"/>
-      <c r="B76" s="23" t="s">
+    <row r="76" spans="1:5" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A76" s="9"/>
+      <c r="B76" s="9" t="s">
         <v>252</v>
       </c>
-      <c r="C76" s="24" t="s">
+      <c r="C76" s="5" t="s">
         <v>259</v>
       </c>
-      <c r="D76" s="19" t="s">
+      <c r="D76" s="7" t="s">
         <v>256</v>
       </c>
-      <c r="E76" s="24" t="s">
+      <c r="E76" s="5" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="77" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B77" s="23" t="s">
+    <row r="77" spans="1:5" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="B77" s="9" t="s">
         <v>252</v>
       </c>
-      <c r="C77" s="24" t="s">
+      <c r="C77" s="5" t="s">
         <v>262</v>
       </c>
-      <c r="D77" s="19" t="s">
+      <c r="D77" s="7" t="s">
         <v>257</v>
       </c>
-      <c r="E77" s="24" t="s">
+      <c r="E77" s="5" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="78" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="B78" s="23" t="s">
+    <row r="78" spans="1:5" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="B78" s="9" t="s">
         <v>252</v>
       </c>
-      <c r="C78" s="24" t="s">
+      <c r="C78" s="5" t="s">
         <v>264</v>
       </c>
-      <c r="D78" s="19" t="s">
+      <c r="D78" s="7" t="s">
         <v>265</v>
       </c>
-      <c r="E78" s="24" t="s">
+      <c r="E78" s="5" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="79" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B79" s="25" t="s">
+    <row r="79" spans="1:5" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="B79" s="7" t="s">
         <v>196</v>
       </c>
-      <c r="C79" s="24" t="s">
+      <c r="C79" s="5" t="s">
         <v>197</v>
       </c>
-      <c r="D79" s="31" t="s">
+      <c r="D79" s="10" t="s">
         <v>198</v>
       </c>
-      <c r="E79" s="24" t="s">
+      <c r="E79" s="5" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="80" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="B80" s="25" t="s">
+    <row r="80" spans="1:5" s="7" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="B80" s="7" t="s">
         <v>196</v>
       </c>
-      <c r="C80" s="24" t="s">
+      <c r="C80" s="5" t="s">
         <v>200</v>
       </c>
-      <c r="D80" s="31" t="s">
+      <c r="D80" s="10" t="s">
         <v>201</v>
       </c>
-      <c r="E80" s="24" t="s">
+      <c r="E80" s="5" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="81" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B81" s="25" t="s">
+    <row r="81" spans="2:5" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="B81" s="7" t="s">
         <v>196</v>
       </c>
-      <c r="C81" s="24" t="s">
+      <c r="C81" s="5" t="s">
         <v>200</v>
       </c>
-      <c r="D81" s="31" t="s">
+      <c r="D81" s="10" t="s">
         <v>203</v>
       </c>
-      <c r="E81" s="26" t="s">
+      <c r="E81" s="21" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="82" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B82" s="25" t="s">
+    <row r="82" spans="2:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B82" s="7" t="s">
         <v>196</v>
       </c>
-      <c r="C82" s="30" t="s">
+      <c r="C82" s="8" t="s">
         <v>205</v>
       </c>
-      <c r="D82" s="31" t="s">
+      <c r="D82" s="10" t="s">
         <v>206</v>
       </c>
-      <c r="E82" s="23" t="s">
+      <c r="E82" s="9" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="83" spans="2:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="B83" s="25" t="s">
+    <row r="83" spans="2:5" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="B83" s="7" t="s">
         <v>196</v>
       </c>
-      <c r="C83" s="30" t="s">
+      <c r="C83" s="8" t="s">
         <v>208</v>
       </c>
-      <c r="D83" s="25" t="s">
+      <c r="D83" s="7" t="s">
         <v>209</v>
       </c>
-      <c r="E83" s="24" t="s">
+      <c r="E83" s="5" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="84" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B84" s="25" t="s">
+    <row r="84" spans="2:5" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="B84" s="7" t="s">
         <v>196</v>
       </c>
-      <c r="C84" s="24" t="s">
+      <c r="C84" s="5" t="s">
         <v>211</v>
       </c>
-      <c r="D84" s="25" t="s">
+      <c r="D84" s="7" t="s">
         <v>212</v>
       </c>
-      <c r="E84" s="24" t="s">
+      <c r="E84" s="5" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="85" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B85" s="25" t="s">
+    <row r="85" spans="2:5" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="B85" s="7" t="s">
         <v>196</v>
       </c>
-      <c r="C85" s="30" t="s">
+      <c r="C85" s="8" t="s">
         <v>214</v>
       </c>
-      <c r="D85" s="31" t="s">
+      <c r="D85" s="10" t="s">
         <v>215</v>
       </c>
-      <c r="E85" s="27" t="s">
+      <c r="E85" s="22" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="86" spans="2:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="B86" s="25" t="s">
+    <row r="86" spans="2:5" s="7" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="B86" s="7" t="s">
         <v>217</v>
       </c>
-      <c r="C86" s="24" t="s">
+      <c r="C86" s="5" t="s">
         <v>218</v>
       </c>
-      <c r="D86" s="25" t="s">
+      <c r="D86" s="7" t="s">
         <v>219</v>
       </c>
-      <c r="E86" s="24" t="s">
+      <c r="E86" s="5" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="87" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B87" s="25" t="s">
+    <row r="87" spans="2:5" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="B87" s="7" t="s">
         <v>221</v>
       </c>
-      <c r="C87" s="24" t="s">
+      <c r="C87" s="5" t="s">
         <v>222</v>
       </c>
-      <c r="D87" s="31" t="s">
+      <c r="D87" s="10" t="s">
         <v>187</v>
       </c>
-      <c r="E87" s="24" t="s">
+      <c r="E87" s="5" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="88" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B88" s="3" t="s">
+    <row r="88" spans="2:5" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="B88" s="7" t="s">
         <v>225</v>
       </c>
-      <c r="C88" s="2" t="s">
+      <c r="C88" s="5" t="s">
         <v>226</v>
       </c>
-      <c r="D88" t="s">
+      <c r="D88" s="9" t="s">
         <v>228</v>
       </c>
-      <c r="E88" s="2" t="s">
+      <c r="E88" s="5" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="89" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="C89" s="2" t="s">
+    <row r="89" spans="2:5" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="C89" s="5" t="s">
         <v>227</v>
       </c>
-      <c r="D89" s="3" t="s">
+      <c r="D89" s="7" t="s">
         <v>231</v>
       </c>
-      <c r="E89" s="2" t="s">
+      <c r="E89" s="5" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="90" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="C90" s="24" t="s">
+    <row r="90" spans="2:5" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="C90" s="5" t="s">
         <v>227</v>
       </c>
-      <c r="D90" s="25" t="s">
+      <c r="D90" s="7" t="s">
         <v>231</v>
       </c>
-      <c r="E90" s="2" t="s">
+      <c r="E90" s="5" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="91" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="C91" s="2" t="s">
+    <row r="91" spans="2:5" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="C91" s="5" t="s">
         <v>234</v>
       </c>
-      <c r="D91" s="3" t="s">
+      <c r="D91" s="7" t="s">
         <v>232</v>
       </c>
-      <c r="E91" s="2" t="s">
+      <c r="E91" s="5" t="s">
         <v>233</v>
+      </c>
+    </row>
+    <row r="92" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C92" s="24" t="s">
+        <v>267</v>
+      </c>
+      <c r="D92" s="23" t="s">
+        <v>266</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
aspect (state verbs, part)
</commit_message>
<xml_diff>
--- a/tecto2umr/PDT-mozne-chyby.xlsx
+++ b/tecto2umr/PDT-mozne-chyby.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lopatkova\SVN\GitHub-UMR\tecto2umr\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28635" windowHeight="12870"/>
   </bookViews>
@@ -15,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="272">
   <si>
     <t>#Gen</t>
   </si>
@@ -2540,9 +2545,6 @@
     </r>
   </si>
   <si>
-    <t>lk-28105_04.01-SCzechT-lk-28105_04-d1e551-x5-root 2</t>
-  </si>
-  <si>
     <t xml:space="preserve">pk_015.06-SCzechT-pk_015-d1e1641-x2-root </t>
   </si>
   <si>
@@ -2711,6 +2713,64 @@
   </si>
   <si>
     <t>t_lemma = ",#Comma" … nadbytečná</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Ve druhém tahu 18. týdne Sportky v I. pořadí je 1 výhra 1998352 Kč, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ve II. není žádná výhra,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ve III. je 73 výher po 9759 Kč, ve IV. je 4630 výher po 307 Kč, v V. je 80873 výher po 37 Kč.</t>
+    </r>
+  </si>
+  <si>
+    <t>#Neg.RHEM patří pod "být" (2. klauze)</t>
+  </si>
+  <si>
+    <t>#Neg.RHEM patří pod "mít" nebo k "výlučně"</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Nebudeme mít žáky výlučně z velmi bohatých rodin</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, upozorňuje ředitel Ward.</t>
+    </r>
+  </si>
+  <si>
+    <t>lk-28105_04.01-SCzechT-lk-28105_04-d1e551-x5-root</t>
   </si>
 </sst>
 </file>
@@ -2864,7 +2924,7 @@
     <xf numFmtId="0" fontId="11" fillId="4" borderId="1" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="1" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -2930,12 +2990,15 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
+    <cellStyle name="Check Cell" xfId="1" builtinId="23"/>
     <cellStyle name="Excel Built-in Check Cell" xfId="4"/>
     <cellStyle name="Excel Built-in Check Cell 1" xfId="3"/>
-    <cellStyle name="Kontrolní buňka" xfId="1" builtinId="23"/>
-    <cellStyle name="Normální" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normální 2" xfId="2"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2943,6 +3006,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -3203,7 +3269,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3211,11 +3277,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E92"/>
+  <dimension ref="A1:E94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A86" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E104" sqref="E104"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A69" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C78" sqref="C78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4132,7 +4198,7 @@
       <c r="B72" s="9" t="s">
         <v>249</v>
       </c>
-      <c r="C72" s="5" t="s">
+      <c r="C72" s="8" t="s">
         <v>246</v>
       </c>
       <c r="D72" s="7" t="s">
@@ -4147,7 +4213,7 @@
       <c r="B73" s="9" t="s">
         <v>252</v>
       </c>
-      <c r="C73" s="5" t="s">
+      <c r="C73" s="8" t="s">
         <v>251</v>
       </c>
       <c r="D73" s="7" t="s">
@@ -4162,7 +4228,7 @@
       <c r="B74" s="9" t="s">
         <v>252</v>
       </c>
-      <c r="C74" s="5" t="s">
+      <c r="C74" s="8" t="s">
         <v>194</v>
       </c>
       <c r="D74" s="7" t="s">
@@ -4177,14 +4243,14 @@
       <c r="B75" s="9" t="s">
         <v>252</v>
       </c>
-      <c r="C75" s="5" t="s">
+      <c r="C75" s="8" t="s">
         <v>195</v>
       </c>
       <c r="D75" s="7" t="s">
-        <v>255</v>
+        <v>271</v>
       </c>
       <c r="E75" s="5" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="76" spans="1:5" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -4192,42 +4258,42 @@
       <c r="B76" s="9" t="s">
         <v>252</v>
       </c>
-      <c r="C76" s="5" t="s">
+      <c r="C76" s="8" t="s">
+        <v>258</v>
+      </c>
+      <c r="D76" s="7" t="s">
+        <v>255</v>
+      </c>
+      <c r="E76" s="5" t="s">
         <v>259</v>
-      </c>
-      <c r="D76" s="7" t="s">
-        <v>256</v>
-      </c>
-      <c r="E76" s="5" t="s">
-        <v>260</v>
       </c>
     </row>
     <row r="77" spans="1:5" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B77" s="9" t="s">
         <v>252</v>
       </c>
-      <c r="C77" s="5" t="s">
-        <v>262</v>
+      <c r="C77" s="8" t="s">
+        <v>261</v>
       </c>
       <c r="D77" s="7" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E77" s="5" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="78" spans="1:5" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="B78" s="9" t="s">
         <v>252</v>
       </c>
-      <c r="C78" s="5" t="s">
+      <c r="C78" s="8" t="s">
+        <v>263</v>
+      </c>
+      <c r="D78" s="7" t="s">
         <v>264</v>
       </c>
-      <c r="D78" s="7" t="s">
-        <v>265</v>
-      </c>
       <c r="E78" s="5" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="79" spans="1:5" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -4405,10 +4471,32 @@
     </row>
     <row r="92" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C92" s="24" t="s">
+        <v>266</v>
+      </c>
+      <c r="D92" s="23" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="93" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="C93" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="D93" s="25" t="s">
+        <v>187</v>
+      </c>
+      <c r="E93" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="D92" s="23" t="s">
-        <v>266</v>
+    </row>
+    <row r="94" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C94" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="D94" t="s">
+        <v>188</v>
+      </c>
+      <c r="E94" s="1" t="s">
+        <v>270</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
negace - chyby (update)
</commit_message>
<xml_diff>
--- a/tecto2umr/PDT-mozne-chyby.xlsx
+++ b/tecto2umr/PDT-mozne-chyby.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lopatkova\SVN\GitHub-UMR\tecto2umr\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28635" windowHeight="12870"/>
   </bookViews>
@@ -1875,12 +1870,6 @@
     <t xml:space="preserve">faust_2010_07_jh_05-SCzechT-p0436-s1A-root </t>
   </si>
   <si>
-    <t>?? jak se pozná, k čemu patří #Neg (k být, nikoli k trávit)</t>
-  </si>
-  <si>
-    <t>?? jak se pozná, k čemu patří #Neg (k prvnímu nezdálo)</t>
-  </si>
-  <si>
     <t>GRAD</t>
   </si>
   <si>
@@ -2408,18 +2397,97 @@
 nebo kde je zachycena info o negaci ??? (v Manuálu jsem nenašla)</t>
   </si>
   <si>
-    <t xml:space="preserve">??? nerozumím moc anotaci - jak se pozná, k čemu patří #Neg.CM (prohlídka nebyla účelem) a k čemu pouze.CM (pouze bylo účelem) ...
-spíš bych doplnila na něco jako: "nebyla" účelem prohlídka, pouze [bylo účelem] zastavit se a ... </t>
-  </si>
-  <si>
     <t>lk_123.06-SCzechT-lk_123-285-root</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
+    <t>#Neg.CM</t>
+  </si>
+  <si>
+    <t>ADVS</t>
+  </si>
+  <si>
+    <t>dk_132.02-SCzechT-dk_132-111-root</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pk_015.06-SCzechT-pk_015-d1e1641-x2-root </t>
+  </si>
+  <si>
+    <t>T-wsj0089-001-p1s20</t>
+  </si>
+  <si>
+    <t>T-wsj1092-001-p1s27</t>
+  </si>
+  <si>
+    <t>ml_043.03-SCzechT-m-d1e1117-x4-457</t>
+  </si>
+  <si>
+    <t>t_lemma = ",#Comma" … nadbytečná</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Ve druhém tahu 18. týdne Sportky v I. pořadí je 1 výhra 1998352 Kč, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ve II. není žádná výhra,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ve III. je 73 výher po 9759 Kč, ve IV. je 4630 výher po 307 Kč, v V. je 80873 výher po 37 Kč.</t>
+    </r>
+  </si>
+  <si>
+    <t>#Neg.RHEM patří pod "být" (2. klauze)</t>
+  </si>
+  <si>
+    <t>#Neg.RHEM patří pod "mít" nebo k "výlučně"</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Nebudeme mít žáky výlučně z velmi bohatých rodin</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, upozorňuje ředitel Ward.</t>
+    </r>
+  </si>
+  <si>
+    <t>lk-28105_04.01-SCzechT-lk-28105_04-d1e551-x5-root</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <strike/>
+        <sz val="11"/>
+        <color theme="0" tint="-0.499984740745262"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -2428,8 +2496,9 @@
     </r>
     <r>
       <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
+        <strike/>
+        <sz val="11"/>
+        <color theme="0" tint="-0.499984740745262"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -2439,8 +2508,9 @@
     <r>
       <rPr>
         <b/>
-        <sz val="11"/>
-        <color theme="1"/>
+        <strike/>
+        <sz val="11"/>
+        <color theme="0" tint="-0.499984740745262"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -2449,8 +2519,9 @@
     </r>
     <r>
       <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
+        <strike/>
+        <sz val="11"/>
+        <color theme="0" tint="-0.499984740745262"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -2459,17 +2530,15 @@
     </r>
   </si>
   <si>
-    <t>#Neg.CM</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">Normální kamarádi tuhle vnitřní bolest </t>
     </r>
     <r>
       <rPr>
         <b/>
-        <sz val="11"/>
-        <color theme="1"/>
+        <strike/>
+        <sz val="11"/>
+        <color theme="0" tint="-0.499984740745262"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -2478,8 +2547,9 @@
     </r>
     <r>
       <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
+        <strike/>
+        <sz val="11"/>
+        <color theme="0" tint="-0.499984740745262"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -2488,24 +2558,15 @@
     </r>
   </si>
   <si>
-    <t>?? prož negace až za "vidět" a za čárkou
-?? špatná segmentace na věty</t>
-  </si>
-  <si>
-    <t>ADVS</t>
-  </si>
-  <si>
-    <t>dk_132.02-SCzechT-dk_132-111-root</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">Tam se dalo ve skupině , aniž </t>
     </r>
     <r>
       <rPr>
         <b/>
-        <sz val="11"/>
-        <color theme="1"/>
+        <strike/>
+        <sz val="11"/>
+        <color theme="0" tint="-0.499984740745262"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -2514,8 +2575,9 @@
     </r>
     <r>
       <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
+        <strike/>
+        <sz val="11"/>
+        <color theme="0" tint="-0.499984740745262"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -2525,8 +2587,9 @@
     <r>
       <rPr>
         <b/>
-        <sz val="11"/>
-        <color theme="1"/>
+        <strike/>
+        <sz val="11"/>
+        <color theme="0" tint="-0.499984740745262"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -2535,8 +2598,9 @@
     </r>
     <r>
       <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
+        <strike/>
+        <sz val="11"/>
+        <color theme="0" tint="-0.499984740745262"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -2545,20 +2609,15 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">pk_015.06-SCzechT-pk_015-d1e1641-x2-root </t>
-  </si>
-  <si>
-    <t>T-wsj0089-001-p1s20</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">Jako odborník jsem měl za úkol , abych všechno , co se mně </t>
     </r>
     <r>
       <rPr>
         <b/>
-        <sz val="11"/>
-        <color theme="1"/>
+        <strike/>
+        <sz val="11"/>
+        <color theme="0" tint="-0.499984740745262"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -2567,8 +2626,9 @@
     </r>
     <r>
       <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
+        <strike/>
+        <sz val="11"/>
+        <color theme="0" tint="-0.499984740745262"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -2577,7 +2637,35 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">#Neg až za ADVS, patří k "odevzdávat", tj. asi by mělo být za "aniž"?  </t>
+    <r>
+      <t xml:space="preserve">?? prož negace až za "vidět" a za čárkou
+?? špatná segmentace na věty
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>#Neg.CM --&gt; #Neg.RHEM a převěšeno pod sloveso</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">?? jak se pozná, k čemu patří #Neg (k prvnímu nezdálo)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>#Neg.CM --&gt; #Neg.RHEM a převěšeno pod sloveso</t>
+    </r>
   </si>
   <si>
     <r>
@@ -2586,8 +2674,9 @@
     <r>
       <rPr>
         <b/>
-        <sz val="11"/>
-        <color theme="1"/>
+        <strike/>
+        <sz val="11"/>
+        <color theme="0" tint="-0.499984740745262"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -2596,8 +2685,9 @@
     </r>
     <r>
       <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
+        <strike/>
+        <sz val="11"/>
+        <color theme="0" tint="-0.499984740745262"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -2607,8 +2697,9 @@
     <r>
       <rPr>
         <b/>
-        <sz val="11"/>
-        <color theme="1"/>
+        <strike/>
+        <sz val="11"/>
+        <color theme="0" tint="-0.499984740745262"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -2617,8 +2708,9 @@
     </r>
     <r>
       <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
+        <strike/>
+        <sz val="11"/>
+        <color theme="0" tint="-0.499984740745262"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -2633,8 +2725,9 @@
     <r>
       <rPr>
         <b/>
-        <sz val="11"/>
-        <color theme="1"/>
+        <strike/>
+        <sz val="11"/>
+        <color theme="0" tint="-0.499984740745262"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -2643,8 +2736,9 @@
     </r>
     <r>
       <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
+        <strike/>
+        <sz val="11"/>
+        <color theme="0" tint="-0.499984740745262"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -2654,8 +2748,9 @@
     <r>
       <rPr>
         <b/>
-        <sz val="11"/>
-        <color theme="1"/>
+        <strike/>
+        <sz val="11"/>
+        <color theme="0" tint="-0.499984740745262"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -2664,8 +2759,9 @@
     </r>
     <r>
       <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
+        <strike/>
+        <sz val="11"/>
+        <color theme="0" tint="-0.499984740745262"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -2674,17 +2770,15 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">#Neg až za ADVS, patří k "měnit",  tj. asi by mělo být za "aniž"?   </t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">Když je odpověď na kritiku pouze lepším vysvětlením strategií, aniž by </t>
     </r>
     <r>
       <rPr>
         <b/>
-        <sz val="11"/>
-        <color theme="1"/>
+        <strike/>
+        <sz val="11"/>
+        <color theme="0" tint="-0.499984740745262"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -2693,8 +2787,9 @@
     </r>
     <r>
       <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
+        <strike/>
+        <sz val="11"/>
+        <color theme="0" tint="-0.499984740745262"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -2703,81 +2798,97 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">#Neg až za ADVS, patří k "změnit_se",  tj. asi by mělo být za "aniž"?   </t>
-  </si>
-  <si>
-    <t>T-wsj1092-001-p1s27</t>
-  </si>
-  <si>
-    <t>ml_043.03-SCzechT-m-d1e1117-x4-457</t>
-  </si>
-  <si>
-    <t>t_lemma = ",#Comma" … nadbytečná</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Ve druhém tahu 18. týdne Sportky v I. pořadí je 1 výhra 1998352 Kč, </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>ve II. není žádná výhra,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> ve III. je 73 výher po 9759 Kč, ve IV. je 4630 výher po 307 Kč, v V. je 80873 výher po 37 Kč.</t>
-    </r>
-  </si>
-  <si>
-    <t>#Neg.RHEM patří pod "být" (2. klauze)</t>
-  </si>
-  <si>
-    <t>#Neg.RHEM patří pod "mít" nebo k "výlučně"</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Nebudeme mít žáky výlučně z velmi bohatých rodin</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>, upozorňuje ředitel Ward.</t>
-    </r>
-  </si>
-  <si>
-    <t>lk-28105_04.01-SCzechT-lk-28105_04-d1e551-x5-root</t>
+    <r>
+      <t xml:space="preserve">??? nerozumím moc anotaci - jak se pozná, k čemu patří #Neg.CM (prohlídka nebyla účelem) a k čemu pouze.CM (pouze bylo účelem) ...
+spíš bych doplnila na něco jako: "nebyla" účelem prohlídka, pouze [bylo účelem] zastavit se a ... 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>upravena pozice #Neg (JŠ)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>?? jak se pozná, k čemu patří #Neg (k být, nikoli k trávit)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>upravena pozice #Neg (JŠ)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">#Neg až za ADVS, patří k "odevzdávat", tj. asi by mělo být za "aniž"?  
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>upravena pozice #Neg (JŠ)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">#Neg až za ADVS, patří k "měnit",  tj. asi by mělo být za "aniž"?   
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>upravena pozice #Neg (JŠ)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">#Neg až za ADVS, patří k "změnit_se",  tj. asi by mělo být za "aniž"?   
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>upravena pozice #Neg (JŠ)</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2867,6 +2978,15 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <b/>
+      <strike/>
+      <sz val="11"/>
+      <color theme="0" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -2924,7 +3044,7 @@
     <xf numFmtId="0" fontId="11" fillId="4" borderId="1" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="1" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -2993,12 +3113,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
-    <cellStyle name="Check Cell" xfId="1" builtinId="23"/>
     <cellStyle name="Excel Built-in Check Cell" xfId="4"/>
     <cellStyle name="Excel Built-in Check Cell 1" xfId="3"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Kontrolní buňka" xfId="1" builtinId="23"/>
+    <cellStyle name="Normální" xfId="0" builtinId="0"/>
     <cellStyle name="Normální 2" xfId="2"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -3269,7 +3393,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3279,9 +3403,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E94"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A69" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C78" sqref="C78"/>
+      <selection pane="bottomLeft" activeCell="E73" sqref="E73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4109,7 +4233,7 @@
         <v>177</v>
       </c>
       <c r="C64" s="5" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="E64" s="5"/>
     </row>
@@ -4130,7 +4254,7 @@
         <v>182</v>
       </c>
       <c r="D66" s="10" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="E66" s="11" t="s">
         <v>180</v>
@@ -4138,21 +4262,21 @@
     </row>
     <row r="67" spans="1:5" s="7" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="C67" s="5" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D67" s="5" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="E67" s="5" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="68" spans="1:5" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="C68" s="5" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D68" s="7" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="E68" s="11" t="s">
         <v>183</v>
@@ -4163,7 +4287,7 @@
         <v>185</v>
       </c>
       <c r="D69" s="5" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="E69" s="5" t="s">
         <v>184</v>
@@ -4171,13 +4295,13 @@
     </row>
     <row r="70" spans="1:5" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="C70" s="5" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="D70" s="7" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="E70" s="5" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="71" spans="1:5" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -4193,310 +4317,310 @@
         <v>192</v>
       </c>
     </row>
-    <row r="72" spans="1:5" s="7" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" s="7" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A72" s="9"/>
-      <c r="B72" s="9" t="s">
-        <v>249</v>
-      </c>
-      <c r="C72" s="8" t="s">
+      <c r="B72" s="26" t="s">
+        <v>245</v>
+      </c>
+      <c r="C72" s="16" t="s">
+        <v>267</v>
+      </c>
+      <c r="D72" s="27" t="s">
+        <v>244</v>
+      </c>
+      <c r="E72" s="16" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A73" s="9"/>
+      <c r="B73" s="26" t="s">
         <v>246</v>
       </c>
-      <c r="D72" s="7" t="s">
+      <c r="C73" s="16" t="s">
+        <v>262</v>
+      </c>
+      <c r="D73" s="27" t="s">
+        <v>193</v>
+      </c>
+      <c r="E73" s="16" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A74" s="9"/>
+      <c r="B74" s="26" t="s">
+        <v>246</v>
+      </c>
+      <c r="C74" s="16" t="s">
+        <v>268</v>
+      </c>
+      <c r="D74" s="27" t="s">
         <v>247</v>
       </c>
-      <c r="E72" s="5" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A73" s="9"/>
-      <c r="B73" s="9" t="s">
-        <v>252</v>
-      </c>
-      <c r="C73" s="8" t="s">
-        <v>251</v>
-      </c>
-      <c r="D73" s="7" t="s">
-        <v>193</v>
-      </c>
-      <c r="E73" s="5" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="9"/>
-      <c r="B74" s="9" t="s">
-        <v>252</v>
-      </c>
-      <c r="C74" s="8" t="s">
-        <v>194</v>
-      </c>
-      <c r="D74" s="7" t="s">
-        <v>253</v>
-      </c>
-      <c r="E74" s="5" t="s">
-        <v>254</v>
+      <c r="E74" s="16" t="s">
+        <v>260</v>
       </c>
     </row>
     <row r="75" spans="1:5" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A75" s="9"/>
-      <c r="B75" s="9" t="s">
-        <v>252</v>
-      </c>
-      <c r="C75" s="8" t="s">
-        <v>195</v>
-      </c>
-      <c r="D75" s="7" t="s">
+      <c r="B75" s="26" t="s">
+        <v>246</v>
+      </c>
+      <c r="C75" s="16" t="s">
+        <v>263</v>
+      </c>
+      <c r="D75" s="27" t="s">
+        <v>257</v>
+      </c>
+      <c r="E75" s="16" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A76" s="9"/>
+      <c r="B76" s="26" t="s">
+        <v>246</v>
+      </c>
+      <c r="C76" s="16" t="s">
+        <v>269</v>
+      </c>
+      <c r="D76" s="27" t="s">
+        <v>248</v>
+      </c>
+      <c r="E76" s="16" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="B77" s="26" t="s">
+        <v>246</v>
+      </c>
+      <c r="C77" s="16" t="s">
+        <v>270</v>
+      </c>
+      <c r="D77" s="27" t="s">
+        <v>249</v>
+      </c>
+      <c r="E77" s="16" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="B78" s="26" t="s">
+        <v>246</v>
+      </c>
+      <c r="C78" s="16" t="s">
         <v>271</v>
       </c>
-      <c r="E75" s="5" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A76" s="9"/>
-      <c r="B76" s="9" t="s">
-        <v>252</v>
-      </c>
-      <c r="C76" s="8" t="s">
-        <v>258</v>
-      </c>
-      <c r="D76" s="7" t="s">
-        <v>255</v>
-      </c>
-      <c r="E76" s="5" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="B77" s="9" t="s">
-        <v>252</v>
-      </c>
-      <c r="C77" s="8" t="s">
-        <v>261</v>
-      </c>
-      <c r="D77" s="7" t="s">
-        <v>256</v>
-      </c>
-      <c r="E77" s="5" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="B78" s="9" t="s">
-        <v>252</v>
-      </c>
-      <c r="C78" s="8" t="s">
-        <v>263</v>
-      </c>
-      <c r="D78" s="7" t="s">
-        <v>264</v>
-      </c>
-      <c r="E78" s="5" t="s">
-        <v>262</v>
+      <c r="D78" s="27" t="s">
+        <v>250</v>
+      </c>
+      <c r="E78" s="16" t="s">
+        <v>266</v>
       </c>
     </row>
     <row r="79" spans="1:5" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B79" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="C79" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="D79" s="10" t="s">
         <v>196</v>
       </c>
-      <c r="C79" s="5" t="s">
+      <c r="E79" s="5" t="s">
         <v>197</v>
-      </c>
-      <c r="D79" s="10" t="s">
-        <v>198</v>
-      </c>
-      <c r="E79" s="5" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="80" spans="1:5" s="7" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="B80" s="7" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C80" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="D80" s="10" t="s">
+        <v>199</v>
+      </c>
+      <c r="E80" s="5" t="s">
         <v>200</v>
-      </c>
-      <c r="D80" s="10" t="s">
-        <v>201</v>
-      </c>
-      <c r="E80" s="5" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="81" spans="2:5" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B81" s="7" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C81" s="5" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D81" s="10" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="E81" s="21" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="82" spans="2:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B82" s="7" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C82" s="8" t="s">
+        <v>203</v>
+      </c>
+      <c r="D82" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="E82" s="9" t="s">
         <v>205</v>
-      </c>
-      <c r="D82" s="10" t="s">
-        <v>206</v>
-      </c>
-      <c r="E82" s="9" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="83" spans="2:5" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="B83" s="7" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C83" s="8" t="s">
+        <v>206</v>
+      </c>
+      <c r="D83" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="E83" s="5" t="s">
         <v>208</v>
-      </c>
-      <c r="D83" s="7" t="s">
-        <v>209</v>
-      </c>
-      <c r="E83" s="5" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="84" spans="2:5" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B84" s="7" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C84" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="D84" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="E84" s="5" t="s">
         <v>211</v>
-      </c>
-      <c r="D84" s="7" t="s">
-        <v>212</v>
-      </c>
-      <c r="E84" s="5" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="85" spans="2:5" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B85" s="7" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C85" s="8" t="s">
+        <v>212</v>
+      </c>
+      <c r="D85" s="10" t="s">
+        <v>213</v>
+      </c>
+      <c r="E85" s="22" t="s">
         <v>214</v>
-      </c>
-      <c r="D85" s="10" t="s">
-        <v>215</v>
-      </c>
-      <c r="E85" s="22" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="86" spans="2:5" s="7" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="B86" s="7" t="s">
+        <v>215</v>
+      </c>
+      <c r="C86" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="D86" s="7" t="s">
         <v>217</v>
       </c>
-      <c r="C86" s="5" t="s">
+      <c r="E86" s="5" t="s">
         <v>218</v>
-      </c>
-      <c r="D86" s="7" t="s">
-        <v>219</v>
-      </c>
-      <c r="E86" s="5" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="87" spans="2:5" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B87" s="7" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C87" s="5" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D87" s="10" t="s">
         <v>187</v>
       </c>
       <c r="E87" s="5" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="88" spans="2:5" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B88" s="7" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C88" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="D88" s="9" t="s">
         <v>226</v>
       </c>
-      <c r="D88" s="9" t="s">
-        <v>228</v>
-      </c>
       <c r="E88" s="5" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="89" spans="2:5" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="C89" s="5" t="s">
+        <v>225</v>
+      </c>
+      <c r="D89" s="7" t="s">
+        <v>229</v>
+      </c>
+      <c r="E89" s="5" t="s">
         <v>227</v>
-      </c>
-      <c r="D89" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="E89" s="5" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="90" spans="2:5" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="C90" s="5" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="D90" s="7" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="E90" s="5" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="91" spans="2:5" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="C91" s="5" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D91" s="7" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="E91" s="5" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="92" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C92" s="24" t="s">
-        <v>266</v>
+        <v>252</v>
       </c>
       <c r="D92" s="23" t="s">
-        <v>265</v>
+        <v>251</v>
       </c>
     </row>
     <row r="93" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="C93" s="1" t="s">
-        <v>268</v>
+        <v>254</v>
       </c>
       <c r="D93" s="25" t="s">
         <v>187</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>267</v>
+        <v>253</v>
       </c>
     </row>
     <row r="94" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C94" s="1" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="D94" t="s">
         <v>188</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>270</v>
+        <v>256</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
byt - frames conversion (part)
</commit_message>
<xml_diff>
--- a/tecto2umr/PDT-mozne-chyby.xlsx
+++ b/tecto2umr/PDT-mozne-chyby.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28635" windowHeight="12870"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28635" windowHeight="12870" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="2025-Oct-23" sheetId="1" r:id="rId1"/>
+    <sheet name="2025-May" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="145621" iterateDelta="1E-4"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="328">
   <si>
     <t>#Gen</t>
   </si>
@@ -1868,6 +1868,12 @@
   </si>
   <si>
     <t xml:space="preserve">faust_2010_07_jh_05-SCzechT-p0436-s1A-root </t>
+  </si>
+  <si>
+    <t>?? jak se pozná, k čemu patří #Neg (k být, nikoli k trávit)</t>
+  </si>
+  <si>
+    <t>?? jak se pozná, k čemu patří #Neg (k prvnímu nezdálo)</t>
   </si>
   <si>
     <t>GRAD</t>
@@ -2397,491 +2403,600 @@
 nebo kde je zachycena info o negaci ??? (v Manuálu jsem nenašla)</t>
   </si>
   <si>
+    <t xml:space="preserve">??? nerozumím moc anotaci - jak se pozná, k čemu patří #Neg.CM (prohlídka nebyla účelem) a k čemu pouze.CM (pouze bylo účelem) ...
+spíš bych doplnila na něco jako: "nebyla" účelem prohlídka, pouze [bylo účelem] zastavit se a ... </t>
+  </si>
+  <si>
     <t>lk_123.06-SCzechT-lk_123-285-root</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Nebyla účelem</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> velká prohlídka , </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>pouze</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> zastavit se a podívat se na tehdejší trhy , které tam byly , a pokračovat dál .</t>
+    </r>
+  </si>
+  <si>
     <t>#Neg.CM</t>
   </si>
   <si>
+    <r>
+      <t xml:space="preserve">Normální kamarádi tuhle vnitřní bolest </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>nevidí</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> , jenom mí nejbližší ji poznají .</t>
+    </r>
+  </si>
+  <si>
+    <t>?? prož negace až za "vidět" a za čárkou
+?? špatná segmentace na věty</t>
+  </si>
+  <si>
     <t>ADVS</t>
   </si>
   <si>
     <t>dk_132.02-SCzechT-dk_132-111-root</t>
   </si>
   <si>
+    <r>
+      <t xml:space="preserve">Tam se dalo ve skupině , aniž </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>byla</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> příliš podezřelá , </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>trávit</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> řadu týdnů .</t>
+    </r>
+  </si>
+  <si>
+    <t>lk-28105_04.01-SCzechT-lk-28105_04-d1e551-x5-root 2</t>
+  </si>
+  <si>
     <t xml:space="preserve">pk_015.06-SCzechT-pk_015-d1e1641-x2-root </t>
   </si>
   <si>
     <t>T-wsj0089-001-p1s20</t>
   </si>
   <si>
+    <r>
+      <t xml:space="preserve">Jako odborník jsem měl za úkol , abych všechno , co se mně </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>nezdálo</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> na jatka , ale k dalšímu chovu , dostával do svých stájí .</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">#Neg až za ADVS, patří k "odevzdávat", tj. asi by mělo být za "aniž"?  </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Řekla : " Půjdeme tam dopoledne na cihly a dostaneme tam oběd , </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>aniž</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> bychom </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>odevzdávaly</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> přídělové lístky . "</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Zvoníci poté začnou na znamení měnit pořadí, v němž zvony znějí, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>aniž</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> by </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>měnili</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> pravidelný rytmus úderů.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">#Neg až za ADVS, patří k "měnit",  tj. asi by mělo být za "aniž"?   </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Když je odpověď na kritiku pouze lepším vysvětlením strategií, aniž by </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>se změnily</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> důvody té kritiky, jsem přesvědčen, že pan Kageyama stále nezaútočil na základní příčinu problému a léčí jen jeho příznaky.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">#Neg až za ADVS, patří k "změnit_se",  tj. asi by mělo být za "aniž"?   </t>
+  </si>
+  <si>
     <t>T-wsj1092-001-p1s27</t>
   </si>
   <si>
-    <t>ml_043.03-SCzechT-m-d1e1117-x4-457</t>
-  </si>
-  <si>
-    <t>t_lemma = ",#Comma" … nadbytečná</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Ve druhém tahu 18. týdne Sportky v I. pořadí je 1 výhra 1998352 Kč, </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>ve II. není žádná výhra,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> ve III. je 73 výher po 9759 Kč, ve IV. je 4630 výher po 307 Kč, v V. je 80873 výher po 37 Kč.</t>
-    </r>
-  </si>
-  <si>
-    <t>#Neg.RHEM patří pod "být" (2. klauze)</t>
-  </si>
-  <si>
-    <t>#Neg.RHEM patří pod "mít" nebo k "výlučně"</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Nebudeme mít žáky výlučně z velmi bohatých rodin</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>, upozorňuje ředitel Ward.</t>
-    </r>
-  </si>
-  <si>
-    <t>lk-28105_04.01-SCzechT-lk-28105_04-d1e551-x5-root</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <strike/>
-        <sz val="11"/>
-        <color theme="0" tint="-0.499984740745262"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Nebyla účelem</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="0" tint="-0.499984740745262"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> velká prohlídka , </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <strike/>
-        <sz val="11"/>
-        <color theme="0" tint="-0.499984740745262"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>pouze</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="0" tint="-0.499984740745262"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> zastavit se a podívat se na tehdejší trhy , které tam byly , a pokračovat dál .</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Normální kamarádi tuhle vnitřní bolest </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <strike/>
-        <sz val="11"/>
-        <color theme="0" tint="-0.499984740745262"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>nevidí</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="0" tint="-0.499984740745262"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> , jenom mí nejbližší ji poznají .</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Tam se dalo ve skupině , aniž </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <strike/>
-        <sz val="11"/>
-        <color theme="0" tint="-0.499984740745262"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>byla</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="0" tint="-0.499984740745262"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> příliš podezřelá , </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <strike/>
-        <sz val="11"/>
-        <color theme="0" tint="-0.499984740745262"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>trávit</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="0" tint="-0.499984740745262"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> řadu týdnů .</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Jako odborník jsem měl za úkol , abych všechno , co se mně </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <strike/>
-        <sz val="11"/>
-        <color theme="0" tint="-0.499984740745262"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>nezdálo</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="0" tint="-0.499984740745262"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> na jatka , ale k dalšímu chovu , dostával do svých stájí .</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">?? prož negace až za "vidět" a za čárkou
-?? špatná segmentace na věty
+    <t>kde</t>
+  </si>
+  <si>
+    <t>typ</t>
+  </si>
+  <si>
+    <t>chybně</t>
+  </si>
+  <si>
+    <t>správně</t>
+  </si>
+  <si>
+    <t>komentář</t>
+  </si>
+  <si>
+    <t>chybný rámec</t>
+  </si>
+  <si>
+    <t>být-002, v41jsC</t>
+  </si>
+  <si>
+    <t>být-011, v41jsU</t>
+  </si>
+  <si>
+    <t>špatně přiřazen val. rámec, má být zástupné a existenční</t>
+  </si>
+  <si>
+    <t>prohozeny aktanty</t>
+  </si>
+  <si>
+    <t>být-002, v41lsC
+ACT co (7x)
+PAT tenhle|to</t>
+  </si>
+  <si>
+    <t>ACT … tenhle|to
+PAT … co (172x)</t>
+  </si>
+  <si>
+    <t>po změně bude uniformní přiřazení ACT a PAT</t>
+  </si>
+  <si>
+    <t>lk_010.06-SCzechT-lk_010-d1e2515-x2-root</t>
+  </si>
+  <si>
+    <t>Jakobín od Antonína Dvořáka.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> t-ln94200-153-p6s7</t>
+  </si>
+  <si>
+    <t>být-005, v41lsF</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">To.ACT </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[=argument, že všude se vyplácejí prémie za zápasy, tak proč by to u nás mělo být jinak]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> je (jako kdyby si stěžoval...).PAT </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">… nesedí forma ani sémantika PAT. 
 </t>
     </r>
     <r>
       <rPr>
         <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>#Neg.CM --&gt; #Neg.RHEM a převěšeno pod sloveso</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">?? jak se pozná, k čemu patří #Neg (k prvnímu nezdálo)
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>#Neg.CM --&gt; #Neg.RHEM a převěšeno pod sloveso</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Řekla : " Půjdeme tam dopoledne na cihly a dostaneme tam oběd , </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <strike/>
-        <sz val="11"/>
-        <color theme="0" tint="-0.499984740745262"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>aniž</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="0" tint="-0.499984740745262"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> bychom </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <strike/>
-        <sz val="11"/>
-        <color theme="0" tint="-0.499984740745262"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>odevzdávaly</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="0" tint="-0.499984740745262"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> přídělové lístky . "</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Zvoníci poté začnou na znamení měnit pořadí, v němž zvony znějí, </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <strike/>
-        <sz val="11"/>
-        <color theme="0" tint="-0.499984740745262"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>aniž</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="0" tint="-0.499984740745262"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> by </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <strike/>
-        <sz val="11"/>
-        <color theme="0" tint="-0.499984740745262"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>měnili</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="0" tint="-0.499984740745262"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> pravidelný rytmus úderů.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Když je odpověď na kritiku pouze lepším vysvětlením strategií, aniž by </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <strike/>
-        <sz val="11"/>
-        <color theme="0" tint="-0.499984740745262"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>se změnily</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="0" tint="-0.499984740745262"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> důvody té kritiky, jsem přesvědčen, že pan Kageyama stále nezaútočil na základní příčinu problému a léčí jen jeho příznaky.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">??? nerozumím moc anotaci - jak se pozná, k čemu patří #Neg.CM (prohlídka nebyla účelem) a k čemu pouze.CM (pouze bylo účelem) ...
-spíš bych doplnila na něco jako: "nebyla" účelem prohlídka, pouze [bylo účelem] zastavit se a ... 
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>upravena pozice #Neg (JŠ)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>?? jak se pozná, k čemu patří #Neg (k být, nikoli k trávit)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0" tint="-0.499984740745262"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>upravena pozice #Neg (JŠ)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">#Neg až za ADVS, patří k "odevzdávat", tj. asi by mělo být za "aniž"?  
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>upravena pozice #Neg (JŠ)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">#Neg až za ADVS, patří k "měnit",  tj. asi by mělo být za "aniž"?   
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>upravena pozice #Neg (JŠ)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">#Neg až za ADVS, patří k "změnit_se",  tj. asi by mělo být za "aniž"?   
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>upravena pozice #Neg (JŠ)</t>
-    </r>
+        <color theme="4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ZU … ANO,je to špatně</t>
+    </r>
+  </si>
+  <si>
+    <t>lk_035.09-SCzechT-lk_035-d1e2793-x2-root</t>
+  </si>
+  <si>
+    <r>
+      <t>Na tom.PAT něco.ACT je</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> #PersPron.EFF ???</t>
+    </r>
+  </si>
+  <si>
+    <t>???</t>
+  </si>
+  <si>
+    <t>být-004, v41lsD</t>
+  </si>
+  <si>
+    <t>ak_065.06-SCzechT-ak_065-d1e1979-x3-roo</t>
+  </si>
+  <si>
+    <t>lemmatizace</t>
+  </si>
+  <si>
+    <t>let --&gt; rok</t>
+  </si>
+  <si>
+    <t>ju_038.06-SCzechT-ju_038-d1e1848-x2-root</t>
+  </si>
+  <si>
+    <t>ml_043.11-SCzechT-ml_043-d1e3740-x2-root</t>
+  </si>
+  <si>
+    <t>ml_013.07-SCzechT-ml_013-d1e2766-x2-root</t>
+  </si>
+  <si>
+    <t>ml_025.03-SCzechT-ml_025-d1e1565-x2-root</t>
+  </si>
+  <si>
+    <t>ez_039.00-SCzechT-ez_039-d1e285-x2-root</t>
+  </si>
+  <si>
+    <t>lk_012.05-SCzechT-lk_012-d1e2247-x2-root</t>
+  </si>
+  <si>
+    <t>t-mf930709-009-p2s1</t>
+  </si>
+  <si>
+    <t>být-002, v41lsC
+ACT co, PAT tenhle|to</t>
+  </si>
+  <si>
+    <t>pk_015.08-SCzechT-pk_015-d1e2094-x2-root</t>
+  </si>
+  <si>
+    <t>ak_054.09-SCzechT-ak_054-d1e2148-x3-root</t>
+  </si>
+  <si>
+    <t>ak_054.09-SCzechT-ak_054-d1e2162-x2-root</t>
+  </si>
+  <si>
+    <t>hg_005.08-SCzechT-hg_005-d1e2945-x2-root</t>
+  </si>
+  <si>
+    <t>hg_005.08-SCzechT-hg_005-d1e2949-x2-root</t>
+  </si>
+  <si>
+    <t>t-ln94208-101-p5s19</t>
+  </si>
+  <si>
+    <t>Od Toronta mám problémy s nohou, nikdo neví, co mi je.</t>
+  </si>
+  <si>
+    <t>Co vám bylo ?</t>
+  </si>
+  <si>
+    <t>Co mu je ?</t>
+  </si>
+  <si>
+    <t>ju_027.03-SCzechT-ju_027-d1e1019-x2-root</t>
+  </si>
+  <si>
+    <t>ak_062.06-SCzechT-ak_062-d1e1343-x3-root</t>
+  </si>
+  <si>
+    <t>Straszheim čeká, že mu bude pěkné vedro a má pravdu.</t>
+  </si>
+  <si>
+    <t>T-wsj0569-001-p1s2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sice dativ subjektu, ale jiný význam
+(cca 1285x učení věku) </t>
+  </si>
+  <si>
+    <t>být-009, v41jsQ</t>
+  </si>
+  <si>
+    <t>ml_119.03-SCzechT-ml_119-d1e753-x3-root</t>
+  </si>
+  <si>
+    <t>lépe --&gt; dobře</t>
+  </si>
+  <si>
+    <t>Dětem by tam bývalo možná bylo líp než tady v Praze .</t>
+  </si>
+  <si>
+    <t>hg_022.08-SCzechT-hg_022-716-root</t>
+  </si>
+  <si>
+    <t>… protože mi tam není smutno …</t>
+  </si>
+  <si>
+    <t>chybný aktant</t>
+  </si>
+  <si>
+    <t>není mi smutno.TWHEN</t>
+  </si>
+  <si>
+    <t>není mi smutno.MANN</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> stejně jako v "… takže mu taky , to víte , není veselo.MANN"
+(ml_009.06-SCzechT-ml_009-1190-root)</t>
+  </si>
+  <si>
+    <t>lematizace</t>
+  </si>
+  <si>
+    <t>věty s val. rámcem v41jsAD (být jedno; být hanba)</t>
+  </si>
+  <si>
+    <t>CPHR lematizováno různě:</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">CPHR 27x jako </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"jedno",</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> které má 25x sepos adv.denot.ngrad.nneg, 1x adv.denot.ngrad.neg a 1x n.quant.def;
+CPHR 10x jako </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"jeden",</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> sempos n.quant.def</t>
+    </r>
+  </si>
+  <si>
+    <t>?? sjednotit asi na "jedno" s adverbiálním sempos</t>
   </si>
 </sst>
 </file>
@@ -2964,25 +3079,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
+      <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="0" tint="-0.249977111117893"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
+      <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <strike/>
       <sz val="11"/>
-      <color theme="0" tint="-0.499984740745262"/>
+      <color theme="4"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -3008,8 +3121,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor rgb="FFA6A6A6"/>
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -3037,15 +3150,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -3095,35 +3208,68 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="5">
-    <cellStyle name="Excel Built-in Check Cell" xfId="4"/>
-    <cellStyle name="Excel Built-in Check Cell 1" xfId="3"/>
+  <cellStyles count="2">
     <cellStyle name="Kontrolní buňka" xfId="1" builtinId="23"/>
     <cellStyle name="Normální" xfId="0" builtinId="0"/>
-    <cellStyle name="Normální 2" xfId="2"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -3393,7 +3539,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3401,1226 +3547,1196 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E94"/>
+  <dimension ref="A1:E91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A69" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E70" sqref="E70"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C92" sqref="C92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.42578125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="30.85546875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="54.85546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="49.7109375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="86" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.7109375" style="2"/>
+    <col min="1" max="1" width="23.42578125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="30.85546875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="54.85546875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="49.7109375" style="3" customWidth="1"/>
+    <col min="5" max="5" width="86" style="2" customWidth="1"/>
+    <col min="6" max="16384" width="8.7109375" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="4" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="7" customFormat="1" ht="60.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+    <row r="2" spans="1:5" s="8" customFormat="1" ht="60.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="6" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="7" customFormat="1" ht="135" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+    <row r="3" spans="1:5" s="8" customFormat="1" ht="135" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="6" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+    <row r="4" spans="1:5" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="6" t="s">
+      <c r="B4" s="6"/>
+      <c r="C4" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="6" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+    <row r="5" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="6" t="s">
+      <c r="B5" s="6"/>
+      <c r="C5" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="E5" s="5"/>
-    </row>
-    <row r="6" spans="1:5" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+      <c r="E5" s="6"/>
+    </row>
+    <row r="6" spans="1:5" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="8" t="s">
+      <c r="B6" s="6"/>
+      <c r="C6" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E6" s="6" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+    <row r="7" spans="1:5" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="6" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:5" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
+    <row r="8" spans="1:5" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="6" t="s">
+      <c r="B8" s="6"/>
+      <c r="C8" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="E8" s="6" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:5" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+    <row r="9" spans="1:5" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="5"/>
-      <c r="C9" s="8" t="s">
+      <c r="B9" s="6"/>
+      <c r="C9" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D9" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="E9" s="6" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:5" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
+    <row r="10" spans="1:5" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="E10" s="6" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:5" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
+    <row r="11" spans="1:5" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="5"/>
-      <c r="C11" s="6" t="s">
+      <c r="B11" s="6"/>
+      <c r="C11" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="E11" s="6" t="s">
+      <c r="E11" s="7" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
+    <row r="12" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="5"/>
-      <c r="C12" s="6" t="s">
+      <c r="B12" s="6"/>
+      <c r="C12" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="D12" s="10" t="s">
+      <c r="D12" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="E12" s="6" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="13" spans="1:5" s="7" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
+    <row r="13" spans="1:5" s="8" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="5"/>
-      <c r="C13" s="8" t="s">
+      <c r="B13" s="6"/>
+      <c r="C13" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="D13" s="10" t="s">
+      <c r="D13" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="E13" s="11" t="s">
+      <c r="E13" s="12" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="14" spans="1:5" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
+    <row r="14" spans="1:5" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="D14" s="10" t="s">
+      <c r="D14" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="E14" s="11" t="s">
+      <c r="E14" s="12" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="15" spans="1:5" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
+    <row r="15" spans="1:5" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="5"/>
-      <c r="C15" s="6" t="s">
+      <c r="B15" s="6"/>
+      <c r="C15" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="D15" s="10" t="s">
+      <c r="D15" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="E15" s="11" t="s">
+      <c r="E15" s="12" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="16" spans="1:5" s="7" customFormat="1" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="C16" s="5"/>
-      <c r="E16" s="5"/>
-    </row>
-    <row r="17" spans="1:5" s="7" customFormat="1" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="C17" s="5"/>
-      <c r="E17" s="5"/>
-    </row>
-    <row r="18" spans="1:5" s="7" customFormat="1" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="C18" s="5"/>
-      <c r="E18" s="5"/>
-    </row>
-    <row r="19" spans="1:5" s="7" customFormat="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C19" s="5"/>
-      <c r="E19" s="5"/>
-    </row>
-    <row r="20" spans="1:5" s="7" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="12" t="s">
+    <row r="16" spans="1:5" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="C16" s="6"/>
+      <c r="E16" s="6"/>
+    </row>
+    <row r="17" spans="1:5" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="C17" s="6"/>
+      <c r="E17" s="6"/>
+    </row>
+    <row r="18" spans="1:5" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="C18" s="6"/>
+      <c r="E18" s="6"/>
+    </row>
+    <row r="19" spans="1:5" s="8" customFormat="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C19" s="6"/>
+      <c r="E19" s="6"/>
+    </row>
+    <row r="20" spans="1:5" s="8" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="B20" s="13" t="s">
+      <c r="B20" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="C20" s="12" t="s">
+      <c r="C20" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="D20" s="13" t="s">
+      <c r="D20" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="E20" s="12" t="s">
+      <c r="E20" s="13" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="21" spans="1:5" s="7" customFormat="1" ht="59.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="5" t="s">
+    <row r="21" spans="1:5" s="8" customFormat="1" ht="59.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="B21" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="C21" s="5" t="s">
+      <c r="C21" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="E21" s="10"/>
-    </row>
-    <row r="22" spans="1:5" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="5" t="s">
+      <c r="E21" s="11"/>
+    </row>
+    <row r="22" spans="1:5" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="B22" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="C22" s="5" t="s">
+      <c r="C22" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="D22" s="10" t="s">
+      <c r="D22" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="E22" s="10" t="s">
+      <c r="E22" s="11" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="23" spans="1:5" s="7" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A23" s="5" t="s">
+    <row r="23" spans="1:5" s="8" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="B23" s="5" t="s">
+      <c r="B23" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="C23" s="5" t="s">
+      <c r="C23" s="6" t="s">
         <v>128</v>
       </c>
-      <c r="D23" s="7" t="s">
+      <c r="D23" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="E23" s="14" t="s">
+      <c r="E23" s="15" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="24" spans="1:5" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="15" t="s">
+    <row r="24" spans="1:5" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="B24" s="16" t="s">
+      <c r="B24" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="C24" s="16" t="s">
+      <c r="C24" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="E24" s="5"/>
-    </row>
-    <row r="25" spans="1:5" s="7" customFormat="1" ht="90" x14ac:dyDescent="0.25">
-      <c r="A25" s="5" t="s">
+      <c r="E24" s="6"/>
+    </row>
+    <row r="25" spans="1:5" s="8" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A25" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="B25" s="5" t="s">
+      <c r="B25" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="C25" s="5" t="s">
+      <c r="C25" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="E25" s="5"/>
-    </row>
-    <row r="26" spans="1:5" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A26" s="15" t="s">
+      <c r="E25" s="6"/>
+    </row>
+    <row r="26" spans="1:5" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A26" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="B26" s="16" t="s">
+      <c r="B26" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="C26" s="16" t="s">
+      <c r="C26" s="17" t="s">
         <v>79</v>
       </c>
-      <c r="E26" s="5"/>
-    </row>
-    <row r="27" spans="1:5" s="7" customFormat="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A27" s="5"/>
-      <c r="B27" s="5"/>
-      <c r="C27" s="5"/>
-      <c r="E27" s="5"/>
-    </row>
-    <row r="28" spans="1:5" s="7" customFormat="1" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="12" t="s">
+      <c r="E26" s="6"/>
+    </row>
+    <row r="27" spans="1:5" s="8" customFormat="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A27" s="6"/>
+      <c r="B27" s="6"/>
+      <c r="C27" s="6"/>
+      <c r="E27" s="6"/>
+    </row>
+    <row r="28" spans="1:5" s="8" customFormat="1" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="B28" s="13" t="s">
+      <c r="B28" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="C28" s="12" t="s">
+      <c r="C28" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="D28" s="13" t="s">
+      <c r="D28" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="E28" s="13" t="s">
+      <c r="E28" s="14" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="29" spans="1:5" s="7" customFormat="1" ht="45.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="9" t="s">
+    <row r="29" spans="1:5" s="8" customFormat="1" ht="45.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="B29" s="11" t="s">
+      <c r="B29" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="C29" s="5" t="s">
+      <c r="C29" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="D29" s="5" t="s">
+      <c r="D29" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="E29" s="5"/>
-    </row>
-    <row r="30" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="9" t="s">
+      <c r="E29" s="6"/>
+    </row>
+    <row r="30" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="B30" s="11"/>
-      <c r="C30" s="5" t="s">
+      <c r="B30" s="12"/>
+      <c r="C30" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="D30" s="7" t="s">
+      <c r="D30" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="E30" s="5"/>
-    </row>
-    <row r="31" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="7" t="s">
+      <c r="E30" s="6"/>
+    </row>
+    <row r="31" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="B31" s="11" t="s">
+      <c r="B31" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="C31" s="5" t="s">
+      <c r="C31" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="D31" s="10" t="s">
+      <c r="D31" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="E31" s="5"/>
-    </row>
-    <row r="32" spans="1:5" s="7" customFormat="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C32" s="5"/>
-      <c r="E32" s="5"/>
-    </row>
-    <row r="33" spans="1:5" s="7" customFormat="1" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="12" t="s">
+      <c r="E31" s="6"/>
+    </row>
+    <row r="32" spans="1:5" s="8" customFormat="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C32" s="6"/>
+      <c r="E32" s="6"/>
+    </row>
+    <row r="33" spans="1:5" s="8" customFormat="1" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="B33" s="13" t="s">
+      <c r="B33" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="C33" s="12" t="s">
+      <c r="C33" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="D33" s="13" t="s">
+      <c r="D33" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="E33" s="13" t="s">
+      <c r="E33" s="14" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="34" spans="1:5" s="7" customFormat="1" ht="120.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="9" t="s">
+    <row r="34" spans="1:5" s="8" customFormat="1" ht="120.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="10" t="s">
         <v>97</v>
       </c>
-      <c r="B34" s="11" t="s">
+      <c r="B34" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="C34" s="17" t="s">
+      <c r="C34" s="18" t="s">
         <v>122</v>
       </c>
-      <c r="D34" s="5"/>
-      <c r="E34" s="5"/>
-    </row>
-    <row r="35" spans="1:5" s="7" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A35" s="5" t="s">
+      <c r="D34" s="6"/>
+      <c r="E34" s="6"/>
+    </row>
+    <row r="35" spans="1:5" s="8" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A35" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="C35" s="5" t="s">
+      <c r="C35" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="E35" s="5" t="s">
+      <c r="E35" s="6" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="36" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="7" t="s">
+    <row r="36" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="C36" s="5" t="s">
+      <c r="C36" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="E36" s="10" t="s">
+      <c r="E36" s="11" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="37" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C37" s="5" t="s">
+    <row r="37" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C37" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="E37" s="10" t="s">
+      <c r="E37" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="38" spans="1:5" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="B38" s="7" t="s">
+    <row r="38" spans="1:5" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="B38" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="C38" s="5" t="s">
+      <c r="C38" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="E38" s="5" t="s">
+      <c r="E38" s="6" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="39" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="7" t="s">
+    <row r="39" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B39" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="C39" s="5" t="s">
+      <c r="C39" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="E39" s="5" t="s">
+      <c r="E39" s="6" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="40" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="7" t="s">
+    <row r="40" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B40" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="C40" s="5" t="s">
+      <c r="C40" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="E40" s="5" t="s">
+      <c r="E40" s="6" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="41" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="7" t="s">
+    <row r="41" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B41" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="C41" s="5" t="s">
+      <c r="C41" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="E41" s="10" t="s">
+      <c r="E41" s="11" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="42" spans="1:5" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="B42" s="7" t="s">
+    <row r="42" spans="1:5" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="B42" s="8" t="s">
         <v>114</v>
       </c>
-      <c r="C42" s="5" t="s">
+      <c r="C42" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="E42" s="10" t="s">
+      <c r="E42" s="11" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="43" spans="1:5" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="B43" s="7" t="s">
+    <row r="43" spans="1:5" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="B43" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="C43" s="5" t="s">
+      <c r="C43" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="E43" s="10" t="s">
+      <c r="E43" s="11" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="44" spans="1:5" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="B44" s="7" t="s">
+    <row r="44" spans="1:5" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="B44" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="C44" s="5" t="s">
+      <c r="C44" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="E44" s="10" t="s">
+      <c r="E44" s="11" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="45" spans="1:5" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="B45" s="7" t="s">
+    <row r="45" spans="1:5" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="B45" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="C45" s="5" t="s">
+      <c r="C45" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="E45" s="10" t="s">
+      <c r="E45" s="11" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="46" spans="1:5" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="B46" s="7" t="s">
+    <row r="46" spans="1:5" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="B46" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="C46" s="5" t="s">
+      <c r="C46" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="E46" s="5" t="s">
+      <c r="E46" s="6" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="47" spans="1:5" s="7" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="7" t="s">
+    <row r="47" spans="1:5" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="C47" s="5"/>
-      <c r="E47" s="5"/>
+      <c r="C47" s="6"/>
+      <c r="E47" s="6"/>
     </row>
     <row r="48" spans="1:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A48" s="3" t="s">
+      <c r="A48" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="B48" s="4" t="s">
+      <c r="B48" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C48" s="3"/>
-      <c r="D48" s="4"/>
-      <c r="E48" s="4"/>
-    </row>
-    <row r="49" spans="1:5" s="7" customFormat="1" ht="60.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="11" t="s">
+      <c r="C48" s="4"/>
+      <c r="D48" s="5"/>
+      <c r="E48" s="5"/>
+    </row>
+    <row r="49" spans="1:5" ht="60.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="B49" s="7" t="s">
+      <c r="B49" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="C49" s="5" t="s">
+      <c r="C49" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="D49" s="7" t="s">
+      <c r="D49" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="E49" s="11" t="s">
+      <c r="E49" s="1" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="50" spans="1:5" s="7" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="B50" s="7" t="s">
+    <row r="50" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="B50" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="C50" s="5" t="s">
+      <c r="C50" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="D50" s="7" t="s">
+      <c r="D50" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="E50" s="11" t="s">
+      <c r="E50" s="1" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="51" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B51" s="7" t="s">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B51" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="C51" s="5" t="s">
+      <c r="C51" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="D51" s="10" t="s">
+      <c r="D51" s="20" t="s">
         <v>164</v>
       </c>
-      <c r="E51" s="5" t="s">
+      <c r="E51" s="2" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="52" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="7" t="s">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B52" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="C52" s="5" t="s">
+      <c r="C52" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="D52" s="7" t="s">
+      <c r="D52" s="19" t="s">
         <v>163</v>
       </c>
-      <c r="E52" s="10" t="s">
+      <c r="E52" s="20" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="53" spans="1:5" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="B53" s="7" t="s">
+    <row r="53" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="B53" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="C53" s="5" t="s">
+      <c r="C53" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="D53" s="7" t="s">
+      <c r="D53" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="E53" s="11" t="s">
+      <c r="E53" s="1" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="54" spans="1:5" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="B54" s="7" t="s">
+    <row r="54" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B54" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="C54" s="5" t="s">
+      <c r="C54" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="D54" s="7" t="s">
+      <c r="D54" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="E54" s="11" t="s">
+      <c r="E54" s="1" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="55" spans="1:5" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="B55" s="7" t="s">
+    <row r="55" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="B55" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="C55" s="5" t="s">
+      <c r="C55" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="D55" s="10" t="s">
+      <c r="D55" s="20" t="s">
         <v>165</v>
       </c>
-      <c r="E55" s="5" t="s">
+      <c r="E55" s="2" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="56" spans="1:5" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="B56" s="7" t="s">
+    <row r="56" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B56" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="C56" s="5" t="s">
+      <c r="C56" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="D56" s="10" t="s">
+      <c r="D56" s="20" t="s">
         <v>166</v>
       </c>
-      <c r="E56" s="5" t="s">
+      <c r="E56" s="2" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="57" spans="1:5" s="7" customFormat="1" ht="90" x14ac:dyDescent="0.25">
-      <c r="B57" s="7" t="s">
+    <row r="57" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="B57" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="C57" s="5" t="s">
+      <c r="C57" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="D57" s="7" t="s">
+      <c r="D57" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="E57" s="5" t="s">
+      <c r="E57" s="2" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="58" spans="1:5" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="B58" s="7" t="s">
+    <row r="58" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B58" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="C58" s="5" t="s">
+      <c r="C58" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="D58" s="7" t="s">
+      <c r="D58" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="E58" s="10" t="s">
+      <c r="E58" s="20" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="59" spans="1:5" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="B59" s="7" t="s">
+    <row r="59" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B59" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="C59" s="5" t="s">
+      <c r="C59" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="D59" s="10" t="s">
+      <c r="D59" s="20" t="s">
         <v>157</v>
       </c>
-      <c r="E59" s="5" t="s">
+      <c r="E59" s="2" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="60" spans="1:5" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="B60" s="7" t="s">
+    <row r="60" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B60" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="C60" s="5" t="s">
+      <c r="C60" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="D60" s="7" t="s">
+      <c r="D60" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="E60" s="11" t="s">
+      <c r="E60" s="1" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="61" spans="1:5" s="7" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="B61" s="7" t="s">
+    <row r="61" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="B61" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="C61" s="5" t="s">
+      <c r="C61" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="D61" s="5" t="s">
+      <c r="D61" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="E61" s="18" t="s">
+      <c r="E61" s="21" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="62" spans="1:5" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="B62" s="7" t="s">
+    <row r="62" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B62" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="C62" s="5" t="s">
+      <c r="C62" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="D62" s="7" t="s">
+      <c r="D62" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="E62" s="14" t="s">
+      <c r="E62" s="22" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="63" spans="1:5" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="B63" s="7" t="s">
+    <row r="63" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B63" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="C63" s="5" t="s">
+      <c r="C63" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="D63" s="7" t="s">
+      <c r="D63" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="E63" s="5" t="s">
+      <c r="E63" s="2" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="64" spans="1:5" s="7" customFormat="1" ht="210" x14ac:dyDescent="0.25">
-      <c r="B64" s="7" t="s">
+    <row r="64" spans="1:5" ht="210" x14ac:dyDescent="0.25">
+      <c r="B64" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="C64" s="5" t="s">
+      <c r="C64" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="D64" s="32"/>
+    </row>
+    <row r="65" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="B65" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="D65" s="32"/>
+    </row>
+    <row r="66" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B66" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="D66" s="31" t="s">
+        <v>236</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="C67" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="D67" s="33" t="s">
+        <v>239</v>
+      </c>
+      <c r="E67" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="C68" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="D68" s="19" t="s">
+        <v>241</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="C69" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="D69" s="33" t="s">
+        <v>242</v>
+      </c>
+      <c r="E69" s="2" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="C70" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="D70" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="E70" s="2" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A71" s="23"/>
+      <c r="B71" s="23"/>
+      <c r="C71" s="28" t="s">
+        <v>190</v>
+      </c>
+      <c r="D71" s="29" t="s">
+        <v>191</v>
+      </c>
+      <c r="E71" s="28" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A72" s="23"/>
+      <c r="B72" s="23" t="s">
+        <v>249</v>
+      </c>
+      <c r="C72" s="24" t="s">
+        <v>246</v>
+      </c>
+      <c r="D72" s="19" t="s">
+        <v>247</v>
+      </c>
+      <c r="E72" s="24" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A73" s="23"/>
+      <c r="B73" s="23" t="s">
+        <v>252</v>
+      </c>
+      <c r="C73" s="24" t="s">
+        <v>251</v>
+      </c>
+      <c r="D73" s="25" t="s">
+        <v>193</v>
+      </c>
+      <c r="E73" s="24" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" s="23"/>
+      <c r="B74" s="23" t="s">
+        <v>252</v>
+      </c>
+      <c r="C74" s="24" t="s">
+        <v>194</v>
+      </c>
+      <c r="D74" s="19" t="s">
+        <v>253</v>
+      </c>
+      <c r="E74" s="24" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A75" s="23"/>
+      <c r="B75" s="23" t="s">
+        <v>252</v>
+      </c>
+      <c r="C75" s="24" t="s">
+        <v>195</v>
+      </c>
+      <c r="D75" s="19" t="s">
+        <v>255</v>
+      </c>
+      <c r="E75" s="24" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A76" s="23"/>
+      <c r="B76" s="23" t="s">
+        <v>252</v>
+      </c>
+      <c r="C76" s="24" t="s">
+        <v>259</v>
+      </c>
+      <c r="D76" s="19" t="s">
+        <v>256</v>
+      </c>
+      <c r="E76" s="24" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B77" s="23" t="s">
+        <v>252</v>
+      </c>
+      <c r="C77" s="24" t="s">
+        <v>262</v>
+      </c>
+      <c r="D77" s="19" t="s">
+        <v>257</v>
+      </c>
+      <c r="E77" s="24" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="B78" s="23" t="s">
+        <v>252</v>
+      </c>
+      <c r="C78" s="24" t="s">
+        <v>264</v>
+      </c>
+      <c r="D78" s="19" t="s">
+        <v>265</v>
+      </c>
+      <c r="E78" s="24" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B79" s="25" t="s">
+        <v>196</v>
+      </c>
+      <c r="C79" s="24" t="s">
+        <v>197</v>
+      </c>
+      <c r="D79" s="31" t="s">
+        <v>198</v>
+      </c>
+      <c r="E79" s="24" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="B80" s="25" t="s">
+        <v>196</v>
+      </c>
+      <c r="C80" s="24" t="s">
+        <v>200</v>
+      </c>
+      <c r="D80" s="31" t="s">
+        <v>201</v>
+      </c>
+      <c r="E80" s="24" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="81" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B81" s="25" t="s">
+        <v>196</v>
+      </c>
+      <c r="C81" s="24" t="s">
+        <v>200</v>
+      </c>
+      <c r="D81" s="31" t="s">
+        <v>203</v>
+      </c>
+      <c r="E81" s="26" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="82" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B82" s="25" t="s">
+        <v>196</v>
+      </c>
+      <c r="C82" s="30" t="s">
+        <v>205</v>
+      </c>
+      <c r="D82" s="31" t="s">
+        <v>206</v>
+      </c>
+      <c r="E82" s="23" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="83" spans="2:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="B83" s="25" t="s">
+        <v>196</v>
+      </c>
+      <c r="C83" s="30" t="s">
+        <v>208</v>
+      </c>
+      <c r="D83" s="25" t="s">
+        <v>209</v>
+      </c>
+      <c r="E83" s="24" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="84" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B84" s="25" t="s">
+        <v>196</v>
+      </c>
+      <c r="C84" s="24" t="s">
+        <v>211</v>
+      </c>
+      <c r="D84" s="25" t="s">
+        <v>212</v>
+      </c>
+      <c r="E84" s="24" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="85" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B85" s="25" t="s">
+        <v>196</v>
+      </c>
+      <c r="C85" s="30" t="s">
+        <v>214</v>
+      </c>
+      <c r="D85" s="31" t="s">
+        <v>215</v>
+      </c>
+      <c r="E85" s="27" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="86" spans="2:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="B86" s="25" t="s">
+        <v>217</v>
+      </c>
+      <c r="C86" s="24" t="s">
+        <v>218</v>
+      </c>
+      <c r="D86" s="25" t="s">
+        <v>219</v>
+      </c>
+      <c r="E86" s="24" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="87" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B87" s="25" t="s">
+        <v>221</v>
+      </c>
+      <c r="C87" s="24" t="s">
+        <v>222</v>
+      </c>
+      <c r="D87" s="31" t="s">
+        <v>187</v>
+      </c>
+      <c r="E87" s="24" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="88" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B88" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="C88" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="D88" t="s">
+        <v>228</v>
+      </c>
+      <c r="E88" s="2" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="89" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="C89" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="D89" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="E89" s="2" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="90" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="C90" s="24" t="s">
+        <v>227</v>
+      </c>
+      <c r="D90" s="25" t="s">
+        <v>231</v>
+      </c>
+      <c r="E90" s="2" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="91" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="C91" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="D91" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="E91" s="2" t="s">
         <v>233</v>
-      </c>
-      <c r="E64" s="5"/>
-    </row>
-    <row r="65" spans="1:5" s="7" customFormat="1" ht="90" x14ac:dyDescent="0.25">
-      <c r="B65" s="7" t="s">
-        <v>178</v>
-      </c>
-      <c r="C65" s="5" t="s">
-        <v>179</v>
-      </c>
-      <c r="E65" s="5"/>
-    </row>
-    <row r="66" spans="1:5" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="B66" s="7" t="s">
-        <v>181</v>
-      </c>
-      <c r="C66" s="5" t="s">
-        <v>182</v>
-      </c>
-      <c r="D66" s="10" t="s">
-        <v>234</v>
-      </c>
-      <c r="E66" s="11" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" s="7" customFormat="1" ht="105" x14ac:dyDescent="0.25">
-      <c r="C67" s="5" t="s">
-        <v>236</v>
-      </c>
-      <c r="D67" s="5" t="s">
-        <v>237</v>
-      </c>
-      <c r="E67" s="5" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="C68" s="5" t="s">
-        <v>238</v>
-      </c>
-      <c r="D68" s="7" t="s">
-        <v>239</v>
-      </c>
-      <c r="E68" s="11" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" s="7" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="C69" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="D69" s="5" t="s">
-        <v>240</v>
-      </c>
-      <c r="E69" s="5" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="C70" s="5" t="s">
-        <v>243</v>
-      </c>
-      <c r="D70" s="7" t="s">
-        <v>242</v>
-      </c>
-      <c r="E70" s="5" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A71" s="9"/>
-      <c r="B71" s="9"/>
-      <c r="C71" s="19" t="s">
-        <v>190</v>
-      </c>
-      <c r="D71" s="20" t="s">
-        <v>191</v>
-      </c>
-      <c r="E71" s="19" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" s="7" customFormat="1" ht="90" x14ac:dyDescent="0.25">
-      <c r="A72" s="9"/>
-      <c r="B72" s="26" t="s">
-        <v>245</v>
-      </c>
-      <c r="C72" s="16" t="s">
-        <v>267</v>
-      </c>
-      <c r="D72" s="27" t="s">
-        <v>244</v>
-      </c>
-      <c r="E72" s="16" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A73" s="9"/>
-      <c r="B73" s="26" t="s">
-        <v>246</v>
-      </c>
-      <c r="C73" s="16" t="s">
-        <v>262</v>
-      </c>
-      <c r="D73" s="27" t="s">
-        <v>193</v>
-      </c>
-      <c r="E73" s="16" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A74" s="9"/>
-      <c r="B74" s="26" t="s">
-        <v>246</v>
-      </c>
-      <c r="C74" s="16" t="s">
-        <v>268</v>
-      </c>
-      <c r="D74" s="27" t="s">
-        <v>247</v>
-      </c>
-      <c r="E74" s="16" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A75" s="9"/>
-      <c r="B75" s="26" t="s">
-        <v>246</v>
-      </c>
-      <c r="C75" s="16" t="s">
-        <v>263</v>
-      </c>
-      <c r="D75" s="27" t="s">
-        <v>257</v>
-      </c>
-      <c r="E75" s="16" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A76" s="9"/>
-      <c r="B76" s="26" t="s">
-        <v>246</v>
-      </c>
-      <c r="C76" s="16" t="s">
-        <v>269</v>
-      </c>
-      <c r="D76" s="27" t="s">
-        <v>248</v>
-      </c>
-      <c r="E76" s="16" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="B77" s="26" t="s">
-        <v>246</v>
-      </c>
-      <c r="C77" s="16" t="s">
-        <v>270</v>
-      </c>
-      <c r="D77" s="27" t="s">
-        <v>249</v>
-      </c>
-      <c r="E77" s="16" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="B78" s="26" t="s">
-        <v>246</v>
-      </c>
-      <c r="C78" s="16" t="s">
-        <v>271</v>
-      </c>
-      <c r="D78" s="27" t="s">
-        <v>250</v>
-      </c>
-      <c r="E78" s="16" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="B79" s="7" t="s">
-        <v>194</v>
-      </c>
-      <c r="C79" s="5" t="s">
-        <v>195</v>
-      </c>
-      <c r="D79" s="10" t="s">
-        <v>196</v>
-      </c>
-      <c r="E79" s="5" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" s="7" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="B80" s="7" t="s">
-        <v>194</v>
-      </c>
-      <c r="C80" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="D80" s="10" t="s">
-        <v>199</v>
-      </c>
-      <c r="E80" s="5" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="81" spans="2:5" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="B81" s="7" t="s">
-        <v>194</v>
-      </c>
-      <c r="C81" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="D81" s="10" t="s">
-        <v>201</v>
-      </c>
-      <c r="E81" s="21" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="82" spans="2:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B82" s="7" t="s">
-        <v>194</v>
-      </c>
-      <c r="C82" s="8" t="s">
-        <v>203</v>
-      </c>
-      <c r="D82" s="10" t="s">
-        <v>204</v>
-      </c>
-      <c r="E82" s="9" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="83" spans="2:5" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="B83" s="7" t="s">
-        <v>194</v>
-      </c>
-      <c r="C83" s="8" t="s">
-        <v>206</v>
-      </c>
-      <c r="D83" s="7" t="s">
-        <v>207</v>
-      </c>
-      <c r="E83" s="5" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="84" spans="2:5" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="B84" s="7" t="s">
-        <v>194</v>
-      </c>
-      <c r="C84" s="5" t="s">
-        <v>209</v>
-      </c>
-      <c r="D84" s="7" t="s">
-        <v>210</v>
-      </c>
-      <c r="E84" s="5" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="85" spans="2:5" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="B85" s="7" t="s">
-        <v>194</v>
-      </c>
-      <c r="C85" s="8" t="s">
-        <v>212</v>
-      </c>
-      <c r="D85" s="10" t="s">
-        <v>213</v>
-      </c>
-      <c r="E85" s="22" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="86" spans="2:5" s="7" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="B86" s="7" t="s">
-        <v>215</v>
-      </c>
-      <c r="C86" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="D86" s="7" t="s">
-        <v>217</v>
-      </c>
-      <c r="E86" s="5" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="87" spans="2:5" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="B87" s="7" t="s">
-        <v>219</v>
-      </c>
-      <c r="C87" s="5" t="s">
-        <v>220</v>
-      </c>
-      <c r="D87" s="10" t="s">
-        <v>187</v>
-      </c>
-      <c r="E87" s="5" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="88" spans="2:5" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="B88" s="7" t="s">
-        <v>223</v>
-      </c>
-      <c r="C88" s="5" t="s">
-        <v>224</v>
-      </c>
-      <c r="D88" s="9" t="s">
-        <v>226</v>
-      </c>
-      <c r="E88" s="5" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="89" spans="2:5" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="C89" s="5" t="s">
-        <v>225</v>
-      </c>
-      <c r="D89" s="7" t="s">
-        <v>229</v>
-      </c>
-      <c r="E89" s="5" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="90" spans="2:5" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="C90" s="5" t="s">
-        <v>225</v>
-      </c>
-      <c r="D90" s="7" t="s">
-        <v>229</v>
-      </c>
-      <c r="E90" s="5" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="91" spans="2:5" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="C91" s="5" t="s">
-        <v>232</v>
-      </c>
-      <c r="D91" s="7" t="s">
-        <v>230</v>
-      </c>
-      <c r="E91" s="5" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="92" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C92" s="24" t="s">
-        <v>252</v>
-      </c>
-      <c r="D92" s="23" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="93" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="C93" s="1" t="s">
-        <v>254</v>
-      </c>
-      <c r="D93" s="25" t="s">
-        <v>187</v>
-      </c>
-      <c r="E93" s="1" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="94" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C94" s="1" t="s">
-        <v>255</v>
-      </c>
-      <c r="D94" t="s">
-        <v>188</v>
-      </c>
-      <c r="E94" s="1" t="s">
-        <v>256</v>
       </c>
     </row>
   </sheetData>
@@ -4631,12 +4747,389 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="600" topLeftCell="A10" activePane="bottomLeft"/>
+      <selection sqref="A1:XFD1"/>
+      <selection pane="bottomLeft" activeCell="E28" sqref="E28"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="53.5703125" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" customWidth="1"/>
+    <col min="3" max="3" width="32.85546875" style="36" customWidth="1"/>
+    <col min="4" max="4" width="19.42578125" customWidth="1"/>
+    <col min="5" max="5" width="50.28515625" customWidth="1"/>
+    <col min="6" max="6" width="40.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="37" t="s">
+        <v>266</v>
+      </c>
+      <c r="B1" s="37" t="s">
+        <v>267</v>
+      </c>
+      <c r="C1" s="41" t="s">
+        <v>268</v>
+      </c>
+      <c r="D1" s="37" t="s">
+        <v>269</v>
+      </c>
+      <c r="E1" s="37" t="s">
+        <v>270</v>
+      </c>
+      <c r="F1" s="37" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="35" t="s">
+        <v>279</v>
+      </c>
+      <c r="B2" s="35" t="s">
+        <v>271</v>
+      </c>
+      <c r="C2" s="36" t="s">
+        <v>272</v>
+      </c>
+      <c r="D2" s="35" t="s">
+        <v>273</v>
+      </c>
+      <c r="E2" s="36" t="s">
+        <v>274</v>
+      </c>
+      <c r="F2" s="34" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="36" t="s">
+        <v>297</v>
+      </c>
+      <c r="B3" s="35" t="s">
+        <v>275</v>
+      </c>
+      <c r="C3" s="36" t="s">
+        <v>276</v>
+      </c>
+      <c r="D3" s="36" t="s">
+        <v>277</v>
+      </c>
+      <c r="E3" s="36" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" s="35" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="36" t="s">
+        <v>296</v>
+      </c>
+      <c r="B4" s="35" t="s">
+        <v>275</v>
+      </c>
+      <c r="C4" s="36" t="s">
+        <v>298</v>
+      </c>
+      <c r="D4" s="36" t="s">
+        <v>277</v>
+      </c>
+      <c r="E4" s="36"/>
+    </row>
+    <row r="5" spans="1:6" s="35" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="36" t="s">
+        <v>295</v>
+      </c>
+      <c r="B5" s="35" t="s">
+        <v>275</v>
+      </c>
+      <c r="C5" s="36" t="s">
+        <v>298</v>
+      </c>
+      <c r="D5" s="36" t="s">
+        <v>277</v>
+      </c>
+      <c r="E5" s="36"/>
+    </row>
+    <row r="6" spans="1:6" s="35" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="36" t="s">
+        <v>294</v>
+      </c>
+      <c r="B6" s="35" t="s">
+        <v>275</v>
+      </c>
+      <c r="C6" s="36" t="s">
+        <v>298</v>
+      </c>
+      <c r="D6" s="36" t="s">
+        <v>277</v>
+      </c>
+      <c r="E6" s="36"/>
+    </row>
+    <row r="7" spans="1:6" s="35" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="36" t="s">
+        <v>292</v>
+      </c>
+      <c r="B7" s="35" t="s">
+        <v>275</v>
+      </c>
+      <c r="C7" s="36" t="s">
+        <v>298</v>
+      </c>
+      <c r="D7" s="36" t="s">
+        <v>277</v>
+      </c>
+      <c r="E7" s="36"/>
+    </row>
+    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>293</v>
+      </c>
+      <c r="B8" s="35" t="s">
+        <v>275</v>
+      </c>
+      <c r="C8" s="36" t="s">
+        <v>298</v>
+      </c>
+      <c r="D8" s="36" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" s="35" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="36" t="s">
+        <v>291</v>
+      </c>
+      <c r="B9" s="35" t="s">
+        <v>275</v>
+      </c>
+      <c r="C9" s="36" t="s">
+        <v>298</v>
+      </c>
+      <c r="D9" s="36" t="s">
+        <v>277</v>
+      </c>
+      <c r="E9" s="36"/>
+    </row>
+    <row r="10" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>284</v>
+      </c>
+      <c r="B10" s="40" t="s">
+        <v>286</v>
+      </c>
+      <c r="C10" s="36" t="s">
+        <v>287</v>
+      </c>
+      <c r="D10" s="38"/>
+      <c r="E10" s="39" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>281</v>
+      </c>
+      <c r="B11" s="35" t="s">
+        <v>271</v>
+      </c>
+      <c r="C11" s="36" t="s">
+        <v>282</v>
+      </c>
+      <c r="D11" s="38"/>
+      <c r="E11" s="36" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>288</v>
+      </c>
+      <c r="B12" s="40" t="s">
+        <v>289</v>
+      </c>
+      <c r="C12" s="36" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>299</v>
+      </c>
+      <c r="B13" s="40" t="s">
+        <v>289</v>
+      </c>
+      <c r="C13" s="36" t="s">
+        <v>290</v>
+      </c>
+      <c r="E13" s="39"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>300</v>
+      </c>
+      <c r="B14" s="40" t="s">
+        <v>289</v>
+      </c>
+      <c r="C14" s="36" t="s">
+        <v>290</v>
+      </c>
+      <c r="E14" s="39"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>301</v>
+      </c>
+      <c r="B15" s="40" t="s">
+        <v>289</v>
+      </c>
+      <c r="C15" s="36" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>302</v>
+      </c>
+      <c r="B16" s="40" t="s">
+        <v>289</v>
+      </c>
+      <c r="C16" s="36" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>303</v>
+      </c>
+      <c r="B17" s="40" t="s">
+        <v>289</v>
+      </c>
+      <c r="C17" s="36" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>304</v>
+      </c>
+      <c r="B18" s="40" t="s">
+        <v>271</v>
+      </c>
+      <c r="C18" s="36" t="s">
+        <v>312</v>
+      </c>
+      <c r="D18" s="42" t="s">
+        <v>313</v>
+      </c>
+      <c r="F18" s="26" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>309</v>
+      </c>
+      <c r="B19" s="40" t="s">
+        <v>271</v>
+      </c>
+      <c r="C19" s="36" t="s">
+        <v>312</v>
+      </c>
+      <c r="D19" s="42" t="s">
+        <v>313</v>
+      </c>
+      <c r="F19" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>308</v>
+      </c>
+      <c r="B20" s="40" t="s">
+        <v>271</v>
+      </c>
+      <c r="C20" s="36" t="s">
+        <v>312</v>
+      </c>
+      <c r="D20" s="42" t="s">
+        <v>313</v>
+      </c>
+      <c r="F20" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>311</v>
+      </c>
+      <c r="B21" s="40" t="s">
+        <v>271</v>
+      </c>
+      <c r="C21" s="36" t="s">
+        <v>312</v>
+      </c>
+      <c r="D21" s="35" t="s">
+        <v>313</v>
+      </c>
+      <c r="F21" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>314</v>
+      </c>
+      <c r="B22" s="40" t="s">
+        <v>289</v>
+      </c>
+      <c r="C22" s="36" t="s">
+        <v>315</v>
+      </c>
+      <c r="F22" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>317</v>
+      </c>
+      <c r="B23" s="40" t="s">
+        <v>319</v>
+      </c>
+      <c r="C23" s="36" t="s">
+        <v>320</v>
+      </c>
+      <c r="D23" s="36" t="s">
+        <v>321</v>
+      </c>
+      <c r="E23" s="36" t="s">
+        <v>322</v>
+      </c>
+      <c r="F23" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A24" s="43" t="s">
+        <v>324</v>
+      </c>
+      <c r="B24" s="44" t="s">
+        <v>323</v>
+      </c>
+      <c r="C24" s="36" t="s">
+        <v>325</v>
+      </c>
+      <c r="D24" s="36" t="s">
+        <v>327</v>
+      </c>
+      <c r="E24" s="36" t="s">
+        <v>326</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>